<commit_message>
Settings functionality implemented where required, unused settings removed. Dutch localization added.
</commit_message>
<xml_diff>
--- a/Unity/Assets/Resources/Localization/IT Alert UI Translation.xlsx
+++ b/Unity/Assets/Resources/Localization/IT Alert UI Translation.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="207">
   <si>
     <t>Key</t>
   </si>
@@ -28,421 +28,610 @@
     <t>Quick Game</t>
   </si>
   <si>
+    <t>Snel Spel</t>
+  </si>
+  <si>
+    <t>MENU_BUTTON_JOIN_GAME</t>
+  </si>
+  <si>
+    <t>Join Game</t>
+  </si>
+  <si>
+    <t>Meedoen met Spel</t>
+  </si>
+  <si>
+    <t>MENU_BUTTON_CREATE_GAME</t>
+  </si>
+  <si>
+    <t>Create Game</t>
+  </si>
+  <si>
+    <t>Spel Maken</t>
+  </si>
+  <si>
+    <t>MENU_BUTTON_SETTINGS</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Instellingen</t>
+  </si>
+  <si>
+    <t>MENU_BUTTON_QUIT</t>
+  </si>
+  <si>
+    <t>Quit</t>
+  </si>
+  <si>
+    <t>Stoppen</t>
+  </si>
+  <si>
+    <t>JOIN_TITLE</t>
+  </si>
+  <si>
+    <t>JOIN_LABEL_GAME_NAME</t>
+  </si>
+  <si>
+    <t>Game Name</t>
+  </si>
+  <si>
+    <t>Spel Naam</t>
+  </si>
+  <si>
+    <t>JOIN_LABEL_SCENARIO</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>JOIN_LABEL_PLAYERS</t>
+  </si>
+  <si>
+    <t>Players</t>
+  </si>
+  <si>
+    <t>Spelers</t>
+  </si>
+  <si>
+    <t>JOIN_BUTTON_JOIN</t>
+  </si>
+  <si>
+    <t>Join</t>
+  </si>
+  <si>
+    <t>Meedoen</t>
+  </si>
+  <si>
+    <t>JOIN_BUTTON_BACK</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Terug</t>
+  </si>
+  <si>
+    <t>JOIN_BUTTON_REFRESH</t>
+  </si>
+  <si>
+    <t>Refresh</t>
+  </si>
+  <si>
+    <t>Verversen</t>
+  </si>
+  <si>
+    <t>CREATE_LABEL_TITLE</t>
+  </si>
+  <si>
+    <t>CREATE_LABEL_GAME_NAME</t>
+  </si>
+  <si>
+    <t>CREATE_LABEL_NUM_PLAYERS</t>
+  </si>
+  <si>
+    <t>Max Players</t>
+  </si>
+  <si>
+    <t>Max Spelers</t>
+  </si>
+  <si>
+    <t>CREATE_BUTTON_BACK</t>
+  </si>
+  <si>
+    <t>CREATE_BUTTON_CREATE</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Maken</t>
+  </si>
+  <si>
+    <t>SCENARIO_LABEL_TITLE</t>
+  </si>
+  <si>
+    <t>Scenarios</t>
+  </si>
+  <si>
+    <t>Scenario's</t>
+  </si>
+  <si>
+    <t>SCENARIO_LABEL_SCENARIO_NAME</t>
+  </si>
+  <si>
+    <t>Scenario Name</t>
+  </si>
+  <si>
+    <t>Scenario Naam</t>
+  </si>
+  <si>
+    <t>SCENARIO_LABEL_REQUIRED_PLAYERS</t>
+  </si>
+  <si>
+    <t>Players Required</t>
+  </si>
+  <si>
+    <t>Spelers Benodigd</t>
+  </si>
+  <si>
+    <t>SCENARIO_LABEL_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Scenario Description</t>
+  </si>
+  <si>
+    <t>Scenario Beschrijving</t>
+  </si>
+  <si>
+    <t>SCENARIO_BUTTON_SELECT</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>Selecteer</t>
+  </si>
+  <si>
+    <t>SCENARIO_BUTTON_BACK</t>
+  </si>
+  <si>
+    <t>SETTINGS_LABEL_TITLE</t>
+  </si>
+  <si>
+    <t>PAUSE_BUTTON_CONTINUE</t>
+  </si>
+  <si>
+    <t>Continue</t>
+  </si>
+  <si>
+    <t>Doorgaan</t>
+  </si>
+  <si>
+    <t>PAUSE_BUTTON_SETTINGS</t>
+  </si>
+  <si>
+    <t>PAUSE_BUTTON_MENU</t>
+  </si>
+  <si>
+    <t>Main Menu</t>
+  </si>
+  <si>
+    <t>Hoofdmenu</t>
+  </si>
+  <si>
+    <t>VOICE_PUSH_TO_TALK</t>
+  </si>
+  <si>
+    <t>Push {0} to talk</t>
+  </si>
+  <si>
+    <t>Druk {0} om te praten</t>
+  </si>
+  <si>
+    <t>ERROR_LABEL_TITLE</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Fout</t>
+  </si>
+  <si>
+    <t>CONNECTION_LABEL</t>
+  </si>
+  <si>
+    <t>Game Server:</t>
+  </si>
+  <si>
+    <t>Spel Server:</t>
+  </si>
+  <si>
+    <t>CONNECTION_LABEL_CONNECTED</t>
+  </si>
+  <si>
+    <t>Connected</t>
+  </si>
+  <si>
+    <t>Verbonden</t>
+  </si>
+  <si>
+    <t>CONNECTION_LABEL_NOT_CONNECTED</t>
+  </si>
+  <si>
+    <t>Not Connected</t>
+  </si>
+  <si>
+    <t>Niet Verbonden</t>
+  </si>
+  <si>
+    <t>LOBBY_LABEL_TITLE</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>LOBBY_BUTTON_BACK</t>
+  </si>
+  <si>
+    <t>Go Back</t>
+  </si>
+  <si>
+    <t>Ga Terug</t>
+  </si>
+  <si>
+    <t>LOBBY_BUTTON_COLOUR</t>
+  </si>
+  <si>
+    <t>Change Colour</t>
+  </si>
+  <si>
+    <t>Verander Kleur</t>
+  </si>
+  <si>
+    <t>LOBBY_BUTTON_READY</t>
+  </si>
+  <si>
+    <t>Ready</t>
+  </si>
+  <si>
+    <t>Klaar</t>
+  </si>
+  <si>
+    <t>LOBBY_LABEL_WAITING</t>
+  </si>
+  <si>
+    <t>Waiting</t>
+  </si>
+  <si>
+    <t>Wachten</t>
+  </si>
+  <si>
+    <t>FEEDBACK_LABEL_TITLE</t>
+  </si>
+  <si>
+    <t>Team Feedback</t>
+  </si>
+  <si>
+    <t>FEEDBACK_LABEL_INSTRUCTION</t>
+  </si>
+  <si>
+    <t>Rank your teammates in each category</t>
+  </si>
+  <si>
+    <t>Plaats je team spelers in elke categorie</t>
+  </si>
+  <si>
+    <t>FEEDBACK_LABEL_ERROR</t>
+  </si>
+  <si>
+    <t>Not all players have been ranked in category {0}</t>
+  </si>
+  <si>
+    <t>Niet alle spelers zijn geplaatst in categorie {0}</t>
+  </si>
+  <si>
+    <t>FEEDBACK_LABEL_CATEGORY_1</t>
+  </si>
+  <si>
+    <t>Leadership</t>
+  </si>
+  <si>
+    <t>Leiderschap</t>
+  </si>
+  <si>
+    <t>FEEDBACK_LABEL_CATEGORY_2</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Communicatie</t>
+  </si>
+  <si>
+    <t>FEEDBACK_LABEL_CATEGORY_3</t>
+  </si>
+  <si>
+    <t>Cooperation</t>
+  </si>
+  <si>
+    <t>Samenwerking</t>
+  </si>
+  <si>
+    <t>FEEBACK_BUTTON_CONTINUE</t>
+  </si>
+  <si>
+    <t>GAME_COMPLETION_SUCCESS</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Succes</t>
+  </si>
+  <si>
+    <t>GAME_COMPLETION_FAILURE</t>
+  </si>
+  <si>
+    <t>Failure</t>
+  </si>
+  <si>
+    <t>Gefaald</t>
+  </si>
+  <si>
+    <t>SUGAR_LABEL_NOT_SIGNED_IN</t>
+  </si>
+  <si>
+    <t>Not Signed In</t>
+  </si>
+  <si>
+    <t>Niet ingelogd</t>
+  </si>
+  <si>
+    <t>ERROR_BUTTON_CLOSE</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>COLOUR_PICKER_LABEL_TITLE</t>
+  </si>
+  <si>
+    <t>Change Player Colour</t>
+  </si>
+  <si>
+    <t>Verander Kleur Speler</t>
+  </si>
+  <si>
+    <t>COLOUR_PICKER_BUTTON_CANCEL</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>Annuleer</t>
+  </si>
+  <si>
+    <t>COLOUR_PICKER_BUTTON_SELECT</t>
+  </si>
+  <si>
+    <t>Set Colour</t>
+  </si>
+  <si>
+    <t>Zet Kleur</t>
+  </si>
+  <si>
+    <t>SETTINGS_LABEL_RESOLUTION</t>
+  </si>
+  <si>
+    <t>Screen Resolution</t>
+  </si>
+  <si>
+    <t>Scherm Resolutie</t>
+  </si>
+  <si>
+    <t>SETTINGS_LABEL_QUALITY</t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>Kwaliteit</t>
+  </si>
+  <si>
+    <t>SETTINGS_LABEL_LANGUAGE</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Taal</t>
+  </si>
+  <si>
+    <t>SETTINGS_LABEL_FULLSCREEN</t>
+  </si>
+  <si>
+    <t>Full Screen</t>
+  </si>
+  <si>
+    <t>Volledig Scherm</t>
+  </si>
+  <si>
+    <t>SETTINGS_QUALITY_FASTEST</t>
+  </si>
+  <si>
+    <t>Fastest</t>
+  </si>
+  <si>
+    <t>Snelst</t>
+  </si>
+  <si>
+    <t>SETTINGS_QUALITY_FAST</t>
+  </si>
+  <si>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>Snel</t>
+  </si>
+  <si>
+    <t>SETTINGS_QUALITY_SIMPLE</t>
+  </si>
+  <si>
+    <t>Simple</t>
+  </si>
+  <si>
+    <t>Eenvoudig</t>
+  </si>
+  <si>
+    <t>SETTINGS_QUALITY_GOOD</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Goed</t>
+  </si>
+  <si>
+    <t>SETTINGS_QUALITY_BEAUTIFUL</t>
+  </si>
+  <si>
+    <t>Beautiful</t>
+  </si>
+  <si>
+    <t>Mooi</t>
+  </si>
+  <si>
+    <t>SETTINGS_QUALITY_FANTASTIC</t>
+  </si>
+  <si>
+    <t>Fantastic</t>
+  </si>
+  <si>
+    <t>Fantastisch</t>
+  </si>
+  <si>
+    <t>SETTINGS_LABEL_VOLUME</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>SETTINGS_BUTTON_APPLY</t>
+  </si>
+  <si>
+    <t>Apply</t>
+  </si>
+  <si>
+    <t>Toepassen</t>
+  </si>
+  <si>
+    <t>SETTINGS_BUTTON_CANCEL</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Sluiten</t>
+  </si>
+  <si>
+    <t>SETTINGS_BUTTON_SAVE</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Bewaren</t>
+  </si>
+  <si>
+    <t>SETTINGS_LABEL_DISPLAY</t>
+  </si>
+  <si>
+    <t>DIsplay</t>
+  </si>
+  <si>
+    <t>Scherm</t>
+  </si>
+  <si>
+    <t>SETTINGS_LABEL_VOICE</t>
+  </si>
+  <si>
+    <t>Voice</t>
+  </si>
+  <si>
+    <t>Spraak</t>
+  </si>
+  <si>
+    <t>SETTINGS_LABEL_VOICE_ENABLED</t>
+  </si>
+  <si>
+    <t>Voice Enabled</t>
+  </si>
+  <si>
+    <t>Geluid Ingeschakeld</t>
+  </si>
+  <si>
+    <t>SETTINGS_LABEL_MICROPHONE_VOLUME</t>
+  </si>
+  <si>
+    <t>Microphone Volume</t>
+  </si>
+  <si>
+    <t>Volume Microfoon</t>
+  </si>
+  <si>
+    <t>SETTINGS_LABEL_RECEIVE_VOLUME</t>
+  </si>
+  <si>
+    <t>Receive Volume</t>
+  </si>
+  <si>
+    <t>Volume Ontvanger</t>
+  </si>
+  <si>
+    <t>SETTINGS_BUTTON_TEST_MICROPHONE</t>
+  </si>
+  <si>
+    <t>Test Microphone</t>
+  </si>
+  <si>
+    <t>Test Microfoon</t>
+  </si>
+  <si>
+    <t>SETTINGS_LABEL_SOUND</t>
+  </si>
+  <si>
+    <t>Sound</t>
+  </si>
+  <si>
+    <t>Geluid</t>
+  </si>
+  <si>
+    <t>SETTINGS_LABEL_MUSIC_VOLUME</t>
+  </si>
+  <si>
+    <t>Music Volume</t>
+  </si>
+  <si>
+    <t>Volume Muziek</t>
+  </si>
+  <si>
+    <t>SETTINGS_LABEL_SFX_VOLUME</t>
+  </si>
+  <si>
+    <t>SFX Volume</t>
+  </si>
+  <si>
+    <t>Volume Effecten</t>
+  </si>
+  <si>
+    <t>SETTINGS_LABEL_MICROPHONE_DEVICE</t>
+  </si>
+  <si>
+    <t>Microphone Device</t>
+  </si>
+  <si>
     <t>XXXX</t>
-  </si>
-  <si>
-    <t>MENU_BUTTON_JOIN_GAME</t>
-  </si>
-  <si>
-    <t>Join Game</t>
-  </si>
-  <si>
-    <t>MENU_BUTTON_CREATE_GAME</t>
-  </si>
-  <si>
-    <t>Create Game</t>
-  </si>
-  <si>
-    <t>MENU_BUTTON_SETTINGS</t>
-  </si>
-  <si>
-    <t>Settings</t>
-  </si>
-  <si>
-    <t>MENU_BUTTON_QUIT</t>
-  </si>
-  <si>
-    <t>Quit</t>
-  </si>
-  <si>
-    <t>JOIN_TITLE</t>
-  </si>
-  <si>
-    <t>JOIN_LABEL_GAME_NAME</t>
-  </si>
-  <si>
-    <t>Game Name</t>
-  </si>
-  <si>
-    <t>JOIN_LABEL_SCENARIO</t>
-  </si>
-  <si>
-    <t>Scenario</t>
-  </si>
-  <si>
-    <t>JOIN_LABEL_PLAYERS</t>
-  </si>
-  <si>
-    <t>Players</t>
-  </si>
-  <si>
-    <t>JOIN_BUTTON_JOIN</t>
-  </si>
-  <si>
-    <t>Join</t>
-  </si>
-  <si>
-    <t>JOIN_BUTTON_BACK</t>
-  </si>
-  <si>
-    <t>Back</t>
-  </si>
-  <si>
-    <t>JOIN_BUTTON_REFRESH</t>
-  </si>
-  <si>
-    <t>Refresh</t>
-  </si>
-  <si>
-    <t>CREATE_LABEL_TITLE</t>
-  </si>
-  <si>
-    <t>CREATE_LABEL_GAME_NAME</t>
-  </si>
-  <si>
-    <t>CREATE_LABEL_NUM_PLAYERS</t>
-  </si>
-  <si>
-    <t>Max Players</t>
-  </si>
-  <si>
-    <t>CREATE_BUTTON_BACK</t>
-  </si>
-  <si>
-    <t>CREATE_BUTTON_CREATE</t>
-  </si>
-  <si>
-    <t>Create</t>
-  </si>
-  <si>
-    <t>SCENARIO_LABEL_TITLE</t>
-  </si>
-  <si>
-    <t>Scenarios</t>
-  </si>
-  <si>
-    <t>SCENARIO_LABEL_SCENARIO_NAME</t>
-  </si>
-  <si>
-    <t>Scenario Name</t>
-  </si>
-  <si>
-    <t>SCENARIO_LABEL_REQUIRED_PLAYERS</t>
-  </si>
-  <si>
-    <t>Players Required</t>
-  </si>
-  <si>
-    <t>SCENARIO_LABEL_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>Scenario Description</t>
-  </si>
-  <si>
-    <t>SCENARIO_BUTTON_SELECT</t>
-  </si>
-  <si>
-    <t>Select</t>
-  </si>
-  <si>
-    <t>SCENARIO_BUTTON_BACK</t>
-  </si>
-  <si>
-    <t>SETTINGS_LABEL_TITLE</t>
-  </si>
-  <si>
-    <t>PAUSE_BUTTON_CONTINUE</t>
-  </si>
-  <si>
-    <t>Continue</t>
-  </si>
-  <si>
-    <t>PAUSE_BUTTON_SETTINGS</t>
-  </si>
-  <si>
-    <t>PAUSE_BUTTON_MENU</t>
-  </si>
-  <si>
-    <t>Main Menu</t>
-  </si>
-  <si>
-    <t>VOICE_PUSH_TO_TALK</t>
-  </si>
-  <si>
-    <t>Push {0} to talk</t>
-  </si>
-  <si>
-    <t>ERROR_LABEL_TITLE</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>CONNECTION_LABEL</t>
-  </si>
-  <si>
-    <t>Game Server:</t>
-  </si>
-  <si>
-    <t>CONNECTION_LABEL_CONNECTED</t>
-  </si>
-  <si>
-    <t>Connected</t>
-  </si>
-  <si>
-    <t>CONNECTION_LABEL_NOT_CONNECTED</t>
-  </si>
-  <si>
-    <t>Not Connected</t>
-  </si>
-  <si>
-    <t>LOBBY_LABEL_TITLE</t>
-  </si>
-  <si>
-    <t>Team</t>
-  </si>
-  <si>
-    <t>LOBBY_BUTTON_BACK</t>
-  </si>
-  <si>
-    <t>Go Back</t>
-  </si>
-  <si>
-    <t>LOBBY_BUTTON_COLOUR</t>
-  </si>
-  <si>
-    <t>Change Colour</t>
-  </si>
-  <si>
-    <t>LOBBY_BUTTON_READY</t>
-  </si>
-  <si>
-    <t>Ready</t>
-  </si>
-  <si>
-    <t>LOBBY_LABEL_WAITING</t>
-  </si>
-  <si>
-    <t>Waiting</t>
-  </si>
-  <si>
-    <t>FEEDBACK_LABEL_TITLE</t>
-  </si>
-  <si>
-    <t>Team Feedback</t>
-  </si>
-  <si>
-    <t>FEEDBACK_LABEL_INSTRUCTION</t>
-  </si>
-  <si>
-    <t>Rank your teammates in each category</t>
-  </si>
-  <si>
-    <t>FEEDBACK_LABEL_ERROR</t>
-  </si>
-  <si>
-    <t>Not all players have been ranked in category {0}</t>
-  </si>
-  <si>
-    <t>FEEDBACK_LABEL_CATEGORY_1</t>
-  </si>
-  <si>
-    <t>Leadership</t>
-  </si>
-  <si>
-    <t>FEEDBACK_LABEL_CATEGORY_2</t>
-  </si>
-  <si>
-    <t>Communication</t>
-  </si>
-  <si>
-    <t>FEEDBACK_LABEL_CATEGORY_3</t>
-  </si>
-  <si>
-    <t>Cooperation</t>
-  </si>
-  <si>
-    <t>FEEBACK_BUTTON_CONTINUE</t>
-  </si>
-  <si>
-    <t>GAME_COMPLETION_SUCCESS</t>
-  </si>
-  <si>
-    <t>Success</t>
-  </si>
-  <si>
-    <t>GAME_COMPLETION_FAILURE</t>
-  </si>
-  <si>
-    <t>Failure</t>
-  </si>
-  <si>
-    <t>SUGAR_LABEL_NOT_SIGNED_IN</t>
-  </si>
-  <si>
-    <t>Not Signed In</t>
-  </si>
-  <si>
-    <t>ERROR_BUTTON_CLOSE</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>COLOUR_PICKER_LABEL_TITLE</t>
-  </si>
-  <si>
-    <t>Change Player Colour</t>
-  </si>
-  <si>
-    <t>COLOUR_PICKER_BUTTON_CANCEL</t>
-  </si>
-  <si>
-    <t>Cancel</t>
-  </si>
-  <si>
-    <t>COLOUR_PICKER_BUTTON_SELECT</t>
-  </si>
-  <si>
-    <t>Set Colour</t>
-  </si>
-  <si>
-    <t>SETTINGS_LABEL_RESOLUTION</t>
-  </si>
-  <si>
-    <t>Resolution</t>
-  </si>
-  <si>
-    <t>SETTINGS_LABEL_QUALITY</t>
-  </si>
-  <si>
-    <t>Quality</t>
-  </si>
-  <si>
-    <t>SETTINGS_LABEL_LANGUAGE</t>
-  </si>
-  <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>SETTINGS_LABEL_FULLSCREEN</t>
-  </si>
-  <si>
-    <t>Full Screen</t>
-  </si>
-  <si>
-    <t>SETTINGS_QUALITY_FASTEST</t>
-  </si>
-  <si>
-    <t>Fastest</t>
-  </si>
-  <si>
-    <t>SETTINGS_QUALITY_FAST</t>
-  </si>
-  <si>
-    <t>Fast</t>
-  </si>
-  <si>
-    <t>SETTINGS_QUALITY_SIMPLE</t>
-  </si>
-  <si>
-    <t>Simple</t>
-  </si>
-  <si>
-    <t>SETTINGS_QUALITY_GOOD</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
-    <t>SETTINGS_QUALITY_BEAUTIFUL</t>
-  </si>
-  <si>
-    <t>Beautiful</t>
-  </si>
-  <si>
-    <t>SETTINGS_QUALITY_FANTASTIC</t>
-  </si>
-  <si>
-    <t>Fantastic</t>
-  </si>
-  <si>
-    <t>SETTINGS_LABEL_VOLUME</t>
-  </si>
-  <si>
-    <t>Volume</t>
-  </si>
-  <si>
-    <t>SETTINGS_BUTTON_APPLY</t>
-  </si>
-  <si>
-    <t>Apply</t>
-  </si>
-  <si>
-    <t>SETTINGS_BUTTON_CANCEL</t>
-  </si>
-  <si>
-    <t>Close</t>
-  </si>
-  <si>
-    <t>SETTINGS_BUTTON_SAVE</t>
-  </si>
-  <si>
-    <t>Save</t>
-  </si>
-  <si>
-    <t>SETTINGS_LABEL_DISPLAY</t>
-  </si>
-  <si>
-    <t>DIsplay</t>
-  </si>
-  <si>
-    <t>SETTINGS_LABEL_VOICE</t>
-  </si>
-  <si>
-    <t>Voice</t>
-  </si>
-  <si>
-    <t>SETTINGS_LABEL_VOICE_ENABLED</t>
-  </si>
-  <si>
-    <t>Voice Enabled</t>
-  </si>
-  <si>
-    <t>SETTINGS_LABEL_MICROPHONE_VOLUME</t>
-  </si>
-  <si>
-    <t>Microphone Volume</t>
-  </si>
-  <si>
-    <t>SETTINGS_LABEL_RECEIVE_VOLUME</t>
-  </si>
-  <si>
-    <t>Receive Volume</t>
-  </si>
-  <si>
-    <t>SETTINGS_BUTTON_TEST_MICROPHONE</t>
-  </si>
-  <si>
-    <t>Test Microphone</t>
-  </si>
-  <si>
-    <t>SETTINGS_LABEL_SOUND</t>
-  </si>
-  <si>
-    <t>Sound</t>
-  </si>
-  <si>
-    <t>SETTINGS_LABEL_MUSIC_VOLUME</t>
-  </si>
-  <si>
-    <t>Music Volume</t>
-  </si>
-  <si>
-    <t>SETTINGS_LABEL_SFX_VOLUME</t>
-  </si>
-  <si>
-    <t>SFX Volume</t>
   </si>
 </sst>
 </file>
@@ -566,6 +755,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="48.14"/>
     <col customWidth="1" min="2" max="2" width="51.86"/>
+    <col customWidth="1" min="3" max="3" width="38.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -619,7 +809,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -627,13 +817,13 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -641,13 +831,13 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -655,13 +845,13 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -669,13 +859,13 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -683,13 +873,13 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -697,13 +887,13 @@
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -711,13 +901,13 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -725,13 +915,13 @@
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -739,13 +929,13 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -753,13 +943,13 @@
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -767,13 +957,13 @@
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -781,13 +971,13 @@
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -795,13 +985,13 @@
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -809,13 +999,13 @@
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -823,13 +1013,13 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -837,13 +1027,13 @@
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -851,13 +1041,13 @@
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -865,13 +1055,13 @@
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -879,13 +1069,13 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -893,13 +1083,13 @@
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -907,13 +1097,13 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -921,13 +1111,13 @@
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -935,13 +1125,13 @@
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -949,13 +1139,13 @@
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -963,13 +1153,13 @@
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -977,13 +1167,13 @@
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -991,13 +1181,13 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -1005,13 +1195,13 @@
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
@@ -1019,13 +1209,13 @@
     </row>
     <row r="32">
       <c r="A32" s="7" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -1033,13 +1223,13 @@
     </row>
     <row r="33">
       <c r="A33" s="7" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -1047,13 +1237,13 @@
     </row>
     <row r="34">
       <c r="A34" s="4" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -1061,13 +1251,13 @@
     </row>
     <row r="35">
       <c r="A35" s="4" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -1075,13 +1265,13 @@
     </row>
     <row r="36">
       <c r="A36" s="4" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
@@ -1089,13 +1279,13 @@
     </row>
     <row r="37">
       <c r="A37" s="4" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>5</v>
+        <v>94</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -1103,13 +1293,13 @@
     </row>
     <row r="38">
       <c r="A38" s="4" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>5</v>
+        <v>97</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
@@ -1117,13 +1307,13 @@
     </row>
     <row r="39">
       <c r="A39" s="4" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -1131,13 +1321,13 @@
     </row>
     <row r="40">
       <c r="A40" s="4" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -1145,13 +1335,13 @@
     </row>
     <row r="41">
       <c r="A41" s="4" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
@@ -1159,13 +1349,13 @@
     </row>
     <row r="42">
       <c r="A42" s="4" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>5</v>
+        <v>108</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -1173,13 +1363,13 @@
     </row>
     <row r="43">
       <c r="A43" s="4" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>5</v>
+        <v>111</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
@@ -1187,358 +1377,366 @@
     </row>
     <row r="44">
       <c r="A44" s="4" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>5</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="9" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="9" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>5</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="9" t="s">
-        <v>86</v>
+        <v>119</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>5</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="9" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>5</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="9" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>5</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="9" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>93</v>
+        <v>128</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>5</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="9" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>5</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="9" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>97</v>
+        <v>134</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>5</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="9" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>5</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="9" t="s">
-        <v>100</v>
+        <v>139</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>101</v>
+        <v>140</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>5</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="9" t="s">
-        <v>102</v>
+        <v>142</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>5</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="9" t="s">
-        <v>104</v>
+        <v>145</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>105</v>
+        <v>146</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>5</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="9" t="s">
-        <v>106</v>
+        <v>148</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>107</v>
+        <v>149</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>5</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="9" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>109</v>
+        <v>152</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>5</v>
+        <v>153</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="9" t="s">
-        <v>110</v>
+        <v>154</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>111</v>
+        <v>155</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="9" t="s">
-        <v>112</v>
+        <v>157</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>113</v>
+        <v>158</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>5</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="9" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>115</v>
+        <v>161</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>5</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="9" t="s">
-        <v>116</v>
+        <v>163</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>117</v>
+        <v>164</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>5</v>
+        <v>165</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="9" t="s">
-        <v>118</v>
+        <v>166</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>5</v>
+        <v>167</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="9" t="s">
-        <v>120</v>
+        <v>168</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>121</v>
+        <v>169</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>5</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="9" t="s">
-        <v>122</v>
+        <v>171</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>123</v>
+        <v>172</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>5</v>
+        <v>173</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="9" t="s">
-        <v>124</v>
+        <v>174</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>125</v>
+        <v>175</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>5</v>
+        <v>176</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="9" t="s">
-        <v>126</v>
+        <v>177</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>127</v>
+        <v>178</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>5</v>
+        <v>179</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="9" t="s">
-        <v>128</v>
+        <v>180</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>5</v>
+        <v>182</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="9" t="s">
-        <v>130</v>
+        <v>183</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>131</v>
+        <v>184</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>5</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="9" t="s">
-        <v>132</v>
+        <v>186</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>133</v>
+        <v>187</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>5</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="9" t="s">
-        <v>134</v>
+        <v>189</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>135</v>
+        <v>190</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>5</v>
+        <v>191</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="9" t="s">
-        <v>136</v>
+        <v>192</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>137</v>
+        <v>193</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>5</v>
+        <v>194</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="9" t="s">
-        <v>138</v>
+        <v>195</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>139</v>
+        <v>196</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>5</v>
+        <v>197</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="9" t="s">
-        <v>140</v>
+        <v>198</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>141</v>
+        <v>199</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>5</v>
+        <v>200</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="9" t="s">
-        <v>142</v>
+        <v>201</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>143</v>
+        <v>202</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>5</v>
+        <v>203</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="10"/>
+      <c r="A76" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="10"/>

</xml_diff>

<commit_message>
Panel headers moved up. Fix for missing translation and settings dropdown animation.
</commit_message>
<xml_diff>
--- a/Unity/Assets/Resources/Localization/IT Alert UI Translation.xlsx
+++ b/Unity/Assets/Resources/Localization/IT Alert UI Translation.xlsx
@@ -151,10 +151,10 @@
     <t>SCENARIO_LABEL_TITLE</t>
   </si>
   <si>
-    <t>Scenarios</t>
-  </si>
-  <si>
-    <t>Scenario's</t>
+    <t>Select Scenario</t>
+  </si>
+  <si>
+    <t>Selecteer Scenario</t>
   </si>
   <si>
     <t>SCENARIO_LABEL_SCENARIO_NAME</t>
@@ -704,7 +704,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -724,7 +724,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1032,7 +1035,7 @@
       <c r="B19" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="7" t="s">
         <v>47</v>
       </c>
       <c r="D19" s="6"/>
@@ -1152,7 +1155,7 @@
       <c r="F27" s="6"/>
     </row>
     <row r="28">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="8" t="s">
         <v>66</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -1208,7 +1211,7 @@
       <c r="F31" s="6"/>
     </row>
     <row r="32">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="8" t="s">
         <v>78</v>
       </c>
       <c r="B32" s="5" t="s">
@@ -1222,7 +1225,7 @@
       <c r="F32" s="6"/>
     </row>
     <row r="33">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="8" t="s">
         <v>81</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -1379,7 +1382,7 @@
       <c r="A44" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="9" t="s">
         <v>113</v>
       </c>
       <c r="C44" s="5" t="s">
@@ -1387,10 +1390,10 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="9" t="s">
         <v>63</v>
       </c>
       <c r="C45" s="5" t="s">
@@ -1398,3123 +1401,3123 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="9" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="9" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="9" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="9" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="9" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="9" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="9" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="9" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="9" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="9" t="s">
+      <c r="A55" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="9" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="9" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="9" t="s">
+      <c r="A57" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="9" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="C58" s="9" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C59" s="9" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="9" t="s">
+      <c r="A60" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B60" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C60" s="9" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="9" t="s">
+      <c r="A61" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C61" s="9" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="9" t="s">
+      <c r="A62" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="B62" s="8" t="s">
+      <c r="B62" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="C62" s="8" t="s">
+      <c r="C62" s="9" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="9" t="s">
+      <c r="A63" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="B63" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C63" s="8" t="s">
+      <c r="C63" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="9" t="s">
+      <c r="A64" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="C64" s="9" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="9" t="s">
+      <c r="A65" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B65" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C65" s="9" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="9" t="s">
+      <c r="A66" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B66" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C66" s="8" t="s">
+      <c r="C66" s="9" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="9" t="s">
+      <c r="A67" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="B67" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="C67" s="8" t="s">
+      <c r="C67" s="9" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="9" t="s">
+      <c r="A68" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B68" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C68" s="9" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="9" t="s">
+      <c r="A69" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="B69" s="8" t="s">
+      <c r="B69" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="C69" s="8" t="s">
+      <c r="C69" s="9" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="9" t="s">
+      <c r="A70" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="B70" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="C70" s="8" t="s">
+      <c r="C70" s="9" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="9" t="s">
+      <c r="A71" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="B71" s="8" t="s">
+      <c r="B71" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="C71" s="9" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="9" t="s">
+      <c r="A72" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="B72" s="8" t="s">
+      <c r="B72" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="C72" s="8" t="s">
+      <c r="C72" s="9" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="9" t="s">
+      <c r="A73" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="B73" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="C73" s="8" t="s">
+      <c r="C73" s="9" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="9" t="s">
+      <c r="A74" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B74" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="C74" s="8" t="s">
+      <c r="C74" s="9" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="9" t="s">
+      <c r="A75" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="B75" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="C75" s="8" t="s">
+      <c r="C75" s="9" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="9" t="s">
+      <c r="A76" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="B76" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="C76" s="8" t="s">
+      <c r="C76" s="9" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="10"/>
+      <c r="A77" s="11"/>
     </row>
     <row r="78">
-      <c r="A78" s="10"/>
+      <c r="A78" s="11"/>
     </row>
     <row r="79">
-      <c r="A79" s="10"/>
+      <c r="A79" s="11"/>
     </row>
     <row r="80">
-      <c r="A80" s="10"/>
+      <c r="A80" s="11"/>
     </row>
     <row r="81">
-      <c r="A81" s="10"/>
+      <c r="A81" s="11"/>
     </row>
     <row r="82">
-      <c r="A82" s="10"/>
+      <c r="A82" s="11"/>
     </row>
     <row r="83">
-      <c r="A83" s="10"/>
+      <c r="A83" s="11"/>
     </row>
     <row r="84">
-      <c r="A84" s="10"/>
+      <c r="A84" s="11"/>
     </row>
     <row r="85">
-      <c r="A85" s="10"/>
+      <c r="A85" s="11"/>
     </row>
     <row r="86">
-      <c r="A86" s="10"/>
+      <c r="A86" s="11"/>
     </row>
     <row r="87">
-      <c r="A87" s="10"/>
+      <c r="A87" s="11"/>
     </row>
     <row r="88">
-      <c r="A88" s="10"/>
+      <c r="A88" s="11"/>
     </row>
     <row r="89">
-      <c r="A89" s="10"/>
+      <c r="A89" s="11"/>
     </row>
     <row r="90">
-      <c r="A90" s="10"/>
+      <c r="A90" s="11"/>
     </row>
     <row r="91">
-      <c r="A91" s="10"/>
+      <c r="A91" s="11"/>
     </row>
     <row r="92">
-      <c r="A92" s="10"/>
+      <c r="A92" s="11"/>
     </row>
     <row r="93">
-      <c r="A93" s="10"/>
+      <c r="A93" s="11"/>
     </row>
     <row r="94">
-      <c r="A94" s="10"/>
+      <c r="A94" s="11"/>
     </row>
     <row r="95">
-      <c r="A95" s="10"/>
+      <c r="A95" s="11"/>
     </row>
     <row r="96">
-      <c r="A96" s="10"/>
+      <c r="A96" s="11"/>
     </row>
     <row r="97">
-      <c r="A97" s="10"/>
+      <c r="A97" s="11"/>
     </row>
     <row r="98">
-      <c r="A98" s="10"/>
+      <c r="A98" s="11"/>
     </row>
     <row r="99">
-      <c r="A99" s="10"/>
+      <c r="A99" s="11"/>
     </row>
     <row r="100">
-      <c r="A100" s="10"/>
+      <c r="A100" s="11"/>
     </row>
     <row r="101">
-      <c r="A101" s="10"/>
+      <c r="A101" s="11"/>
     </row>
     <row r="102">
-      <c r="A102" s="10"/>
+      <c r="A102" s="11"/>
     </row>
     <row r="103">
-      <c r="A103" s="10"/>
+      <c r="A103" s="11"/>
     </row>
     <row r="104">
-      <c r="A104" s="10"/>
+      <c r="A104" s="11"/>
     </row>
     <row r="105">
-      <c r="A105" s="10"/>
+      <c r="A105" s="11"/>
     </row>
     <row r="106">
-      <c r="A106" s="10"/>
+      <c r="A106" s="11"/>
     </row>
     <row r="107">
-      <c r="A107" s="10"/>
+      <c r="A107" s="11"/>
     </row>
     <row r="108">
-      <c r="A108" s="10"/>
+      <c r="A108" s="11"/>
     </row>
     <row r="109">
-      <c r="A109" s="10"/>
+      <c r="A109" s="11"/>
     </row>
     <row r="110">
-      <c r="A110" s="10"/>
+      <c r="A110" s="11"/>
     </row>
     <row r="111">
-      <c r="A111" s="10"/>
+      <c r="A111" s="11"/>
     </row>
     <row r="112">
-      <c r="A112" s="10"/>
+      <c r="A112" s="11"/>
     </row>
     <row r="113">
-      <c r="A113" s="10"/>
+      <c r="A113" s="11"/>
     </row>
     <row r="114">
-      <c r="A114" s="10"/>
+      <c r="A114" s="11"/>
     </row>
     <row r="115">
-      <c r="A115" s="10"/>
+      <c r="A115" s="11"/>
     </row>
     <row r="116">
-      <c r="A116" s="10"/>
+      <c r="A116" s="11"/>
     </row>
     <row r="117">
-      <c r="A117" s="10"/>
+      <c r="A117" s="11"/>
     </row>
     <row r="118">
-      <c r="A118" s="10"/>
+      <c r="A118" s="11"/>
     </row>
     <row r="119">
-      <c r="A119" s="10"/>
+      <c r="A119" s="11"/>
     </row>
     <row r="120">
-      <c r="A120" s="10"/>
+      <c r="A120" s="11"/>
     </row>
     <row r="121">
-      <c r="A121" s="10"/>
+      <c r="A121" s="11"/>
     </row>
     <row r="122">
-      <c r="A122" s="10"/>
+      <c r="A122" s="11"/>
     </row>
     <row r="123">
-      <c r="A123" s="10"/>
+      <c r="A123" s="11"/>
     </row>
     <row r="124">
-      <c r="A124" s="10"/>
+      <c r="A124" s="11"/>
     </row>
     <row r="125">
-      <c r="A125" s="10"/>
+      <c r="A125" s="11"/>
     </row>
     <row r="126">
-      <c r="A126" s="10"/>
+      <c r="A126" s="11"/>
     </row>
     <row r="127">
-      <c r="A127" s="10"/>
+      <c r="A127" s="11"/>
     </row>
     <row r="128">
-      <c r="A128" s="10"/>
+      <c r="A128" s="11"/>
     </row>
     <row r="129">
-      <c r="A129" s="10"/>
+      <c r="A129" s="11"/>
     </row>
     <row r="130">
-      <c r="A130" s="10"/>
+      <c r="A130" s="11"/>
     </row>
     <row r="131">
-      <c r="A131" s="10"/>
+      <c r="A131" s="11"/>
     </row>
     <row r="132">
-      <c r="A132" s="10"/>
+      <c r="A132" s="11"/>
     </row>
     <row r="133">
-      <c r="A133" s="10"/>
+      <c r="A133" s="11"/>
     </row>
     <row r="134">
-      <c r="A134" s="10"/>
+      <c r="A134" s="11"/>
     </row>
     <row r="135">
-      <c r="A135" s="10"/>
+      <c r="A135" s="11"/>
     </row>
     <row r="136">
-      <c r="A136" s="10"/>
+      <c r="A136" s="11"/>
     </row>
     <row r="137">
-      <c r="A137" s="10"/>
+      <c r="A137" s="11"/>
     </row>
     <row r="138">
-      <c r="A138" s="10"/>
+      <c r="A138" s="11"/>
     </row>
     <row r="139">
-      <c r="A139" s="10"/>
+      <c r="A139" s="11"/>
     </row>
     <row r="140">
-      <c r="A140" s="10"/>
+      <c r="A140" s="11"/>
     </row>
     <row r="141">
-      <c r="A141" s="10"/>
+      <c r="A141" s="11"/>
     </row>
     <row r="142">
-      <c r="A142" s="10"/>
+      <c r="A142" s="11"/>
     </row>
     <row r="143">
-      <c r="A143" s="10"/>
+      <c r="A143" s="11"/>
     </row>
     <row r="144">
-      <c r="A144" s="10"/>
+      <c r="A144" s="11"/>
     </row>
     <row r="145">
-      <c r="A145" s="10"/>
+      <c r="A145" s="11"/>
     </row>
     <row r="146">
-      <c r="A146" s="10"/>
+      <c r="A146" s="11"/>
     </row>
     <row r="147">
-      <c r="A147" s="10"/>
+      <c r="A147" s="11"/>
     </row>
     <row r="148">
-      <c r="A148" s="10"/>
+      <c r="A148" s="11"/>
     </row>
     <row r="149">
-      <c r="A149" s="10"/>
+      <c r="A149" s="11"/>
     </row>
     <row r="150">
-      <c r="A150" s="10"/>
+      <c r="A150" s="11"/>
     </row>
     <row r="151">
-      <c r="A151" s="10"/>
+      <c r="A151" s="11"/>
     </row>
     <row r="152">
-      <c r="A152" s="10"/>
+      <c r="A152" s="11"/>
     </row>
     <row r="153">
-      <c r="A153" s="10"/>
+      <c r="A153" s="11"/>
     </row>
     <row r="154">
-      <c r="A154" s="10"/>
+      <c r="A154" s="11"/>
     </row>
     <row r="155">
-      <c r="A155" s="10"/>
+      <c r="A155" s="11"/>
     </row>
     <row r="156">
-      <c r="A156" s="10"/>
+      <c r="A156" s="11"/>
     </row>
     <row r="157">
-      <c r="A157" s="10"/>
+      <c r="A157" s="11"/>
     </row>
     <row r="158">
-      <c r="A158" s="10"/>
+      <c r="A158" s="11"/>
     </row>
     <row r="159">
-      <c r="A159" s="10"/>
+      <c r="A159" s="11"/>
     </row>
     <row r="160">
-      <c r="A160" s="10"/>
+      <c r="A160" s="11"/>
     </row>
     <row r="161">
-      <c r="A161" s="10"/>
+      <c r="A161" s="11"/>
     </row>
     <row r="162">
-      <c r="A162" s="10"/>
+      <c r="A162" s="11"/>
     </row>
     <row r="163">
-      <c r="A163" s="10"/>
+      <c r="A163" s="11"/>
     </row>
     <row r="164">
-      <c r="A164" s="10"/>
+      <c r="A164" s="11"/>
     </row>
     <row r="165">
-      <c r="A165" s="10"/>
+      <c r="A165" s="11"/>
     </row>
     <row r="166">
-      <c r="A166" s="10"/>
+      <c r="A166" s="11"/>
     </row>
     <row r="167">
-      <c r="A167" s="10"/>
+      <c r="A167" s="11"/>
     </row>
     <row r="168">
-      <c r="A168" s="10"/>
+      <c r="A168" s="11"/>
     </row>
     <row r="169">
-      <c r="A169" s="10"/>
+      <c r="A169" s="11"/>
     </row>
     <row r="170">
-      <c r="A170" s="10"/>
+      <c r="A170" s="11"/>
     </row>
     <row r="171">
-      <c r="A171" s="10"/>
+      <c r="A171" s="11"/>
     </row>
     <row r="172">
-      <c r="A172" s="10"/>
+      <c r="A172" s="11"/>
     </row>
     <row r="173">
-      <c r="A173" s="10"/>
+      <c r="A173" s="11"/>
     </row>
     <row r="174">
-      <c r="A174" s="10"/>
+      <c r="A174" s="11"/>
     </row>
     <row r="175">
-      <c r="A175" s="10"/>
+      <c r="A175" s="11"/>
     </row>
     <row r="176">
-      <c r="A176" s="10"/>
+      <c r="A176" s="11"/>
     </row>
     <row r="177">
-      <c r="A177" s="10"/>
+      <c r="A177" s="11"/>
     </row>
     <row r="178">
-      <c r="A178" s="10"/>
+      <c r="A178" s="11"/>
     </row>
     <row r="179">
-      <c r="A179" s="10"/>
+      <c r="A179" s="11"/>
     </row>
     <row r="180">
-      <c r="A180" s="10"/>
+      <c r="A180" s="11"/>
     </row>
     <row r="181">
-      <c r="A181" s="10"/>
+      <c r="A181" s="11"/>
     </row>
     <row r="182">
-      <c r="A182" s="10"/>
+      <c r="A182" s="11"/>
     </row>
     <row r="183">
-      <c r="A183" s="10"/>
+      <c r="A183" s="11"/>
     </row>
     <row r="184">
-      <c r="A184" s="10"/>
+      <c r="A184" s="11"/>
     </row>
     <row r="185">
-      <c r="A185" s="10"/>
+      <c r="A185" s="11"/>
     </row>
     <row r="186">
-      <c r="A186" s="10"/>
+      <c r="A186" s="11"/>
     </row>
     <row r="187">
-      <c r="A187" s="10"/>
+      <c r="A187" s="11"/>
     </row>
     <row r="188">
-      <c r="A188" s="10"/>
+      <c r="A188" s="11"/>
     </row>
     <row r="189">
-      <c r="A189" s="10"/>
+      <c r="A189" s="11"/>
     </row>
     <row r="190">
-      <c r="A190" s="10"/>
+      <c r="A190" s="11"/>
     </row>
     <row r="191">
-      <c r="A191" s="10"/>
+      <c r="A191" s="11"/>
     </row>
     <row r="192">
-      <c r="A192" s="10"/>
+      <c r="A192" s="11"/>
     </row>
     <row r="193">
-      <c r="A193" s="10"/>
+      <c r="A193" s="11"/>
     </row>
     <row r="194">
-      <c r="A194" s="10"/>
+      <c r="A194" s="11"/>
     </row>
     <row r="195">
-      <c r="A195" s="10"/>
+      <c r="A195" s="11"/>
     </row>
     <row r="196">
-      <c r="A196" s="10"/>
+      <c r="A196" s="11"/>
     </row>
     <row r="197">
-      <c r="A197" s="10"/>
+      <c r="A197" s="11"/>
     </row>
     <row r="198">
-      <c r="A198" s="10"/>
+      <c r="A198" s="11"/>
     </row>
     <row r="199">
-      <c r="A199" s="10"/>
+      <c r="A199" s="11"/>
     </row>
     <row r="200">
-      <c r="A200" s="10"/>
+      <c r="A200" s="11"/>
     </row>
     <row r="201">
-      <c r="A201" s="10"/>
+      <c r="A201" s="11"/>
     </row>
     <row r="202">
-      <c r="A202" s="10"/>
+      <c r="A202" s="11"/>
     </row>
     <row r="203">
-      <c r="A203" s="10"/>
+      <c r="A203" s="11"/>
     </row>
     <row r="204">
-      <c r="A204" s="10"/>
+      <c r="A204" s="11"/>
     </row>
     <row r="205">
-      <c r="A205" s="10"/>
+      <c r="A205" s="11"/>
     </row>
     <row r="206">
-      <c r="A206" s="10"/>
+      <c r="A206" s="11"/>
     </row>
     <row r="207">
-      <c r="A207" s="10"/>
+      <c r="A207" s="11"/>
     </row>
     <row r="208">
-      <c r="A208" s="10"/>
+      <c r="A208" s="11"/>
     </row>
     <row r="209">
-      <c r="A209" s="10"/>
+      <c r="A209" s="11"/>
     </row>
     <row r="210">
-      <c r="A210" s="10"/>
+      <c r="A210" s="11"/>
     </row>
     <row r="211">
-      <c r="A211" s="10"/>
+      <c r="A211" s="11"/>
     </row>
     <row r="212">
-      <c r="A212" s="10"/>
+      <c r="A212" s="11"/>
     </row>
     <row r="213">
-      <c r="A213" s="10"/>
+      <c r="A213" s="11"/>
     </row>
     <row r="214">
-      <c r="A214" s="10"/>
+      <c r="A214" s="11"/>
     </row>
     <row r="215">
-      <c r="A215" s="10"/>
+      <c r="A215" s="11"/>
     </row>
     <row r="216">
-      <c r="A216" s="10"/>
+      <c r="A216" s="11"/>
     </row>
     <row r="217">
-      <c r="A217" s="10"/>
+      <c r="A217" s="11"/>
     </row>
     <row r="218">
-      <c r="A218" s="10"/>
+      <c r="A218" s="11"/>
     </row>
     <row r="219">
-      <c r="A219" s="10"/>
+      <c r="A219" s="11"/>
     </row>
     <row r="220">
-      <c r="A220" s="10"/>
+      <c r="A220" s="11"/>
     </row>
     <row r="221">
-      <c r="A221" s="10"/>
+      <c r="A221" s="11"/>
     </row>
     <row r="222">
-      <c r="A222" s="10"/>
+      <c r="A222" s="11"/>
     </row>
     <row r="223">
-      <c r="A223" s="10"/>
+      <c r="A223" s="11"/>
     </row>
     <row r="224">
-      <c r="A224" s="10"/>
+      <c r="A224" s="11"/>
     </row>
     <row r="225">
-      <c r="A225" s="10"/>
+      <c r="A225" s="11"/>
     </row>
     <row r="226">
-      <c r="A226" s="10"/>
+      <c r="A226" s="11"/>
     </row>
     <row r="227">
-      <c r="A227" s="10"/>
+      <c r="A227" s="11"/>
     </row>
     <row r="228">
-      <c r="A228" s="10"/>
+      <c r="A228" s="11"/>
     </row>
     <row r="229">
-      <c r="A229" s="10"/>
+      <c r="A229" s="11"/>
     </row>
     <row r="230">
-      <c r="A230" s="10"/>
+      <c r="A230" s="11"/>
     </row>
     <row r="231">
-      <c r="A231" s="10"/>
+      <c r="A231" s="11"/>
     </row>
     <row r="232">
-      <c r="A232" s="10"/>
+      <c r="A232" s="11"/>
     </row>
     <row r="233">
-      <c r="A233" s="10"/>
+      <c r="A233" s="11"/>
     </row>
     <row r="234">
-      <c r="A234" s="10"/>
+      <c r="A234" s="11"/>
     </row>
     <row r="235">
-      <c r="A235" s="10"/>
+      <c r="A235" s="11"/>
     </row>
     <row r="236">
-      <c r="A236" s="10"/>
+      <c r="A236" s="11"/>
     </row>
     <row r="237">
-      <c r="A237" s="10"/>
+      <c r="A237" s="11"/>
     </row>
     <row r="238">
-      <c r="A238" s="10"/>
+      <c r="A238" s="11"/>
     </row>
     <row r="239">
-      <c r="A239" s="10"/>
+      <c r="A239" s="11"/>
     </row>
     <row r="240">
-      <c r="A240" s="10"/>
+      <c r="A240" s="11"/>
     </row>
     <row r="241">
-      <c r="A241" s="10"/>
+      <c r="A241" s="11"/>
     </row>
     <row r="242">
-      <c r="A242" s="10"/>
+      <c r="A242" s="11"/>
     </row>
     <row r="243">
-      <c r="A243" s="10"/>
+      <c r="A243" s="11"/>
     </row>
     <row r="244">
-      <c r="A244" s="10"/>
+      <c r="A244" s="11"/>
     </row>
     <row r="245">
-      <c r="A245" s="10"/>
+      <c r="A245" s="11"/>
     </row>
     <row r="246">
-      <c r="A246" s="10"/>
+      <c r="A246" s="11"/>
     </row>
     <row r="247">
-      <c r="A247" s="10"/>
+      <c r="A247" s="11"/>
     </row>
     <row r="248">
-      <c r="A248" s="10"/>
+      <c r="A248" s="11"/>
     </row>
     <row r="249">
-      <c r="A249" s="10"/>
+      <c r="A249" s="11"/>
     </row>
     <row r="250">
-      <c r="A250" s="10"/>
+      <c r="A250" s="11"/>
     </row>
     <row r="251">
-      <c r="A251" s="10"/>
+      <c r="A251" s="11"/>
     </row>
     <row r="252">
-      <c r="A252" s="10"/>
+      <c r="A252" s="11"/>
     </row>
     <row r="253">
-      <c r="A253" s="10"/>
+      <c r="A253" s="11"/>
     </row>
     <row r="254">
-      <c r="A254" s="10"/>
+      <c r="A254" s="11"/>
     </row>
     <row r="255">
-      <c r="A255" s="10"/>
+      <c r="A255" s="11"/>
     </row>
     <row r="256">
-      <c r="A256" s="10"/>
+      <c r="A256" s="11"/>
     </row>
     <row r="257">
-      <c r="A257" s="10"/>
+      <c r="A257" s="11"/>
     </row>
     <row r="258">
-      <c r="A258" s="10"/>
+      <c r="A258" s="11"/>
     </row>
     <row r="259">
-      <c r="A259" s="10"/>
+      <c r="A259" s="11"/>
     </row>
     <row r="260">
-      <c r="A260" s="10"/>
+      <c r="A260" s="11"/>
     </row>
     <row r="261">
-      <c r="A261" s="10"/>
+      <c r="A261" s="11"/>
     </row>
     <row r="262">
-      <c r="A262" s="10"/>
+      <c r="A262" s="11"/>
     </row>
     <row r="263">
-      <c r="A263" s="10"/>
+      <c r="A263" s="11"/>
     </row>
     <row r="264">
-      <c r="A264" s="10"/>
+      <c r="A264" s="11"/>
     </row>
     <row r="265">
-      <c r="A265" s="10"/>
+      <c r="A265" s="11"/>
     </row>
     <row r="266">
-      <c r="A266" s="10"/>
+      <c r="A266" s="11"/>
     </row>
     <row r="267">
-      <c r="A267" s="10"/>
+      <c r="A267" s="11"/>
     </row>
     <row r="268">
-      <c r="A268" s="10"/>
+      <c r="A268" s="11"/>
     </row>
     <row r="269">
-      <c r="A269" s="10"/>
+      <c r="A269" s="11"/>
     </row>
     <row r="270">
-      <c r="A270" s="10"/>
+      <c r="A270" s="11"/>
     </row>
     <row r="271">
-      <c r="A271" s="10"/>
+      <c r="A271" s="11"/>
     </row>
     <row r="272">
-      <c r="A272" s="10"/>
+      <c r="A272" s="11"/>
     </row>
     <row r="273">
-      <c r="A273" s="10"/>
+      <c r="A273" s="11"/>
     </row>
     <row r="274">
-      <c r="A274" s="10"/>
+      <c r="A274" s="11"/>
     </row>
     <row r="275">
-      <c r="A275" s="10"/>
+      <c r="A275" s="11"/>
     </row>
     <row r="276">
-      <c r="A276" s="10"/>
+      <c r="A276" s="11"/>
     </row>
     <row r="277">
-      <c r="A277" s="10"/>
+      <c r="A277" s="11"/>
     </row>
     <row r="278">
-      <c r="A278" s="10"/>
+      <c r="A278" s="11"/>
     </row>
     <row r="279">
-      <c r="A279" s="10"/>
+      <c r="A279" s="11"/>
     </row>
     <row r="280">
-      <c r="A280" s="10"/>
+      <c r="A280" s="11"/>
     </row>
     <row r="281">
-      <c r="A281" s="10"/>
+      <c r="A281" s="11"/>
     </row>
     <row r="282">
-      <c r="A282" s="10"/>
+      <c r="A282" s="11"/>
     </row>
     <row r="283">
-      <c r="A283" s="10"/>
+      <c r="A283" s="11"/>
     </row>
     <row r="284">
-      <c r="A284" s="10"/>
+      <c r="A284" s="11"/>
     </row>
     <row r="285">
-      <c r="A285" s="10"/>
+      <c r="A285" s="11"/>
     </row>
     <row r="286">
-      <c r="A286" s="10"/>
+      <c r="A286" s="11"/>
     </row>
     <row r="287">
-      <c r="A287" s="10"/>
+      <c r="A287" s="11"/>
     </row>
     <row r="288">
-      <c r="A288" s="10"/>
+      <c r="A288" s="11"/>
     </row>
     <row r="289">
-      <c r="A289" s="10"/>
+      <c r="A289" s="11"/>
     </row>
     <row r="290">
-      <c r="A290" s="10"/>
+      <c r="A290" s="11"/>
     </row>
     <row r="291">
-      <c r="A291" s="10"/>
+      <c r="A291" s="11"/>
     </row>
     <row r="292">
-      <c r="A292" s="10"/>
+      <c r="A292" s="11"/>
     </row>
     <row r="293">
-      <c r="A293" s="10"/>
+      <c r="A293" s="11"/>
     </row>
     <row r="294">
-      <c r="A294" s="10"/>
+      <c r="A294" s="11"/>
     </row>
     <row r="295">
-      <c r="A295" s="10"/>
+      <c r="A295" s="11"/>
     </row>
     <row r="296">
-      <c r="A296" s="10"/>
+      <c r="A296" s="11"/>
     </row>
     <row r="297">
-      <c r="A297" s="10"/>
+      <c r="A297" s="11"/>
     </row>
     <row r="298">
-      <c r="A298" s="10"/>
+      <c r="A298" s="11"/>
     </row>
     <row r="299">
-      <c r="A299" s="10"/>
+      <c r="A299" s="11"/>
     </row>
     <row r="300">
-      <c r="A300" s="10"/>
+      <c r="A300" s="11"/>
     </row>
     <row r="301">
-      <c r="A301" s="10"/>
+      <c r="A301" s="11"/>
     </row>
     <row r="302">
-      <c r="A302" s="10"/>
+      <c r="A302" s="11"/>
     </row>
     <row r="303">
-      <c r="A303" s="10"/>
+      <c r="A303" s="11"/>
     </row>
     <row r="304">
-      <c r="A304" s="10"/>
+      <c r="A304" s="11"/>
     </row>
     <row r="305">
-      <c r="A305" s="10"/>
+      <c r="A305" s="11"/>
     </row>
     <row r="306">
-      <c r="A306" s="10"/>
+      <c r="A306" s="11"/>
     </row>
     <row r="307">
-      <c r="A307" s="10"/>
+      <c r="A307" s="11"/>
     </row>
     <row r="308">
-      <c r="A308" s="10"/>
+      <c r="A308" s="11"/>
     </row>
     <row r="309">
-      <c r="A309" s="10"/>
+      <c r="A309" s="11"/>
     </row>
     <row r="310">
-      <c r="A310" s="10"/>
+      <c r="A310" s="11"/>
     </row>
     <row r="311">
-      <c r="A311" s="10"/>
+      <c r="A311" s="11"/>
     </row>
     <row r="312">
-      <c r="A312" s="10"/>
+      <c r="A312" s="11"/>
     </row>
     <row r="313">
-      <c r="A313" s="10"/>
+      <c r="A313" s="11"/>
     </row>
     <row r="314">
-      <c r="A314" s="10"/>
+      <c r="A314" s="11"/>
     </row>
     <row r="315">
-      <c r="A315" s="10"/>
+      <c r="A315" s="11"/>
     </row>
     <row r="316">
-      <c r="A316" s="10"/>
+      <c r="A316" s="11"/>
     </row>
     <row r="317">
-      <c r="A317" s="10"/>
+      <c r="A317" s="11"/>
     </row>
     <row r="318">
-      <c r="A318" s="10"/>
+      <c r="A318" s="11"/>
     </row>
     <row r="319">
-      <c r="A319" s="10"/>
+      <c r="A319" s="11"/>
     </row>
     <row r="320">
-      <c r="A320" s="10"/>
+      <c r="A320" s="11"/>
     </row>
     <row r="321">
-      <c r="A321" s="10"/>
+      <c r="A321" s="11"/>
     </row>
     <row r="322">
-      <c r="A322" s="10"/>
+      <c r="A322" s="11"/>
     </row>
     <row r="323">
-      <c r="A323" s="10"/>
+      <c r="A323" s="11"/>
     </row>
     <row r="324">
-      <c r="A324" s="10"/>
+      <c r="A324" s="11"/>
     </row>
     <row r="325">
-      <c r="A325" s="10"/>
+      <c r="A325" s="11"/>
     </row>
     <row r="326">
-      <c r="A326" s="10"/>
+      <c r="A326" s="11"/>
     </row>
     <row r="327">
-      <c r="A327" s="10"/>
+      <c r="A327" s="11"/>
     </row>
     <row r="328">
-      <c r="A328" s="10"/>
+      <c r="A328" s="11"/>
     </row>
     <row r="329">
-      <c r="A329" s="10"/>
+      <c r="A329" s="11"/>
     </row>
     <row r="330">
-      <c r="A330" s="10"/>
+      <c r="A330" s="11"/>
     </row>
     <row r="331">
-      <c r="A331" s="10"/>
+      <c r="A331" s="11"/>
     </row>
     <row r="332">
-      <c r="A332" s="10"/>
+      <c r="A332" s="11"/>
     </row>
     <row r="333">
-      <c r="A333" s="10"/>
+      <c r="A333" s="11"/>
     </row>
     <row r="334">
-      <c r="A334" s="10"/>
+      <c r="A334" s="11"/>
     </row>
     <row r="335">
-      <c r="A335" s="10"/>
+      <c r="A335" s="11"/>
     </row>
     <row r="336">
-      <c r="A336" s="10"/>
+      <c r="A336" s="11"/>
     </row>
     <row r="337">
-      <c r="A337" s="10"/>
+      <c r="A337" s="11"/>
     </row>
     <row r="338">
-      <c r="A338" s="10"/>
+      <c r="A338" s="11"/>
     </row>
     <row r="339">
-      <c r="A339" s="10"/>
+      <c r="A339" s="11"/>
     </row>
     <row r="340">
-      <c r="A340" s="10"/>
+      <c r="A340" s="11"/>
     </row>
     <row r="341">
-      <c r="A341" s="10"/>
+      <c r="A341" s="11"/>
     </row>
     <row r="342">
-      <c r="A342" s="10"/>
+      <c r="A342" s="11"/>
     </row>
     <row r="343">
-      <c r="A343" s="10"/>
+      <c r="A343" s="11"/>
     </row>
     <row r="344">
-      <c r="A344" s="10"/>
+      <c r="A344" s="11"/>
     </row>
     <row r="345">
-      <c r="A345" s="10"/>
+      <c r="A345" s="11"/>
     </row>
     <row r="346">
-      <c r="A346" s="10"/>
+      <c r="A346" s="11"/>
     </row>
     <row r="347">
-      <c r="A347" s="10"/>
+      <c r="A347" s="11"/>
     </row>
     <row r="348">
-      <c r="A348" s="10"/>
+      <c r="A348" s="11"/>
     </row>
     <row r="349">
-      <c r="A349" s="10"/>
+      <c r="A349" s="11"/>
     </row>
     <row r="350">
-      <c r="A350" s="10"/>
+      <c r="A350" s="11"/>
     </row>
     <row r="351">
-      <c r="A351" s="10"/>
+      <c r="A351" s="11"/>
     </row>
     <row r="352">
-      <c r="A352" s="10"/>
+      <c r="A352" s="11"/>
     </row>
     <row r="353">
-      <c r="A353" s="10"/>
+      <c r="A353" s="11"/>
     </row>
     <row r="354">
-      <c r="A354" s="10"/>
+      <c r="A354" s="11"/>
     </row>
     <row r="355">
-      <c r="A355" s="10"/>
+      <c r="A355" s="11"/>
     </row>
     <row r="356">
-      <c r="A356" s="10"/>
+      <c r="A356" s="11"/>
     </row>
     <row r="357">
-      <c r="A357" s="10"/>
+      <c r="A357" s="11"/>
     </row>
     <row r="358">
-      <c r="A358" s="10"/>
+      <c r="A358" s="11"/>
     </row>
     <row r="359">
-      <c r="A359" s="10"/>
+      <c r="A359" s="11"/>
     </row>
     <row r="360">
-      <c r="A360" s="10"/>
+      <c r="A360" s="11"/>
     </row>
     <row r="361">
-      <c r="A361" s="10"/>
+      <c r="A361" s="11"/>
     </row>
     <row r="362">
-      <c r="A362" s="10"/>
+      <c r="A362" s="11"/>
     </row>
     <row r="363">
-      <c r="A363" s="10"/>
+      <c r="A363" s="11"/>
     </row>
     <row r="364">
-      <c r="A364" s="10"/>
+      <c r="A364" s="11"/>
     </row>
     <row r="365">
-      <c r="A365" s="10"/>
+      <c r="A365" s="11"/>
     </row>
     <row r="366">
-      <c r="A366" s="10"/>
+      <c r="A366" s="11"/>
     </row>
     <row r="367">
-      <c r="A367" s="10"/>
+      <c r="A367" s="11"/>
     </row>
     <row r="368">
-      <c r="A368" s="10"/>
+      <c r="A368" s="11"/>
     </row>
     <row r="369">
-      <c r="A369" s="10"/>
+      <c r="A369" s="11"/>
     </row>
     <row r="370">
-      <c r="A370" s="10"/>
+      <c r="A370" s="11"/>
     </row>
     <row r="371">
-      <c r="A371" s="10"/>
+      <c r="A371" s="11"/>
     </row>
     <row r="372">
-      <c r="A372" s="10"/>
+      <c r="A372" s="11"/>
     </row>
     <row r="373">
-      <c r="A373" s="10"/>
+      <c r="A373" s="11"/>
     </row>
     <row r="374">
-      <c r="A374" s="10"/>
+      <c r="A374" s="11"/>
     </row>
     <row r="375">
-      <c r="A375" s="10"/>
+      <c r="A375" s="11"/>
     </row>
     <row r="376">
-      <c r="A376" s="10"/>
+      <c r="A376" s="11"/>
     </row>
     <row r="377">
-      <c r="A377" s="10"/>
+      <c r="A377" s="11"/>
     </row>
     <row r="378">
-      <c r="A378" s="10"/>
+      <c r="A378" s="11"/>
     </row>
     <row r="379">
-      <c r="A379" s="10"/>
+      <c r="A379" s="11"/>
     </row>
     <row r="380">
-      <c r="A380" s="10"/>
+      <c r="A380" s="11"/>
     </row>
     <row r="381">
-      <c r="A381" s="10"/>
+      <c r="A381" s="11"/>
     </row>
     <row r="382">
-      <c r="A382" s="10"/>
+      <c r="A382" s="11"/>
     </row>
     <row r="383">
-      <c r="A383" s="10"/>
+      <c r="A383" s="11"/>
     </row>
     <row r="384">
-      <c r="A384" s="10"/>
+      <c r="A384" s="11"/>
     </row>
     <row r="385">
-      <c r="A385" s="10"/>
+      <c r="A385" s="11"/>
     </row>
     <row r="386">
-      <c r="A386" s="10"/>
+      <c r="A386" s="11"/>
     </row>
     <row r="387">
-      <c r="A387" s="10"/>
+      <c r="A387" s="11"/>
     </row>
     <row r="388">
-      <c r="A388" s="10"/>
+      <c r="A388" s="11"/>
     </row>
     <row r="389">
-      <c r="A389" s="10"/>
+      <c r="A389" s="11"/>
     </row>
     <row r="390">
-      <c r="A390" s="10"/>
+      <c r="A390" s="11"/>
     </row>
     <row r="391">
-      <c r="A391" s="10"/>
+      <c r="A391" s="11"/>
     </row>
     <row r="392">
-      <c r="A392" s="10"/>
+      <c r="A392" s="11"/>
     </row>
     <row r="393">
-      <c r="A393" s="10"/>
+      <c r="A393" s="11"/>
     </row>
     <row r="394">
-      <c r="A394" s="10"/>
+      <c r="A394" s="11"/>
     </row>
     <row r="395">
-      <c r="A395" s="10"/>
+      <c r="A395" s="11"/>
     </row>
     <row r="396">
-      <c r="A396" s="10"/>
+      <c r="A396" s="11"/>
     </row>
     <row r="397">
-      <c r="A397" s="10"/>
+      <c r="A397" s="11"/>
     </row>
     <row r="398">
-      <c r="A398" s="10"/>
+      <c r="A398" s="11"/>
     </row>
     <row r="399">
-      <c r="A399" s="10"/>
+      <c r="A399" s="11"/>
     </row>
     <row r="400">
-      <c r="A400" s="10"/>
+      <c r="A400" s="11"/>
     </row>
     <row r="401">
-      <c r="A401" s="10"/>
+      <c r="A401" s="11"/>
     </row>
     <row r="402">
-      <c r="A402" s="10"/>
+      <c r="A402" s="11"/>
     </row>
     <row r="403">
-      <c r="A403" s="10"/>
+      <c r="A403" s="11"/>
     </row>
     <row r="404">
-      <c r="A404" s="10"/>
+      <c r="A404" s="11"/>
     </row>
     <row r="405">
-      <c r="A405" s="10"/>
+      <c r="A405" s="11"/>
     </row>
     <row r="406">
-      <c r="A406" s="10"/>
+      <c r="A406" s="11"/>
     </row>
     <row r="407">
-      <c r="A407" s="10"/>
+      <c r="A407" s="11"/>
     </row>
     <row r="408">
-      <c r="A408" s="10"/>
+      <c r="A408" s="11"/>
     </row>
     <row r="409">
-      <c r="A409" s="10"/>
+      <c r="A409" s="11"/>
     </row>
     <row r="410">
-      <c r="A410" s="10"/>
+      <c r="A410" s="11"/>
     </row>
     <row r="411">
-      <c r="A411" s="10"/>
+      <c r="A411" s="11"/>
     </row>
     <row r="412">
-      <c r="A412" s="10"/>
+      <c r="A412" s="11"/>
     </row>
     <row r="413">
-      <c r="A413" s="10"/>
+      <c r="A413" s="11"/>
     </row>
     <row r="414">
-      <c r="A414" s="10"/>
+      <c r="A414" s="11"/>
     </row>
     <row r="415">
-      <c r="A415" s="10"/>
+      <c r="A415" s="11"/>
     </row>
     <row r="416">
-      <c r="A416" s="10"/>
+      <c r="A416" s="11"/>
     </row>
     <row r="417">
-      <c r="A417" s="10"/>
+      <c r="A417" s="11"/>
     </row>
     <row r="418">
-      <c r="A418" s="10"/>
+      <c r="A418" s="11"/>
     </row>
     <row r="419">
-      <c r="A419" s="10"/>
+      <c r="A419" s="11"/>
     </row>
     <row r="420">
-      <c r="A420" s="10"/>
+      <c r="A420" s="11"/>
     </row>
     <row r="421">
-      <c r="A421" s="10"/>
+      <c r="A421" s="11"/>
     </row>
     <row r="422">
-      <c r="A422" s="10"/>
+      <c r="A422" s="11"/>
     </row>
     <row r="423">
-      <c r="A423" s="10"/>
+      <c r="A423" s="11"/>
     </row>
     <row r="424">
-      <c r="A424" s="10"/>
+      <c r="A424" s="11"/>
     </row>
     <row r="425">
-      <c r="A425" s="10"/>
+      <c r="A425" s="11"/>
     </row>
     <row r="426">
-      <c r="A426" s="10"/>
+      <c r="A426" s="11"/>
     </row>
     <row r="427">
-      <c r="A427" s="10"/>
+      <c r="A427" s="11"/>
     </row>
     <row r="428">
-      <c r="A428" s="10"/>
+      <c r="A428" s="11"/>
     </row>
     <row r="429">
-      <c r="A429" s="10"/>
+      <c r="A429" s="11"/>
     </row>
     <row r="430">
-      <c r="A430" s="10"/>
+      <c r="A430" s="11"/>
     </row>
     <row r="431">
-      <c r="A431" s="10"/>
+      <c r="A431" s="11"/>
     </row>
     <row r="432">
-      <c r="A432" s="10"/>
+      <c r="A432" s="11"/>
     </row>
     <row r="433">
-      <c r="A433" s="10"/>
+      <c r="A433" s="11"/>
     </row>
     <row r="434">
-      <c r="A434" s="10"/>
+      <c r="A434" s="11"/>
     </row>
     <row r="435">
-      <c r="A435" s="10"/>
+      <c r="A435" s="11"/>
     </row>
     <row r="436">
-      <c r="A436" s="10"/>
+      <c r="A436" s="11"/>
     </row>
     <row r="437">
-      <c r="A437" s="10"/>
+      <c r="A437" s="11"/>
     </row>
     <row r="438">
-      <c r="A438" s="10"/>
+      <c r="A438" s="11"/>
     </row>
     <row r="439">
-      <c r="A439" s="10"/>
+      <c r="A439" s="11"/>
     </row>
     <row r="440">
-      <c r="A440" s="10"/>
+      <c r="A440" s="11"/>
     </row>
     <row r="441">
-      <c r="A441" s="10"/>
+      <c r="A441" s="11"/>
     </row>
     <row r="442">
-      <c r="A442" s="10"/>
+      <c r="A442" s="11"/>
     </row>
     <row r="443">
-      <c r="A443" s="10"/>
+      <c r="A443" s="11"/>
     </row>
     <row r="444">
-      <c r="A444" s="10"/>
+      <c r="A444" s="11"/>
     </row>
     <row r="445">
-      <c r="A445" s="10"/>
+      <c r="A445" s="11"/>
     </row>
     <row r="446">
-      <c r="A446" s="10"/>
+      <c r="A446" s="11"/>
     </row>
     <row r="447">
-      <c r="A447" s="10"/>
+      <c r="A447" s="11"/>
     </row>
     <row r="448">
-      <c r="A448" s="10"/>
+      <c r="A448" s="11"/>
     </row>
     <row r="449">
-      <c r="A449" s="10"/>
+      <c r="A449" s="11"/>
     </row>
     <row r="450">
-      <c r="A450" s="10"/>
+      <c r="A450" s="11"/>
     </row>
     <row r="451">
-      <c r="A451" s="10"/>
+      <c r="A451" s="11"/>
     </row>
     <row r="452">
-      <c r="A452" s="10"/>
+      <c r="A452" s="11"/>
     </row>
     <row r="453">
-      <c r="A453" s="10"/>
+      <c r="A453" s="11"/>
     </row>
     <row r="454">
-      <c r="A454" s="10"/>
+      <c r="A454" s="11"/>
     </row>
     <row r="455">
-      <c r="A455" s="10"/>
+      <c r="A455" s="11"/>
     </row>
     <row r="456">
-      <c r="A456" s="10"/>
+      <c r="A456" s="11"/>
     </row>
     <row r="457">
-      <c r="A457" s="10"/>
+      <c r="A457" s="11"/>
     </row>
     <row r="458">
-      <c r="A458" s="10"/>
+      <c r="A458" s="11"/>
     </row>
     <row r="459">
-      <c r="A459" s="10"/>
+      <c r="A459" s="11"/>
     </row>
     <row r="460">
-      <c r="A460" s="10"/>
+      <c r="A460" s="11"/>
     </row>
     <row r="461">
-      <c r="A461" s="10"/>
+      <c r="A461" s="11"/>
     </row>
     <row r="462">
-      <c r="A462" s="10"/>
+      <c r="A462" s="11"/>
     </row>
     <row r="463">
-      <c r="A463" s="10"/>
+      <c r="A463" s="11"/>
     </row>
     <row r="464">
-      <c r="A464" s="10"/>
+      <c r="A464" s="11"/>
     </row>
     <row r="465">
-      <c r="A465" s="10"/>
+      <c r="A465" s="11"/>
     </row>
     <row r="466">
-      <c r="A466" s="10"/>
+      <c r="A466" s="11"/>
     </row>
     <row r="467">
-      <c r="A467" s="10"/>
+      <c r="A467" s="11"/>
     </row>
     <row r="468">
-      <c r="A468" s="10"/>
+      <c r="A468" s="11"/>
     </row>
     <row r="469">
-      <c r="A469" s="10"/>
+      <c r="A469" s="11"/>
     </row>
     <row r="470">
-      <c r="A470" s="10"/>
+      <c r="A470" s="11"/>
     </row>
     <row r="471">
-      <c r="A471" s="10"/>
+      <c r="A471" s="11"/>
     </row>
     <row r="472">
-      <c r="A472" s="10"/>
+      <c r="A472" s="11"/>
     </row>
     <row r="473">
-      <c r="A473" s="10"/>
+      <c r="A473" s="11"/>
     </row>
     <row r="474">
-      <c r="A474" s="10"/>
+      <c r="A474" s="11"/>
     </row>
     <row r="475">
-      <c r="A475" s="10"/>
+      <c r="A475" s="11"/>
     </row>
     <row r="476">
-      <c r="A476" s="10"/>
+      <c r="A476" s="11"/>
     </row>
     <row r="477">
-      <c r="A477" s="10"/>
+      <c r="A477" s="11"/>
     </row>
     <row r="478">
-      <c r="A478" s="10"/>
+      <c r="A478" s="11"/>
     </row>
     <row r="479">
-      <c r="A479" s="10"/>
+      <c r="A479" s="11"/>
     </row>
     <row r="480">
-      <c r="A480" s="10"/>
+      <c r="A480" s="11"/>
     </row>
     <row r="481">
-      <c r="A481" s="10"/>
+      <c r="A481" s="11"/>
     </row>
     <row r="482">
-      <c r="A482" s="10"/>
+      <c r="A482" s="11"/>
     </row>
     <row r="483">
-      <c r="A483" s="10"/>
+      <c r="A483" s="11"/>
     </row>
     <row r="484">
-      <c r="A484" s="10"/>
+      <c r="A484" s="11"/>
     </row>
     <row r="485">
-      <c r="A485" s="10"/>
+      <c r="A485" s="11"/>
     </row>
     <row r="486">
-      <c r="A486" s="10"/>
+      <c r="A486" s="11"/>
     </row>
     <row r="487">
-      <c r="A487" s="10"/>
+      <c r="A487" s="11"/>
     </row>
     <row r="488">
-      <c r="A488" s="10"/>
+      <c r="A488" s="11"/>
     </row>
     <row r="489">
-      <c r="A489" s="10"/>
+      <c r="A489" s="11"/>
     </row>
     <row r="490">
-      <c r="A490" s="10"/>
+      <c r="A490" s="11"/>
     </row>
     <row r="491">
-      <c r="A491" s="10"/>
+      <c r="A491" s="11"/>
     </row>
     <row r="492">
-      <c r="A492" s="10"/>
+      <c r="A492" s="11"/>
     </row>
     <row r="493">
-      <c r="A493" s="10"/>
+      <c r="A493" s="11"/>
     </row>
     <row r="494">
-      <c r="A494" s="10"/>
+      <c r="A494" s="11"/>
     </row>
     <row r="495">
-      <c r="A495" s="10"/>
+      <c r="A495" s="11"/>
     </row>
     <row r="496">
-      <c r="A496" s="10"/>
+      <c r="A496" s="11"/>
     </row>
     <row r="497">
-      <c r="A497" s="10"/>
+      <c r="A497" s="11"/>
     </row>
     <row r="498">
-      <c r="A498" s="10"/>
+      <c r="A498" s="11"/>
     </row>
     <row r="499">
-      <c r="A499" s="10"/>
+      <c r="A499" s="11"/>
     </row>
     <row r="500">
-      <c r="A500" s="10"/>
+      <c r="A500" s="11"/>
     </row>
     <row r="501">
-      <c r="A501" s="10"/>
+      <c r="A501" s="11"/>
     </row>
     <row r="502">
-      <c r="A502" s="10"/>
+      <c r="A502" s="11"/>
     </row>
     <row r="503">
-      <c r="A503" s="10"/>
+      <c r="A503" s="11"/>
     </row>
     <row r="504">
-      <c r="A504" s="10"/>
+      <c r="A504" s="11"/>
     </row>
     <row r="505">
-      <c r="A505" s="10"/>
+      <c r="A505" s="11"/>
     </row>
     <row r="506">
-      <c r="A506" s="10"/>
+      <c r="A506" s="11"/>
     </row>
     <row r="507">
-      <c r="A507" s="10"/>
+      <c r="A507" s="11"/>
     </row>
     <row r="508">
-      <c r="A508" s="10"/>
+      <c r="A508" s="11"/>
     </row>
     <row r="509">
-      <c r="A509" s="10"/>
+      <c r="A509" s="11"/>
     </row>
     <row r="510">
-      <c r="A510" s="10"/>
+      <c r="A510" s="11"/>
     </row>
     <row r="511">
-      <c r="A511" s="10"/>
+      <c r="A511" s="11"/>
     </row>
     <row r="512">
-      <c r="A512" s="10"/>
+      <c r="A512" s="11"/>
     </row>
     <row r="513">
-      <c r="A513" s="10"/>
+      <c r="A513" s="11"/>
     </row>
     <row r="514">
-      <c r="A514" s="10"/>
+      <c r="A514" s="11"/>
     </row>
     <row r="515">
-      <c r="A515" s="10"/>
+      <c r="A515" s="11"/>
     </row>
     <row r="516">
-      <c r="A516" s="10"/>
+      <c r="A516" s="11"/>
     </row>
     <row r="517">
-      <c r="A517" s="10"/>
+      <c r="A517" s="11"/>
     </row>
     <row r="518">
-      <c r="A518" s="10"/>
+      <c r="A518" s="11"/>
     </row>
     <row r="519">
-      <c r="A519" s="10"/>
+      <c r="A519" s="11"/>
     </row>
     <row r="520">
-      <c r="A520" s="10"/>
+      <c r="A520" s="11"/>
     </row>
     <row r="521">
-      <c r="A521" s="10"/>
+      <c r="A521" s="11"/>
     </row>
     <row r="522">
-      <c r="A522" s="10"/>
+      <c r="A522" s="11"/>
     </row>
     <row r="523">
-      <c r="A523" s="10"/>
+      <c r="A523" s="11"/>
     </row>
     <row r="524">
-      <c r="A524" s="10"/>
+      <c r="A524" s="11"/>
     </row>
     <row r="525">
-      <c r="A525" s="10"/>
+      <c r="A525" s="11"/>
     </row>
     <row r="526">
-      <c r="A526" s="10"/>
+      <c r="A526" s="11"/>
     </row>
     <row r="527">
-      <c r="A527" s="10"/>
+      <c r="A527" s="11"/>
     </row>
     <row r="528">
-      <c r="A528" s="10"/>
+      <c r="A528" s="11"/>
     </row>
     <row r="529">
-      <c r="A529" s="10"/>
+      <c r="A529" s="11"/>
     </row>
     <row r="530">
-      <c r="A530" s="10"/>
+      <c r="A530" s="11"/>
     </row>
     <row r="531">
-      <c r="A531" s="10"/>
+      <c r="A531" s="11"/>
     </row>
     <row r="532">
-      <c r="A532" s="10"/>
+      <c r="A532" s="11"/>
     </row>
     <row r="533">
-      <c r="A533" s="10"/>
+      <c r="A533" s="11"/>
     </row>
     <row r="534">
-      <c r="A534" s="10"/>
+      <c r="A534" s="11"/>
     </row>
     <row r="535">
-      <c r="A535" s="10"/>
+      <c r="A535" s="11"/>
     </row>
     <row r="536">
-      <c r="A536" s="10"/>
+      <c r="A536" s="11"/>
     </row>
     <row r="537">
-      <c r="A537" s="10"/>
+      <c r="A537" s="11"/>
     </row>
     <row r="538">
-      <c r="A538" s="10"/>
+      <c r="A538" s="11"/>
     </row>
     <row r="539">
-      <c r="A539" s="10"/>
+      <c r="A539" s="11"/>
     </row>
     <row r="540">
-      <c r="A540" s="10"/>
+      <c r="A540" s="11"/>
     </row>
     <row r="541">
-      <c r="A541" s="10"/>
+      <c r="A541" s="11"/>
     </row>
     <row r="542">
-      <c r="A542" s="10"/>
+      <c r="A542" s="11"/>
     </row>
     <row r="543">
-      <c r="A543" s="10"/>
+      <c r="A543" s="11"/>
     </row>
     <row r="544">
-      <c r="A544" s="10"/>
+      <c r="A544" s="11"/>
     </row>
     <row r="545">
-      <c r="A545" s="10"/>
+      <c r="A545" s="11"/>
     </row>
     <row r="546">
-      <c r="A546" s="10"/>
+      <c r="A546" s="11"/>
     </row>
     <row r="547">
-      <c r="A547" s="10"/>
+      <c r="A547" s="11"/>
     </row>
     <row r="548">
-      <c r="A548" s="10"/>
+      <c r="A548" s="11"/>
     </row>
     <row r="549">
-      <c r="A549" s="10"/>
+      <c r="A549" s="11"/>
     </row>
     <row r="550">
-      <c r="A550" s="10"/>
+      <c r="A550" s="11"/>
     </row>
     <row r="551">
-      <c r="A551" s="10"/>
+      <c r="A551" s="11"/>
     </row>
     <row r="552">
-      <c r="A552" s="10"/>
+      <c r="A552" s="11"/>
     </row>
     <row r="553">
-      <c r="A553" s="10"/>
+      <c r="A553" s="11"/>
     </row>
     <row r="554">
-      <c r="A554" s="10"/>
+      <c r="A554" s="11"/>
     </row>
     <row r="555">
-      <c r="A555" s="10"/>
+      <c r="A555" s="11"/>
     </row>
     <row r="556">
-      <c r="A556" s="10"/>
+      <c r="A556" s="11"/>
     </row>
     <row r="557">
-      <c r="A557" s="10"/>
+      <c r="A557" s="11"/>
     </row>
     <row r="558">
-      <c r="A558" s="10"/>
+      <c r="A558" s="11"/>
     </row>
     <row r="559">
-      <c r="A559" s="10"/>
+      <c r="A559" s="11"/>
     </row>
     <row r="560">
-      <c r="A560" s="10"/>
+      <c r="A560" s="11"/>
     </row>
     <row r="561">
-      <c r="A561" s="10"/>
+      <c r="A561" s="11"/>
     </row>
     <row r="562">
-      <c r="A562" s="10"/>
+      <c r="A562" s="11"/>
     </row>
     <row r="563">
-      <c r="A563" s="10"/>
+      <c r="A563" s="11"/>
     </row>
     <row r="564">
-      <c r="A564" s="10"/>
+      <c r="A564" s="11"/>
     </row>
     <row r="565">
-      <c r="A565" s="10"/>
+      <c r="A565" s="11"/>
     </row>
     <row r="566">
-      <c r="A566" s="10"/>
+      <c r="A566" s="11"/>
     </row>
     <row r="567">
-      <c r="A567" s="10"/>
+      <c r="A567" s="11"/>
     </row>
     <row r="568">
-      <c r="A568" s="10"/>
+      <c r="A568" s="11"/>
     </row>
     <row r="569">
-      <c r="A569" s="10"/>
+      <c r="A569" s="11"/>
     </row>
     <row r="570">
-      <c r="A570" s="10"/>
+      <c r="A570" s="11"/>
     </row>
     <row r="571">
-      <c r="A571" s="10"/>
+      <c r="A571" s="11"/>
     </row>
     <row r="572">
-      <c r="A572" s="10"/>
+      <c r="A572" s="11"/>
     </row>
     <row r="573">
-      <c r="A573" s="10"/>
+      <c r="A573" s="11"/>
     </row>
     <row r="574">
-      <c r="A574" s="10"/>
+      <c r="A574" s="11"/>
     </row>
     <row r="575">
-      <c r="A575" s="10"/>
+      <c r="A575" s="11"/>
     </row>
     <row r="576">
-      <c r="A576" s="10"/>
+      <c r="A576" s="11"/>
     </row>
     <row r="577">
-      <c r="A577" s="10"/>
+      <c r="A577" s="11"/>
     </row>
     <row r="578">
-      <c r="A578" s="10"/>
+      <c r="A578" s="11"/>
     </row>
     <row r="579">
-      <c r="A579" s="10"/>
+      <c r="A579" s="11"/>
     </row>
     <row r="580">
-      <c r="A580" s="10"/>
+      <c r="A580" s="11"/>
     </row>
     <row r="581">
-      <c r="A581" s="10"/>
+      <c r="A581" s="11"/>
     </row>
     <row r="582">
-      <c r="A582" s="10"/>
+      <c r="A582" s="11"/>
     </row>
     <row r="583">
-      <c r="A583" s="10"/>
+      <c r="A583" s="11"/>
     </row>
     <row r="584">
-      <c r="A584" s="10"/>
+      <c r="A584" s="11"/>
     </row>
     <row r="585">
-      <c r="A585" s="10"/>
+      <c r="A585" s="11"/>
     </row>
     <row r="586">
-      <c r="A586" s="10"/>
+      <c r="A586" s="11"/>
     </row>
     <row r="587">
-      <c r="A587" s="10"/>
+      <c r="A587" s="11"/>
     </row>
     <row r="588">
-      <c r="A588" s="10"/>
+      <c r="A588" s="11"/>
     </row>
     <row r="589">
-      <c r="A589" s="10"/>
+      <c r="A589" s="11"/>
     </row>
     <row r="590">
-      <c r="A590" s="10"/>
+      <c r="A590" s="11"/>
     </row>
     <row r="591">
-      <c r="A591" s="10"/>
+      <c r="A591" s="11"/>
     </row>
     <row r="592">
-      <c r="A592" s="10"/>
+      <c r="A592" s="11"/>
     </row>
     <row r="593">
-      <c r="A593" s="10"/>
+      <c r="A593" s="11"/>
     </row>
     <row r="594">
-      <c r="A594" s="10"/>
+      <c r="A594" s="11"/>
     </row>
     <row r="595">
-      <c r="A595" s="10"/>
+      <c r="A595" s="11"/>
     </row>
     <row r="596">
-      <c r="A596" s="10"/>
+      <c r="A596" s="11"/>
     </row>
     <row r="597">
-      <c r="A597" s="10"/>
+      <c r="A597" s="11"/>
     </row>
     <row r="598">
-      <c r="A598" s="10"/>
+      <c r="A598" s="11"/>
     </row>
     <row r="599">
-      <c r="A599" s="10"/>
+      <c r="A599" s="11"/>
     </row>
     <row r="600">
-      <c r="A600" s="10"/>
+      <c r="A600" s="11"/>
     </row>
     <row r="601">
-      <c r="A601" s="10"/>
+      <c r="A601" s="11"/>
     </row>
     <row r="602">
-      <c r="A602" s="10"/>
+      <c r="A602" s="11"/>
     </row>
     <row r="603">
-      <c r="A603" s="10"/>
+      <c r="A603" s="11"/>
     </row>
     <row r="604">
-      <c r="A604" s="10"/>
+      <c r="A604" s="11"/>
     </row>
     <row r="605">
-      <c r="A605" s="10"/>
+      <c r="A605" s="11"/>
     </row>
     <row r="606">
-      <c r="A606" s="10"/>
+      <c r="A606" s="11"/>
     </row>
     <row r="607">
-      <c r="A607" s="10"/>
+      <c r="A607" s="11"/>
     </row>
     <row r="608">
-      <c r="A608" s="10"/>
+      <c r="A608" s="11"/>
     </row>
     <row r="609">
-      <c r="A609" s="10"/>
+      <c r="A609" s="11"/>
     </row>
     <row r="610">
-      <c r="A610" s="10"/>
+      <c r="A610" s="11"/>
     </row>
     <row r="611">
-      <c r="A611" s="10"/>
+      <c r="A611" s="11"/>
     </row>
     <row r="612">
-      <c r="A612" s="10"/>
+      <c r="A612" s="11"/>
     </row>
     <row r="613">
-      <c r="A613" s="10"/>
+      <c r="A613" s="11"/>
     </row>
     <row r="614">
-      <c r="A614" s="10"/>
+      <c r="A614" s="11"/>
     </row>
     <row r="615">
-      <c r="A615" s="10"/>
+      <c r="A615" s="11"/>
     </row>
     <row r="616">
-      <c r="A616" s="10"/>
+      <c r="A616" s="11"/>
     </row>
     <row r="617">
-      <c r="A617" s="10"/>
+      <c r="A617" s="11"/>
     </row>
     <row r="618">
-      <c r="A618" s="10"/>
+      <c r="A618" s="11"/>
     </row>
     <row r="619">
-      <c r="A619" s="10"/>
+      <c r="A619" s="11"/>
     </row>
     <row r="620">
-      <c r="A620" s="10"/>
+      <c r="A620" s="11"/>
     </row>
     <row r="621">
-      <c r="A621" s="10"/>
+      <c r="A621" s="11"/>
     </row>
     <row r="622">
-      <c r="A622" s="10"/>
+      <c r="A622" s="11"/>
     </row>
     <row r="623">
-      <c r="A623" s="10"/>
+      <c r="A623" s="11"/>
     </row>
     <row r="624">
-      <c r="A624" s="10"/>
+      <c r="A624" s="11"/>
     </row>
     <row r="625">
-      <c r="A625" s="10"/>
+      <c r="A625" s="11"/>
     </row>
     <row r="626">
-      <c r="A626" s="10"/>
+      <c r="A626" s="11"/>
     </row>
     <row r="627">
-      <c r="A627" s="10"/>
+      <c r="A627" s="11"/>
     </row>
     <row r="628">
-      <c r="A628" s="10"/>
+      <c r="A628" s="11"/>
     </row>
     <row r="629">
-      <c r="A629" s="10"/>
+      <c r="A629" s="11"/>
     </row>
     <row r="630">
-      <c r="A630" s="10"/>
+      <c r="A630" s="11"/>
     </row>
     <row r="631">
-      <c r="A631" s="10"/>
+      <c r="A631" s="11"/>
     </row>
     <row r="632">
-      <c r="A632" s="10"/>
+      <c r="A632" s="11"/>
     </row>
     <row r="633">
-      <c r="A633" s="10"/>
+      <c r="A633" s="11"/>
     </row>
     <row r="634">
-      <c r="A634" s="10"/>
+      <c r="A634" s="11"/>
     </row>
     <row r="635">
-      <c r="A635" s="10"/>
+      <c r="A635" s="11"/>
     </row>
     <row r="636">
-      <c r="A636" s="10"/>
+      <c r="A636" s="11"/>
     </row>
     <row r="637">
-      <c r="A637" s="10"/>
+      <c r="A637" s="11"/>
     </row>
     <row r="638">
-      <c r="A638" s="10"/>
+      <c r="A638" s="11"/>
     </row>
     <row r="639">
-      <c r="A639" s="10"/>
+      <c r="A639" s="11"/>
     </row>
     <row r="640">
-      <c r="A640" s="10"/>
+      <c r="A640" s="11"/>
     </row>
     <row r="641">
-      <c r="A641" s="10"/>
+      <c r="A641" s="11"/>
     </row>
     <row r="642">
-      <c r="A642" s="10"/>
+      <c r="A642" s="11"/>
     </row>
     <row r="643">
-      <c r="A643" s="10"/>
+      <c r="A643" s="11"/>
     </row>
     <row r="644">
-      <c r="A644" s="10"/>
+      <c r="A644" s="11"/>
     </row>
     <row r="645">
-      <c r="A645" s="10"/>
+      <c r="A645" s="11"/>
     </row>
     <row r="646">
-      <c r="A646" s="10"/>
+      <c r="A646" s="11"/>
     </row>
     <row r="647">
-      <c r="A647" s="10"/>
+      <c r="A647" s="11"/>
     </row>
     <row r="648">
-      <c r="A648" s="10"/>
+      <c r="A648" s="11"/>
     </row>
     <row r="649">
-      <c r="A649" s="10"/>
+      <c r="A649" s="11"/>
     </row>
     <row r="650">
-      <c r="A650" s="10"/>
+      <c r="A650" s="11"/>
     </row>
     <row r="651">
-      <c r="A651" s="10"/>
+      <c r="A651" s="11"/>
     </row>
     <row r="652">
-      <c r="A652" s="10"/>
+      <c r="A652" s="11"/>
     </row>
     <row r="653">
-      <c r="A653" s="10"/>
+      <c r="A653" s="11"/>
     </row>
     <row r="654">
-      <c r="A654" s="10"/>
+      <c r="A654" s="11"/>
     </row>
     <row r="655">
-      <c r="A655" s="10"/>
+      <c r="A655" s="11"/>
     </row>
     <row r="656">
-      <c r="A656" s="10"/>
+      <c r="A656" s="11"/>
     </row>
     <row r="657">
-      <c r="A657" s="10"/>
+      <c r="A657" s="11"/>
     </row>
     <row r="658">
-      <c r="A658" s="10"/>
+      <c r="A658" s="11"/>
     </row>
     <row r="659">
-      <c r="A659" s="10"/>
+      <c r="A659" s="11"/>
     </row>
     <row r="660">
-      <c r="A660" s="10"/>
+      <c r="A660" s="11"/>
     </row>
     <row r="661">
-      <c r="A661" s="10"/>
+      <c r="A661" s="11"/>
     </row>
     <row r="662">
-      <c r="A662" s="10"/>
+      <c r="A662" s="11"/>
     </row>
     <row r="663">
-      <c r="A663" s="10"/>
+      <c r="A663" s="11"/>
     </row>
     <row r="664">
-      <c r="A664" s="10"/>
+      <c r="A664" s="11"/>
     </row>
     <row r="665">
-      <c r="A665" s="10"/>
+      <c r="A665" s="11"/>
     </row>
     <row r="666">
-      <c r="A666" s="10"/>
+      <c r="A666" s="11"/>
     </row>
     <row r="667">
-      <c r="A667" s="10"/>
+      <c r="A667" s="11"/>
     </row>
     <row r="668">
-      <c r="A668" s="10"/>
+      <c r="A668" s="11"/>
     </row>
     <row r="669">
-      <c r="A669" s="10"/>
+      <c r="A669" s="11"/>
     </row>
     <row r="670">
-      <c r="A670" s="10"/>
+      <c r="A670" s="11"/>
     </row>
     <row r="671">
-      <c r="A671" s="10"/>
+      <c r="A671" s="11"/>
     </row>
     <row r="672">
-      <c r="A672" s="10"/>
+      <c r="A672" s="11"/>
     </row>
     <row r="673">
-      <c r="A673" s="10"/>
+      <c r="A673" s="11"/>
     </row>
     <row r="674">
-      <c r="A674" s="10"/>
+      <c r="A674" s="11"/>
     </row>
     <row r="675">
-      <c r="A675" s="10"/>
+      <c r="A675" s="11"/>
     </row>
     <row r="676">
-      <c r="A676" s="10"/>
+      <c r="A676" s="11"/>
     </row>
     <row r="677">
-      <c r="A677" s="10"/>
+      <c r="A677" s="11"/>
     </row>
     <row r="678">
-      <c r="A678" s="10"/>
+      <c r="A678" s="11"/>
     </row>
     <row r="679">
-      <c r="A679" s="10"/>
+      <c r="A679" s="11"/>
     </row>
     <row r="680">
-      <c r="A680" s="10"/>
+      <c r="A680" s="11"/>
     </row>
     <row r="681">
-      <c r="A681" s="10"/>
+      <c r="A681" s="11"/>
     </row>
     <row r="682">
-      <c r="A682" s="10"/>
+      <c r="A682" s="11"/>
     </row>
     <row r="683">
-      <c r="A683" s="10"/>
+      <c r="A683" s="11"/>
     </row>
     <row r="684">
-      <c r="A684" s="10"/>
+      <c r="A684" s="11"/>
     </row>
     <row r="685">
-      <c r="A685" s="10"/>
+      <c r="A685" s="11"/>
     </row>
     <row r="686">
-      <c r="A686" s="10"/>
+      <c r="A686" s="11"/>
     </row>
     <row r="687">
-      <c r="A687" s="10"/>
+      <c r="A687" s="11"/>
     </row>
     <row r="688">
-      <c r="A688" s="10"/>
+      <c r="A688" s="11"/>
     </row>
     <row r="689">
-      <c r="A689" s="10"/>
+      <c r="A689" s="11"/>
     </row>
     <row r="690">
-      <c r="A690" s="10"/>
+      <c r="A690" s="11"/>
     </row>
     <row r="691">
-      <c r="A691" s="10"/>
+      <c r="A691" s="11"/>
     </row>
     <row r="692">
-      <c r="A692" s="10"/>
+      <c r="A692" s="11"/>
     </row>
     <row r="693">
-      <c r="A693" s="10"/>
+      <c r="A693" s="11"/>
     </row>
     <row r="694">
-      <c r="A694" s="10"/>
+      <c r="A694" s="11"/>
     </row>
     <row r="695">
-      <c r="A695" s="10"/>
+      <c r="A695" s="11"/>
     </row>
     <row r="696">
-      <c r="A696" s="10"/>
+      <c r="A696" s="11"/>
     </row>
     <row r="697">
-      <c r="A697" s="10"/>
+      <c r="A697" s="11"/>
     </row>
     <row r="698">
-      <c r="A698" s="10"/>
+      <c r="A698" s="11"/>
     </row>
     <row r="699">
-      <c r="A699" s="10"/>
+      <c r="A699" s="11"/>
     </row>
     <row r="700">
-      <c r="A700" s="10"/>
+      <c r="A700" s="11"/>
     </row>
     <row r="701">
-      <c r="A701" s="10"/>
+      <c r="A701" s="11"/>
     </row>
     <row r="702">
-      <c r="A702" s="10"/>
+      <c r="A702" s="11"/>
     </row>
     <row r="703">
-      <c r="A703" s="10"/>
+      <c r="A703" s="11"/>
     </row>
     <row r="704">
-      <c r="A704" s="10"/>
+      <c r="A704" s="11"/>
     </row>
     <row r="705">
-      <c r="A705" s="10"/>
+      <c r="A705" s="11"/>
     </row>
     <row r="706">
-      <c r="A706" s="10"/>
+      <c r="A706" s="11"/>
     </row>
     <row r="707">
-      <c r="A707" s="10"/>
+      <c r="A707" s="11"/>
     </row>
     <row r="708">
-      <c r="A708" s="10"/>
+      <c r="A708" s="11"/>
     </row>
     <row r="709">
-      <c r="A709" s="10"/>
+      <c r="A709" s="11"/>
     </row>
     <row r="710">
-      <c r="A710" s="10"/>
+      <c r="A710" s="11"/>
     </row>
     <row r="711">
-      <c r="A711" s="10"/>
+      <c r="A711" s="11"/>
     </row>
     <row r="712">
-      <c r="A712" s="10"/>
+      <c r="A712" s="11"/>
     </row>
     <row r="713">
-      <c r="A713" s="10"/>
+      <c r="A713" s="11"/>
     </row>
     <row r="714">
-      <c r="A714" s="10"/>
+      <c r="A714" s="11"/>
     </row>
     <row r="715">
-      <c r="A715" s="10"/>
+      <c r="A715" s="11"/>
     </row>
     <row r="716">
-      <c r="A716" s="10"/>
+      <c r="A716" s="11"/>
     </row>
     <row r="717">
-      <c r="A717" s="10"/>
+      <c r="A717" s="11"/>
     </row>
     <row r="718">
-      <c r="A718" s="10"/>
+      <c r="A718" s="11"/>
     </row>
     <row r="719">
-      <c r="A719" s="10"/>
+      <c r="A719" s="11"/>
     </row>
     <row r="720">
-      <c r="A720" s="10"/>
+      <c r="A720" s="11"/>
     </row>
     <row r="721">
-      <c r="A721" s="10"/>
+      <c r="A721" s="11"/>
     </row>
     <row r="722">
-      <c r="A722" s="10"/>
+      <c r="A722" s="11"/>
     </row>
     <row r="723">
-      <c r="A723" s="10"/>
+      <c r="A723" s="11"/>
     </row>
     <row r="724">
-      <c r="A724" s="10"/>
+      <c r="A724" s="11"/>
     </row>
     <row r="725">
-      <c r="A725" s="10"/>
+      <c r="A725" s="11"/>
     </row>
     <row r="726">
-      <c r="A726" s="10"/>
+      <c r="A726" s="11"/>
     </row>
     <row r="727">
-      <c r="A727" s="10"/>
+      <c r="A727" s="11"/>
     </row>
     <row r="728">
-      <c r="A728" s="10"/>
+      <c r="A728" s="11"/>
     </row>
     <row r="729">
-      <c r="A729" s="10"/>
+      <c r="A729" s="11"/>
     </row>
     <row r="730">
-      <c r="A730" s="10"/>
+      <c r="A730" s="11"/>
     </row>
     <row r="731">
-      <c r="A731" s="10"/>
+      <c r="A731" s="11"/>
     </row>
     <row r="732">
-      <c r="A732" s="10"/>
+      <c r="A732" s="11"/>
     </row>
     <row r="733">
-      <c r="A733" s="10"/>
+      <c r="A733" s="11"/>
     </row>
     <row r="734">
-      <c r="A734" s="10"/>
+      <c r="A734" s="11"/>
     </row>
     <row r="735">
-      <c r="A735" s="10"/>
+      <c r="A735" s="11"/>
     </row>
     <row r="736">
-      <c r="A736" s="10"/>
+      <c r="A736" s="11"/>
     </row>
     <row r="737">
-      <c r="A737" s="10"/>
+      <c r="A737" s="11"/>
     </row>
     <row r="738">
-      <c r="A738" s="10"/>
+      <c r="A738" s="11"/>
     </row>
     <row r="739">
-      <c r="A739" s="10"/>
+      <c r="A739" s="11"/>
     </row>
     <row r="740">
-      <c r="A740" s="10"/>
+      <c r="A740" s="11"/>
     </row>
     <row r="741">
-      <c r="A741" s="10"/>
+      <c r="A741" s="11"/>
     </row>
     <row r="742">
-      <c r="A742" s="10"/>
+      <c r="A742" s="11"/>
     </row>
     <row r="743">
-      <c r="A743" s="10"/>
+      <c r="A743" s="11"/>
     </row>
     <row r="744">
-      <c r="A744" s="10"/>
+      <c r="A744" s="11"/>
     </row>
     <row r="745">
-      <c r="A745" s="10"/>
+      <c r="A745" s="11"/>
     </row>
     <row r="746">
-      <c r="A746" s="10"/>
+      <c r="A746" s="11"/>
     </row>
     <row r="747">
-      <c r="A747" s="10"/>
+      <c r="A747" s="11"/>
     </row>
     <row r="748">
-      <c r="A748" s="10"/>
+      <c r="A748" s="11"/>
     </row>
     <row r="749">
-      <c r="A749" s="10"/>
+      <c r="A749" s="11"/>
     </row>
     <row r="750">
-      <c r="A750" s="10"/>
+      <c r="A750" s="11"/>
     </row>
     <row r="751">
-      <c r="A751" s="10"/>
+      <c r="A751" s="11"/>
     </row>
     <row r="752">
-      <c r="A752" s="10"/>
+      <c r="A752" s="11"/>
     </row>
     <row r="753">
-      <c r="A753" s="10"/>
+      <c r="A753" s="11"/>
     </row>
     <row r="754">
-      <c r="A754" s="10"/>
+      <c r="A754" s="11"/>
     </row>
     <row r="755">
-      <c r="A755" s="10"/>
+      <c r="A755" s="11"/>
     </row>
     <row r="756">
-      <c r="A756" s="10"/>
+      <c r="A756" s="11"/>
     </row>
     <row r="757">
-      <c r="A757" s="10"/>
+      <c r="A757" s="11"/>
     </row>
     <row r="758">
-      <c r="A758" s="10"/>
+      <c r="A758" s="11"/>
     </row>
     <row r="759">
-      <c r="A759" s="10"/>
+      <c r="A759" s="11"/>
     </row>
     <row r="760">
-      <c r="A760" s="10"/>
+      <c r="A760" s="11"/>
     </row>
     <row r="761">
-      <c r="A761" s="10"/>
+      <c r="A761" s="11"/>
     </row>
     <row r="762">
-      <c r="A762" s="10"/>
+      <c r="A762" s="11"/>
     </row>
     <row r="763">
-      <c r="A763" s="10"/>
+      <c r="A763" s="11"/>
     </row>
     <row r="764">
-      <c r="A764" s="10"/>
+      <c r="A764" s="11"/>
     </row>
     <row r="765">
-      <c r="A765" s="10"/>
+      <c r="A765" s="11"/>
     </row>
     <row r="766">
-      <c r="A766" s="10"/>
+      <c r="A766" s="11"/>
     </row>
     <row r="767">
-      <c r="A767" s="10"/>
+      <c r="A767" s="11"/>
     </row>
     <row r="768">
-      <c r="A768" s="10"/>
+      <c r="A768" s="11"/>
     </row>
     <row r="769">
-      <c r="A769" s="10"/>
+      <c r="A769" s="11"/>
     </row>
     <row r="770">
-      <c r="A770" s="10"/>
+      <c r="A770" s="11"/>
     </row>
     <row r="771">
-      <c r="A771" s="10"/>
+      <c r="A771" s="11"/>
     </row>
     <row r="772">
-      <c r="A772" s="10"/>
+      <c r="A772" s="11"/>
     </row>
     <row r="773">
-      <c r="A773" s="10"/>
+      <c r="A773" s="11"/>
     </row>
     <row r="774">
-      <c r="A774" s="10"/>
+      <c r="A774" s="11"/>
     </row>
     <row r="775">
-      <c r="A775" s="10"/>
+      <c r="A775" s="11"/>
     </row>
     <row r="776">
-      <c r="A776" s="10"/>
+      <c r="A776" s="11"/>
     </row>
     <row r="777">
-      <c r="A777" s="10"/>
+      <c r="A777" s="11"/>
     </row>
     <row r="778">
-      <c r="A778" s="10"/>
+      <c r="A778" s="11"/>
     </row>
     <row r="779">
-      <c r="A779" s="10"/>
+      <c r="A779" s="11"/>
     </row>
     <row r="780">
-      <c r="A780" s="10"/>
+      <c r="A780" s="11"/>
     </row>
     <row r="781">
-      <c r="A781" s="10"/>
+      <c r="A781" s="11"/>
     </row>
     <row r="782">
-      <c r="A782" s="10"/>
+      <c r="A782" s="11"/>
     </row>
     <row r="783">
-      <c r="A783" s="10"/>
+      <c r="A783" s="11"/>
     </row>
     <row r="784">
-      <c r="A784" s="10"/>
+      <c r="A784" s="11"/>
     </row>
     <row r="785">
-      <c r="A785" s="10"/>
+      <c r="A785" s="11"/>
     </row>
     <row r="786">
-      <c r="A786" s="10"/>
+      <c r="A786" s="11"/>
     </row>
     <row r="787">
-      <c r="A787" s="10"/>
+      <c r="A787" s="11"/>
     </row>
     <row r="788">
-      <c r="A788" s="10"/>
+      <c r="A788" s="11"/>
     </row>
     <row r="789">
-      <c r="A789" s="10"/>
+      <c r="A789" s="11"/>
     </row>
     <row r="790">
-      <c r="A790" s="10"/>
+      <c r="A790" s="11"/>
     </row>
     <row r="791">
-      <c r="A791" s="10"/>
+      <c r="A791" s="11"/>
     </row>
     <row r="792">
-      <c r="A792" s="10"/>
+      <c r="A792" s="11"/>
     </row>
     <row r="793">
-      <c r="A793" s="10"/>
+      <c r="A793" s="11"/>
     </row>
     <row r="794">
-      <c r="A794" s="10"/>
+      <c r="A794" s="11"/>
     </row>
     <row r="795">
-      <c r="A795" s="10"/>
+      <c r="A795" s="11"/>
     </row>
     <row r="796">
-      <c r="A796" s="10"/>
+      <c r="A796" s="11"/>
     </row>
     <row r="797">
-      <c r="A797" s="10"/>
+      <c r="A797" s="11"/>
     </row>
     <row r="798">
-      <c r="A798" s="10"/>
+      <c r="A798" s="11"/>
     </row>
     <row r="799">
-      <c r="A799" s="10"/>
+      <c r="A799" s="11"/>
     </row>
     <row r="800">
-      <c r="A800" s="10"/>
+      <c r="A800" s="11"/>
     </row>
     <row r="801">
-      <c r="A801" s="10"/>
+      <c r="A801" s="11"/>
     </row>
     <row r="802">
-      <c r="A802" s="10"/>
+      <c r="A802" s="11"/>
     </row>
     <row r="803">
-      <c r="A803" s="10"/>
+      <c r="A803" s="11"/>
     </row>
     <row r="804">
-      <c r="A804" s="10"/>
+      <c r="A804" s="11"/>
     </row>
     <row r="805">
-      <c r="A805" s="10"/>
+      <c r="A805" s="11"/>
     </row>
     <row r="806">
-      <c r="A806" s="10"/>
+      <c r="A806" s="11"/>
     </row>
     <row r="807">
-      <c r="A807" s="10"/>
+      <c r="A807" s="11"/>
     </row>
     <row r="808">
-      <c r="A808" s="10"/>
+      <c r="A808" s="11"/>
     </row>
     <row r="809">
-      <c r="A809" s="10"/>
+      <c r="A809" s="11"/>
     </row>
     <row r="810">
-      <c r="A810" s="10"/>
+      <c r="A810" s="11"/>
     </row>
     <row r="811">
-      <c r="A811" s="10"/>
+      <c r="A811" s="11"/>
     </row>
     <row r="812">
-      <c r="A812" s="10"/>
+      <c r="A812" s="11"/>
     </row>
     <row r="813">
-      <c r="A813" s="10"/>
+      <c r="A813" s="11"/>
     </row>
     <row r="814">
-      <c r="A814" s="10"/>
+      <c r="A814" s="11"/>
     </row>
     <row r="815">
-      <c r="A815" s="10"/>
+      <c r="A815" s="11"/>
     </row>
     <row r="816">
-      <c r="A816" s="10"/>
+      <c r="A816" s="11"/>
     </row>
     <row r="817">
-      <c r="A817" s="10"/>
+      <c r="A817" s="11"/>
     </row>
     <row r="818">
-      <c r="A818" s="10"/>
+      <c r="A818" s="11"/>
     </row>
     <row r="819">
-      <c r="A819" s="10"/>
+      <c r="A819" s="11"/>
     </row>
     <row r="820">
-      <c r="A820" s="10"/>
+      <c r="A820" s="11"/>
     </row>
     <row r="821">
-      <c r="A821" s="10"/>
+      <c r="A821" s="11"/>
     </row>
     <row r="822">
-      <c r="A822" s="10"/>
+      <c r="A822" s="11"/>
     </row>
     <row r="823">
-      <c r="A823" s="10"/>
+      <c r="A823" s="11"/>
     </row>
     <row r="824">
-      <c r="A824" s="10"/>
+      <c r="A824" s="11"/>
     </row>
     <row r="825">
-      <c r="A825" s="10"/>
+      <c r="A825" s="11"/>
     </row>
     <row r="826">
-      <c r="A826" s="10"/>
+      <c r="A826" s="11"/>
     </row>
     <row r="827">
-      <c r="A827" s="10"/>
+      <c r="A827" s="11"/>
     </row>
     <row r="828">
-      <c r="A828" s="10"/>
+      <c r="A828" s="11"/>
     </row>
     <row r="829">
-      <c r="A829" s="10"/>
+      <c r="A829" s="11"/>
     </row>
     <row r="830">
-      <c r="A830" s="10"/>
+      <c r="A830" s="11"/>
     </row>
     <row r="831">
-      <c r="A831" s="10"/>
+      <c r="A831" s="11"/>
     </row>
     <row r="832">
-      <c r="A832" s="10"/>
+      <c r="A832" s="11"/>
     </row>
     <row r="833">
-      <c r="A833" s="10"/>
+      <c r="A833" s="11"/>
     </row>
     <row r="834">
-      <c r="A834" s="10"/>
+      <c r="A834" s="11"/>
     </row>
     <row r="835">
-      <c r="A835" s="10"/>
+      <c r="A835" s="11"/>
     </row>
     <row r="836">
-      <c r="A836" s="10"/>
+      <c r="A836" s="11"/>
     </row>
     <row r="837">
-      <c r="A837" s="10"/>
+      <c r="A837" s="11"/>
     </row>
     <row r="838">
-      <c r="A838" s="10"/>
+      <c r="A838" s="11"/>
     </row>
     <row r="839">
-      <c r="A839" s="10"/>
+      <c r="A839" s="11"/>
     </row>
     <row r="840">
-      <c r="A840" s="10"/>
+      <c r="A840" s="11"/>
     </row>
     <row r="841">
-      <c r="A841" s="10"/>
+      <c r="A841" s="11"/>
     </row>
     <row r="842">
-      <c r="A842" s="10"/>
+      <c r="A842" s="11"/>
     </row>
     <row r="843">
-      <c r="A843" s="10"/>
+      <c r="A843" s="11"/>
     </row>
     <row r="844">
-      <c r="A844" s="10"/>
+      <c r="A844" s="11"/>
     </row>
     <row r="845">
-      <c r="A845" s="10"/>
+      <c r="A845" s="11"/>
     </row>
     <row r="846">
-      <c r="A846" s="10"/>
+      <c r="A846" s="11"/>
     </row>
     <row r="847">
-      <c r="A847" s="10"/>
+      <c r="A847" s="11"/>
     </row>
     <row r="848">
-      <c r="A848" s="10"/>
+      <c r="A848" s="11"/>
     </row>
     <row r="849">
-      <c r="A849" s="10"/>
+      <c r="A849" s="11"/>
     </row>
     <row r="850">
-      <c r="A850" s="10"/>
+      <c r="A850" s="11"/>
     </row>
     <row r="851">
-      <c r="A851" s="10"/>
+      <c r="A851" s="11"/>
     </row>
     <row r="852">
-      <c r="A852" s="10"/>
+      <c r="A852" s="11"/>
     </row>
     <row r="853">
-      <c r="A853" s="10"/>
+      <c r="A853" s="11"/>
     </row>
     <row r="854">
-      <c r="A854" s="10"/>
+      <c r="A854" s="11"/>
     </row>
     <row r="855">
-      <c r="A855" s="10"/>
+      <c r="A855" s="11"/>
     </row>
     <row r="856">
-      <c r="A856" s="10"/>
+      <c r="A856" s="11"/>
     </row>
     <row r="857">
-      <c r="A857" s="10"/>
+      <c r="A857" s="11"/>
     </row>
     <row r="858">
-      <c r="A858" s="10"/>
+      <c r="A858" s="11"/>
     </row>
     <row r="859">
-      <c r="A859" s="10"/>
+      <c r="A859" s="11"/>
     </row>
     <row r="860">
-      <c r="A860" s="10"/>
+      <c r="A860" s="11"/>
     </row>
     <row r="861">
-      <c r="A861" s="10"/>
+      <c r="A861" s="11"/>
     </row>
     <row r="862">
-      <c r="A862" s="10"/>
+      <c r="A862" s="11"/>
     </row>
     <row r="863">
-      <c r="A863" s="10"/>
+      <c r="A863" s="11"/>
     </row>
     <row r="864">
-      <c r="A864" s="10"/>
+      <c r="A864" s="11"/>
     </row>
     <row r="865">
-      <c r="A865" s="10"/>
+      <c r="A865" s="11"/>
     </row>
     <row r="866">
-      <c r="A866" s="10"/>
+      <c r="A866" s="11"/>
     </row>
     <row r="867">
-      <c r="A867" s="10"/>
+      <c r="A867" s="11"/>
     </row>
     <row r="868">
-      <c r="A868" s="10"/>
+      <c r="A868" s="11"/>
     </row>
     <row r="869">
-      <c r="A869" s="10"/>
+      <c r="A869" s="11"/>
     </row>
     <row r="870">
-      <c r="A870" s="10"/>
+      <c r="A870" s="11"/>
     </row>
     <row r="871">
-      <c r="A871" s="10"/>
+      <c r="A871" s="11"/>
     </row>
     <row r="872">
-      <c r="A872" s="10"/>
+      <c r="A872" s="11"/>
     </row>
     <row r="873">
-      <c r="A873" s="10"/>
+      <c r="A873" s="11"/>
     </row>
     <row r="874">
-      <c r="A874" s="10"/>
+      <c r="A874" s="11"/>
     </row>
     <row r="875">
-      <c r="A875" s="10"/>
+      <c r="A875" s="11"/>
     </row>
     <row r="876">
-      <c r="A876" s="10"/>
+      <c r="A876" s="11"/>
     </row>
     <row r="877">
-      <c r="A877" s="10"/>
+      <c r="A877" s="11"/>
     </row>
     <row r="878">
-      <c r="A878" s="10"/>
+      <c r="A878" s="11"/>
     </row>
     <row r="879">
-      <c r="A879" s="10"/>
+      <c r="A879" s="11"/>
     </row>
     <row r="880">
-      <c r="A880" s="10"/>
+      <c r="A880" s="11"/>
     </row>
     <row r="881">
-      <c r="A881" s="10"/>
+      <c r="A881" s="11"/>
     </row>
     <row r="882">
-      <c r="A882" s="10"/>
+      <c r="A882" s="11"/>
     </row>
     <row r="883">
-      <c r="A883" s="10"/>
+      <c r="A883" s="11"/>
     </row>
     <row r="884">
-      <c r="A884" s="10"/>
+      <c r="A884" s="11"/>
     </row>
     <row r="885">
-      <c r="A885" s="10"/>
+      <c r="A885" s="11"/>
     </row>
     <row r="886">
-      <c r="A886" s="10"/>
+      <c r="A886" s="11"/>
     </row>
     <row r="887">
-      <c r="A887" s="10"/>
+      <c r="A887" s="11"/>
     </row>
     <row r="888">
-      <c r="A888" s="10"/>
+      <c r="A888" s="11"/>
     </row>
     <row r="889">
-      <c r="A889" s="10"/>
+      <c r="A889" s="11"/>
     </row>
     <row r="890">
-      <c r="A890" s="10"/>
+      <c r="A890" s="11"/>
     </row>
     <row r="891">
-      <c r="A891" s="10"/>
+      <c r="A891" s="11"/>
     </row>
     <row r="892">
-      <c r="A892" s="10"/>
+      <c r="A892" s="11"/>
     </row>
     <row r="893">
-      <c r="A893" s="10"/>
+      <c r="A893" s="11"/>
     </row>
     <row r="894">
-      <c r="A894" s="10"/>
+      <c r="A894" s="11"/>
     </row>
     <row r="895">
-      <c r="A895" s="10"/>
+      <c r="A895" s="11"/>
     </row>
     <row r="896">
-      <c r="A896" s="10"/>
+      <c r="A896" s="11"/>
     </row>
     <row r="897">
-      <c r="A897" s="10"/>
+      <c r="A897" s="11"/>
     </row>
     <row r="898">
-      <c r="A898" s="10"/>
+      <c r="A898" s="11"/>
     </row>
     <row r="899">
-      <c r="A899" s="10"/>
+      <c r="A899" s="11"/>
     </row>
     <row r="900">
-      <c r="A900" s="10"/>
+      <c r="A900" s="11"/>
     </row>
     <row r="901">
-      <c r="A901" s="10"/>
+      <c r="A901" s="11"/>
     </row>
     <row r="902">
-      <c r="A902" s="10"/>
+      <c r="A902" s="11"/>
     </row>
     <row r="903">
-      <c r="A903" s="10"/>
+      <c r="A903" s="11"/>
     </row>
     <row r="904">
-      <c r="A904" s="10"/>
+      <c r="A904" s="11"/>
     </row>
     <row r="905">
-      <c r="A905" s="10"/>
+      <c r="A905" s="11"/>
     </row>
     <row r="906">
-      <c r="A906" s="10"/>
+      <c r="A906" s="11"/>
     </row>
     <row r="907">
-      <c r="A907" s="10"/>
+      <c r="A907" s="11"/>
     </row>
     <row r="908">
-      <c r="A908" s="10"/>
+      <c r="A908" s="11"/>
     </row>
     <row r="909">
-      <c r="A909" s="10"/>
+      <c r="A909" s="11"/>
     </row>
     <row r="910">
-      <c r="A910" s="10"/>
+      <c r="A910" s="11"/>
     </row>
     <row r="911">
-      <c r="A911" s="10"/>
+      <c r="A911" s="11"/>
     </row>
     <row r="912">
-      <c r="A912" s="10"/>
+      <c r="A912" s="11"/>
     </row>
     <row r="913">
-      <c r="A913" s="10"/>
+      <c r="A913" s="11"/>
     </row>
     <row r="914">
-      <c r="A914" s="10"/>
+      <c r="A914" s="11"/>
     </row>
     <row r="915">
-      <c r="A915" s="10"/>
+      <c r="A915" s="11"/>
     </row>
     <row r="916">
-      <c r="A916" s="10"/>
+      <c r="A916" s="11"/>
     </row>
     <row r="917">
-      <c r="A917" s="10"/>
+      <c r="A917" s="11"/>
     </row>
     <row r="918">
-      <c r="A918" s="10"/>
+      <c r="A918" s="11"/>
     </row>
     <row r="919">
-      <c r="A919" s="10"/>
+      <c r="A919" s="11"/>
     </row>
     <row r="920">
-      <c r="A920" s="10"/>
+      <c r="A920" s="11"/>
     </row>
     <row r="921">
-      <c r="A921" s="10"/>
+      <c r="A921" s="11"/>
     </row>
     <row r="922">
-      <c r="A922" s="10"/>
+      <c r="A922" s="11"/>
     </row>
     <row r="923">
-      <c r="A923" s="10"/>
+      <c r="A923" s="11"/>
     </row>
     <row r="924">
-      <c r="A924" s="10"/>
+      <c r="A924" s="11"/>
     </row>
     <row r="925">
-      <c r="A925" s="10"/>
+      <c r="A925" s="11"/>
     </row>
     <row r="926">
-      <c r="A926" s="10"/>
+      <c r="A926" s="11"/>
     </row>
     <row r="927">
-      <c r="A927" s="10"/>
+      <c r="A927" s="11"/>
     </row>
     <row r="928">
-      <c r="A928" s="10"/>
+      <c r="A928" s="11"/>
     </row>
     <row r="929">
-      <c r="A929" s="10"/>
+      <c r="A929" s="11"/>
     </row>
     <row r="930">
-      <c r="A930" s="10"/>
+      <c r="A930" s="11"/>
     </row>
     <row r="931">
-      <c r="A931" s="10"/>
+      <c r="A931" s="11"/>
     </row>
     <row r="932">
-      <c r="A932" s="10"/>
+      <c r="A932" s="11"/>
     </row>
     <row r="933">
-      <c r="A933" s="10"/>
+      <c r="A933" s="11"/>
     </row>
     <row r="934">
-      <c r="A934" s="10"/>
+      <c r="A934" s="11"/>
     </row>
     <row r="935">
-      <c r="A935" s="10"/>
+      <c r="A935" s="11"/>
     </row>
     <row r="936">
-      <c r="A936" s="10"/>
+      <c r="A936" s="11"/>
     </row>
     <row r="937">
-      <c r="A937" s="10"/>
+      <c r="A937" s="11"/>
     </row>
     <row r="938">
-      <c r="A938" s="10"/>
+      <c r="A938" s="11"/>
     </row>
     <row r="939">
-      <c r="A939" s="10"/>
+      <c r="A939" s="11"/>
     </row>
     <row r="940">
-      <c r="A940" s="10"/>
+      <c r="A940" s="11"/>
     </row>
     <row r="941">
-      <c r="A941" s="10"/>
+      <c r="A941" s="11"/>
     </row>
     <row r="942">
-      <c r="A942" s="10"/>
+      <c r="A942" s="11"/>
     </row>
     <row r="943">
-      <c r="A943" s="10"/>
+      <c r="A943" s="11"/>
     </row>
     <row r="944">
-      <c r="A944" s="10"/>
+      <c r="A944" s="11"/>
     </row>
     <row r="945">
-      <c r="A945" s="10"/>
+      <c r="A945" s="11"/>
     </row>
     <row r="946">
-      <c r="A946" s="10"/>
+      <c r="A946" s="11"/>
     </row>
     <row r="947">
-      <c r="A947" s="10"/>
+      <c r="A947" s="11"/>
     </row>
     <row r="948">
-      <c r="A948" s="10"/>
+      <c r="A948" s="11"/>
     </row>
     <row r="949">
-      <c r="A949" s="10"/>
+      <c r="A949" s="11"/>
     </row>
     <row r="950">
-      <c r="A950" s="10"/>
+      <c r="A950" s="11"/>
     </row>
     <row r="951">
-      <c r="A951" s="10"/>
+      <c r="A951" s="11"/>
     </row>
     <row r="952">
-      <c r="A952" s="10"/>
+      <c r="A952" s="11"/>
     </row>
     <row r="953">
-      <c r="A953" s="10"/>
+      <c r="A953" s="11"/>
     </row>
     <row r="954">
-      <c r="A954" s="10"/>
+      <c r="A954" s="11"/>
     </row>
     <row r="955">
-      <c r="A955" s="10"/>
+      <c r="A955" s="11"/>
     </row>
     <row r="956">
-      <c r="A956" s="10"/>
+      <c r="A956" s="11"/>
     </row>
     <row r="957">
-      <c r="A957" s="10"/>
+      <c r="A957" s="11"/>
     </row>
     <row r="958">
-      <c r="A958" s="10"/>
+      <c r="A958" s="11"/>
     </row>
     <row r="959">
-      <c r="A959" s="10"/>
+      <c r="A959" s="11"/>
     </row>
     <row r="960">
-      <c r="A960" s="10"/>
+      <c r="A960" s="11"/>
     </row>
     <row r="961">
-      <c r="A961" s="10"/>
+      <c r="A961" s="11"/>
     </row>
     <row r="962">
-      <c r="A962" s="10"/>
+      <c r="A962" s="11"/>
     </row>
     <row r="963">
-      <c r="A963" s="10"/>
+      <c r="A963" s="11"/>
     </row>
     <row r="964">
-      <c r="A964" s="10"/>
+      <c r="A964" s="11"/>
     </row>
     <row r="965">
-      <c r="A965" s="10"/>
+      <c r="A965" s="11"/>
     </row>
     <row r="966">
-      <c r="A966" s="10"/>
+      <c r="A966" s="11"/>
     </row>
     <row r="967">
-      <c r="A967" s="10"/>
+      <c r="A967" s="11"/>
     </row>
     <row r="968">
-      <c r="A968" s="10"/>
+      <c r="A968" s="11"/>
     </row>
     <row r="969">
-      <c r="A969" s="10"/>
+      <c r="A969" s="11"/>
     </row>
     <row r="970">
-      <c r="A970" s="10"/>
+      <c r="A970" s="11"/>
     </row>
     <row r="971">
-      <c r="A971" s="10"/>
+      <c r="A971" s="11"/>
     </row>
     <row r="972">
-      <c r="A972" s="10"/>
+      <c r="A972" s="11"/>
     </row>
     <row r="973">
-      <c r="A973" s="10"/>
+      <c r="A973" s="11"/>
     </row>
     <row r="974">
-      <c r="A974" s="10"/>
+      <c r="A974" s="11"/>
     </row>
     <row r="975">
-      <c r="A975" s="10"/>
+      <c r="A975" s="11"/>
     </row>
     <row r="976">
-      <c r="A976" s="10"/>
+      <c r="A976" s="11"/>
     </row>
     <row r="977">
-      <c r="A977" s="10"/>
+      <c r="A977" s="11"/>
     </row>
     <row r="978">
-      <c r="A978" s="10"/>
+      <c r="A978" s="11"/>
     </row>
     <row r="979">
-      <c r="A979" s="10"/>
+      <c r="A979" s="11"/>
     </row>
     <row r="980">
-      <c r="A980" s="10"/>
+      <c r="A980" s="11"/>
     </row>
     <row r="981">
-      <c r="A981" s="10"/>
+      <c r="A981" s="11"/>
     </row>
     <row r="982">
-      <c r="A982" s="10"/>
+      <c r="A982" s="11"/>
     </row>
     <row r="983">
-      <c r="A983" s="10"/>
+      <c r="A983" s="11"/>
     </row>
     <row r="984">
-      <c r="A984" s="10"/>
+      <c r="A984" s="11"/>
     </row>
     <row r="985">
-      <c r="A985" s="10"/>
+      <c r="A985" s="11"/>
     </row>
     <row r="986">
-      <c r="A986" s="10"/>
+      <c r="A986" s="11"/>
     </row>
     <row r="987">
-      <c r="A987" s="10"/>
+      <c r="A987" s="11"/>
     </row>
     <row r="988">
-      <c r="A988" s="10"/>
+      <c r="A988" s="11"/>
     </row>
     <row r="989">
-      <c r="A989" s="10"/>
+      <c r="A989" s="11"/>
     </row>
     <row r="990">
-      <c r="A990" s="10"/>
+      <c r="A990" s="11"/>
     </row>
     <row r="991">
-      <c r="A991" s="10"/>
+      <c r="A991" s="11"/>
     </row>
     <row r="992">
-      <c r="A992" s="10"/>
+      <c r="A992" s="11"/>
     </row>
     <row r="993">
-      <c r="A993" s="10"/>
+      <c r="A993" s="11"/>
     </row>
     <row r="994">
-      <c r="A994" s="10"/>
+      <c r="A994" s="11"/>
     </row>
     <row r="995">
-      <c r="A995" s="10"/>
+      <c r="A995" s="11"/>
     </row>
     <row r="996">
-      <c r="A996" s="10"/>
+      <c r="A996" s="11"/>
     </row>
     <row r="997">
-      <c r="A997" s="10"/>
+      <c r="A997" s="11"/>
     </row>
     <row r="998">
-      <c r="A998" s="10"/>
+      <c r="A998" s="11"/>
     </row>
     <row r="999">
-      <c r="A999" s="10"/>
+      <c r="A999" s="11"/>
     </row>
     <row r="1000">
-      <c r="A1000" s="10"/>
+      <c r="A1000" s="11"/>
     </row>
     <row r="1001">
-      <c r="A1001" s="10"/>
+      <c r="A1001" s="11"/>
     </row>
     <row r="1002">
-      <c r="A1002" s="10"/>
+      <c r="A1002" s="11"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Transitions from end of playing state to feedback and from feedback to menu added.
</commit_message>
<xml_diff>
--- a/Unity/Assets/Resources/Localization/IT Alert UI Translation.xlsx
+++ b/Unity/Assets/Resources/Localization/IT Alert UI Translation.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="210">
   <si>
     <t>Key</t>
   </si>
@@ -632,6 +632,15 @@
   </si>
   <si>
     <t>XXXX</t>
+  </si>
+  <si>
+    <t>GAME_COMPLETION_BUTTON_CONTINUE</t>
+  </si>
+  <si>
+    <t>GAME_COMPLETION_LABEL_TEAM_SCORE</t>
+  </si>
+  <si>
+    <t>Team Score:</t>
   </si>
 </sst>
 </file>
@@ -1742,10 +1751,26 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="11"/>
+      <c r="A77" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="78">
-      <c r="A78" s="11"/>
+      <c r="A78" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="11"/>

</xml_diff>

<commit_message>
Further fixes for item drag and drop. Neutral end game screen added.
</commit_message>
<xml_diff>
--- a/Unity/Assets/Resources/Localization/IT Alert UI Translation.xlsx
+++ b/Unity/Assets/Resources/Localization/IT Alert UI Translation.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="212">
   <si>
     <t>Key</t>
   </si>
@@ -547,7 +547,7 @@
     <t>SETTINGS_LABEL_DISPLAY</t>
   </si>
   <si>
-    <t>DIsplay</t>
+    <t>Display</t>
   </si>
   <si>
     <t>Scherm</t>
@@ -631,7 +631,7 @@
     <t>Microphone Device</t>
   </si>
   <si>
-    <t>XXXX</t>
+    <t>Microfoon</t>
   </si>
   <si>
     <t>GAME_COMPLETION_BUTTON_CONTINUE</t>
@@ -641,6 +641,12 @@
   </si>
   <si>
     <t>Team Score:</t>
+  </si>
+  <si>
+    <t>GAME_COMPLETION_NEUTRAL</t>
+  </si>
+  <si>
+    <t>Game Over</t>
   </si>
 </sst>
 </file>
@@ -713,7 +719,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -745,6 +751,9 @@
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1769,2780 +1778,2788 @@
         <v>209</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="11"/>
+      <c r="A79" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="80">
-      <c r="A80" s="11"/>
+      <c r="A80" s="12"/>
     </row>
     <row r="81">
-      <c r="A81" s="11"/>
+      <c r="A81" s="12"/>
     </row>
     <row r="82">
-      <c r="A82" s="11"/>
+      <c r="A82" s="12"/>
     </row>
     <row r="83">
-      <c r="A83" s="11"/>
+      <c r="A83" s="12"/>
     </row>
     <row r="84">
-      <c r="A84" s="11"/>
+      <c r="A84" s="12"/>
     </row>
     <row r="85">
-      <c r="A85" s="11"/>
+      <c r="A85" s="12"/>
     </row>
     <row r="86">
-      <c r="A86" s="11"/>
+      <c r="A86" s="12"/>
     </row>
     <row r="87">
-      <c r="A87" s="11"/>
+      <c r="A87" s="12"/>
     </row>
     <row r="88">
-      <c r="A88" s="11"/>
+      <c r="A88" s="12"/>
     </row>
     <row r="89">
-      <c r="A89" s="11"/>
+      <c r="A89" s="12"/>
     </row>
     <row r="90">
-      <c r="A90" s="11"/>
+      <c r="A90" s="12"/>
     </row>
     <row r="91">
-      <c r="A91" s="11"/>
+      <c r="A91" s="12"/>
     </row>
     <row r="92">
-      <c r="A92" s="11"/>
+      <c r="A92" s="12"/>
     </row>
     <row r="93">
-      <c r="A93" s="11"/>
+      <c r="A93" s="12"/>
     </row>
     <row r="94">
-      <c r="A94" s="11"/>
+      <c r="A94" s="12"/>
     </row>
     <row r="95">
-      <c r="A95" s="11"/>
+      <c r="A95" s="12"/>
     </row>
     <row r="96">
-      <c r="A96" s="11"/>
+      <c r="A96" s="12"/>
     </row>
     <row r="97">
-      <c r="A97" s="11"/>
+      <c r="A97" s="12"/>
     </row>
     <row r="98">
-      <c r="A98" s="11"/>
+      <c r="A98" s="12"/>
     </row>
     <row r="99">
-      <c r="A99" s="11"/>
+      <c r="A99" s="12"/>
     </row>
     <row r="100">
-      <c r="A100" s="11"/>
+      <c r="A100" s="12"/>
     </row>
     <row r="101">
-      <c r="A101" s="11"/>
+      <c r="A101" s="12"/>
     </row>
     <row r="102">
-      <c r="A102" s="11"/>
+      <c r="A102" s="12"/>
     </row>
     <row r="103">
-      <c r="A103" s="11"/>
+      <c r="A103" s="12"/>
     </row>
     <row r="104">
-      <c r="A104" s="11"/>
+      <c r="A104" s="12"/>
     </row>
     <row r="105">
-      <c r="A105" s="11"/>
+      <c r="A105" s="12"/>
     </row>
     <row r="106">
-      <c r="A106" s="11"/>
+      <c r="A106" s="12"/>
     </row>
     <row r="107">
-      <c r="A107" s="11"/>
+      <c r="A107" s="12"/>
     </row>
     <row r="108">
-      <c r="A108" s="11"/>
+      <c r="A108" s="12"/>
     </row>
     <row r="109">
-      <c r="A109" s="11"/>
+      <c r="A109" s="12"/>
     </row>
     <row r="110">
-      <c r="A110" s="11"/>
+      <c r="A110" s="12"/>
     </row>
     <row r="111">
-      <c r="A111" s="11"/>
+      <c r="A111" s="12"/>
     </row>
     <row r="112">
-      <c r="A112" s="11"/>
+      <c r="A112" s="12"/>
     </row>
     <row r="113">
-      <c r="A113" s="11"/>
+      <c r="A113" s="12"/>
     </row>
     <row r="114">
-      <c r="A114" s="11"/>
+      <c r="A114" s="12"/>
     </row>
     <row r="115">
-      <c r="A115" s="11"/>
+      <c r="A115" s="12"/>
     </row>
     <row r="116">
-      <c r="A116" s="11"/>
+      <c r="A116" s="12"/>
     </row>
     <row r="117">
-      <c r="A117" s="11"/>
+      <c r="A117" s="12"/>
     </row>
     <row r="118">
-      <c r="A118" s="11"/>
+      <c r="A118" s="12"/>
     </row>
     <row r="119">
-      <c r="A119" s="11"/>
+      <c r="A119" s="12"/>
     </row>
     <row r="120">
-      <c r="A120" s="11"/>
+      <c r="A120" s="12"/>
     </row>
     <row r="121">
-      <c r="A121" s="11"/>
+      <c r="A121" s="12"/>
     </row>
     <row r="122">
-      <c r="A122" s="11"/>
+      <c r="A122" s="12"/>
     </row>
     <row r="123">
-      <c r="A123" s="11"/>
+      <c r="A123" s="12"/>
     </row>
     <row r="124">
-      <c r="A124" s="11"/>
+      <c r="A124" s="12"/>
     </row>
     <row r="125">
-      <c r="A125" s="11"/>
+      <c r="A125" s="12"/>
     </row>
     <row r="126">
-      <c r="A126" s="11"/>
+      <c r="A126" s="12"/>
     </row>
     <row r="127">
-      <c r="A127" s="11"/>
+      <c r="A127" s="12"/>
     </row>
     <row r="128">
-      <c r="A128" s="11"/>
+      <c r="A128" s="12"/>
     </row>
     <row r="129">
-      <c r="A129" s="11"/>
+      <c r="A129" s="12"/>
     </row>
     <row r="130">
-      <c r="A130" s="11"/>
+      <c r="A130" s="12"/>
     </row>
     <row r="131">
-      <c r="A131" s="11"/>
+      <c r="A131" s="12"/>
     </row>
     <row r="132">
-      <c r="A132" s="11"/>
+      <c r="A132" s="12"/>
     </row>
     <row r="133">
-      <c r="A133" s="11"/>
+      <c r="A133" s="12"/>
     </row>
     <row r="134">
-      <c r="A134" s="11"/>
+      <c r="A134" s="12"/>
     </row>
     <row r="135">
-      <c r="A135" s="11"/>
+      <c r="A135" s="12"/>
     </row>
     <row r="136">
-      <c r="A136" s="11"/>
+      <c r="A136" s="12"/>
     </row>
     <row r="137">
-      <c r="A137" s="11"/>
+      <c r="A137" s="12"/>
     </row>
     <row r="138">
-      <c r="A138" s="11"/>
+      <c r="A138" s="12"/>
     </row>
     <row r="139">
-      <c r="A139" s="11"/>
+      <c r="A139" s="12"/>
     </row>
     <row r="140">
-      <c r="A140" s="11"/>
+      <c r="A140" s="12"/>
     </row>
     <row r="141">
-      <c r="A141" s="11"/>
+      <c r="A141" s="12"/>
     </row>
     <row r="142">
-      <c r="A142" s="11"/>
+      <c r="A142" s="12"/>
     </row>
     <row r="143">
-      <c r="A143" s="11"/>
+      <c r="A143" s="12"/>
     </row>
     <row r="144">
-      <c r="A144" s="11"/>
+      <c r="A144" s="12"/>
     </row>
     <row r="145">
-      <c r="A145" s="11"/>
+      <c r="A145" s="12"/>
     </row>
     <row r="146">
-      <c r="A146" s="11"/>
+      <c r="A146" s="12"/>
     </row>
     <row r="147">
-      <c r="A147" s="11"/>
+      <c r="A147" s="12"/>
     </row>
     <row r="148">
-      <c r="A148" s="11"/>
+      <c r="A148" s="12"/>
     </row>
     <row r="149">
-      <c r="A149" s="11"/>
+      <c r="A149" s="12"/>
     </row>
     <row r="150">
-      <c r="A150" s="11"/>
+      <c r="A150" s="12"/>
     </row>
     <row r="151">
-      <c r="A151" s="11"/>
+      <c r="A151" s="12"/>
     </row>
     <row r="152">
-      <c r="A152" s="11"/>
+      <c r="A152" s="12"/>
     </row>
     <row r="153">
-      <c r="A153" s="11"/>
+      <c r="A153" s="12"/>
     </row>
     <row r="154">
-      <c r="A154" s="11"/>
+      <c r="A154" s="12"/>
     </row>
     <row r="155">
-      <c r="A155" s="11"/>
+      <c r="A155" s="12"/>
     </row>
     <row r="156">
-      <c r="A156" s="11"/>
+      <c r="A156" s="12"/>
     </row>
     <row r="157">
-      <c r="A157" s="11"/>
+      <c r="A157" s="12"/>
     </row>
     <row r="158">
-      <c r="A158" s="11"/>
+      <c r="A158" s="12"/>
     </row>
     <row r="159">
-      <c r="A159" s="11"/>
+      <c r="A159" s="12"/>
     </row>
     <row r="160">
-      <c r="A160" s="11"/>
+      <c r="A160" s="12"/>
     </row>
     <row r="161">
-      <c r="A161" s="11"/>
+      <c r="A161" s="12"/>
     </row>
     <row r="162">
-      <c r="A162" s="11"/>
+      <c r="A162" s="12"/>
     </row>
     <row r="163">
-      <c r="A163" s="11"/>
+      <c r="A163" s="12"/>
     </row>
     <row r="164">
-      <c r="A164" s="11"/>
+      <c r="A164" s="12"/>
     </row>
     <row r="165">
-      <c r="A165" s="11"/>
+      <c r="A165" s="12"/>
     </row>
     <row r="166">
-      <c r="A166" s="11"/>
+      <c r="A166" s="12"/>
     </row>
     <row r="167">
-      <c r="A167" s="11"/>
+      <c r="A167" s="12"/>
     </row>
     <row r="168">
-      <c r="A168" s="11"/>
+      <c r="A168" s="12"/>
     </row>
     <row r="169">
-      <c r="A169" s="11"/>
+      <c r="A169" s="12"/>
     </row>
     <row r="170">
-      <c r="A170" s="11"/>
+      <c r="A170" s="12"/>
     </row>
     <row r="171">
-      <c r="A171" s="11"/>
+      <c r="A171" s="12"/>
     </row>
     <row r="172">
-      <c r="A172" s="11"/>
+      <c r="A172" s="12"/>
     </row>
     <row r="173">
-      <c r="A173" s="11"/>
+      <c r="A173" s="12"/>
     </row>
     <row r="174">
-      <c r="A174" s="11"/>
+      <c r="A174" s="12"/>
     </row>
     <row r="175">
-      <c r="A175" s="11"/>
+      <c r="A175" s="12"/>
     </row>
     <row r="176">
-      <c r="A176" s="11"/>
+      <c r="A176" s="12"/>
     </row>
     <row r="177">
-      <c r="A177" s="11"/>
+      <c r="A177" s="12"/>
     </row>
     <row r="178">
-      <c r="A178" s="11"/>
+      <c r="A178" s="12"/>
     </row>
     <row r="179">
-      <c r="A179" s="11"/>
+      <c r="A179" s="12"/>
     </row>
     <row r="180">
-      <c r="A180" s="11"/>
+      <c r="A180" s="12"/>
     </row>
     <row r="181">
-      <c r="A181" s="11"/>
+      <c r="A181" s="12"/>
     </row>
     <row r="182">
-      <c r="A182" s="11"/>
+      <c r="A182" s="12"/>
     </row>
     <row r="183">
-      <c r="A183" s="11"/>
+      <c r="A183" s="12"/>
     </row>
     <row r="184">
-      <c r="A184" s="11"/>
+      <c r="A184" s="12"/>
     </row>
     <row r="185">
-      <c r="A185" s="11"/>
+      <c r="A185" s="12"/>
     </row>
     <row r="186">
-      <c r="A186" s="11"/>
+      <c r="A186" s="12"/>
     </row>
     <row r="187">
-      <c r="A187" s="11"/>
+      <c r="A187" s="12"/>
     </row>
     <row r="188">
-      <c r="A188" s="11"/>
+      <c r="A188" s="12"/>
     </row>
     <row r="189">
-      <c r="A189" s="11"/>
+      <c r="A189" s="12"/>
     </row>
     <row r="190">
-      <c r="A190" s="11"/>
+      <c r="A190" s="12"/>
     </row>
     <row r="191">
-      <c r="A191" s="11"/>
+      <c r="A191" s="12"/>
     </row>
     <row r="192">
-      <c r="A192" s="11"/>
+      <c r="A192" s="12"/>
     </row>
     <row r="193">
-      <c r="A193" s="11"/>
+      <c r="A193" s="12"/>
     </row>
     <row r="194">
-      <c r="A194" s="11"/>
+      <c r="A194" s="12"/>
     </row>
     <row r="195">
-      <c r="A195" s="11"/>
+      <c r="A195" s="12"/>
     </row>
     <row r="196">
-      <c r="A196" s="11"/>
+      <c r="A196" s="12"/>
     </row>
     <row r="197">
-      <c r="A197" s="11"/>
+      <c r="A197" s="12"/>
     </row>
     <row r="198">
-      <c r="A198" s="11"/>
+      <c r="A198" s="12"/>
     </row>
     <row r="199">
-      <c r="A199" s="11"/>
+      <c r="A199" s="12"/>
     </row>
     <row r="200">
-      <c r="A200" s="11"/>
+      <c r="A200" s="12"/>
     </row>
     <row r="201">
-      <c r="A201" s="11"/>
+      <c r="A201" s="12"/>
     </row>
     <row r="202">
-      <c r="A202" s="11"/>
+      <c r="A202" s="12"/>
     </row>
     <row r="203">
-      <c r="A203" s="11"/>
+      <c r="A203" s="12"/>
     </row>
     <row r="204">
-      <c r="A204" s="11"/>
+      <c r="A204" s="12"/>
     </row>
     <row r="205">
-      <c r="A205" s="11"/>
+      <c r="A205" s="12"/>
     </row>
     <row r="206">
-      <c r="A206" s="11"/>
+      <c r="A206" s="12"/>
     </row>
     <row r="207">
-      <c r="A207" s="11"/>
+      <c r="A207" s="12"/>
     </row>
     <row r="208">
-      <c r="A208" s="11"/>
+      <c r="A208" s="12"/>
     </row>
     <row r="209">
-      <c r="A209" s="11"/>
+      <c r="A209" s="12"/>
     </row>
     <row r="210">
-      <c r="A210" s="11"/>
+      <c r="A210" s="12"/>
     </row>
     <row r="211">
-      <c r="A211" s="11"/>
+      <c r="A211" s="12"/>
     </row>
     <row r="212">
-      <c r="A212" s="11"/>
+      <c r="A212" s="12"/>
     </row>
     <row r="213">
-      <c r="A213" s="11"/>
+      <c r="A213" s="12"/>
     </row>
     <row r="214">
-      <c r="A214" s="11"/>
+      <c r="A214" s="12"/>
     </row>
     <row r="215">
-      <c r="A215" s="11"/>
+      <c r="A215" s="12"/>
     </row>
     <row r="216">
-      <c r="A216" s="11"/>
+      <c r="A216" s="12"/>
     </row>
     <row r="217">
-      <c r="A217" s="11"/>
+      <c r="A217" s="12"/>
     </row>
     <row r="218">
-      <c r="A218" s="11"/>
+      <c r="A218" s="12"/>
     </row>
     <row r="219">
-      <c r="A219" s="11"/>
+      <c r="A219" s="12"/>
     </row>
     <row r="220">
-      <c r="A220" s="11"/>
+      <c r="A220" s="12"/>
     </row>
     <row r="221">
-      <c r="A221" s="11"/>
+      <c r="A221" s="12"/>
     </row>
     <row r="222">
-      <c r="A222" s="11"/>
+      <c r="A222" s="12"/>
     </row>
     <row r="223">
-      <c r="A223" s="11"/>
+      <c r="A223" s="12"/>
     </row>
     <row r="224">
-      <c r="A224" s="11"/>
+      <c r="A224" s="12"/>
     </row>
     <row r="225">
-      <c r="A225" s="11"/>
+      <c r="A225" s="12"/>
     </row>
     <row r="226">
-      <c r="A226" s="11"/>
+      <c r="A226" s="12"/>
     </row>
     <row r="227">
-      <c r="A227" s="11"/>
+      <c r="A227" s="12"/>
     </row>
     <row r="228">
-      <c r="A228" s="11"/>
+      <c r="A228" s="12"/>
     </row>
     <row r="229">
-      <c r="A229" s="11"/>
+      <c r="A229" s="12"/>
     </row>
     <row r="230">
-      <c r="A230" s="11"/>
+      <c r="A230" s="12"/>
     </row>
     <row r="231">
-      <c r="A231" s="11"/>
+      <c r="A231" s="12"/>
     </row>
     <row r="232">
-      <c r="A232" s="11"/>
+      <c r="A232" s="12"/>
     </row>
     <row r="233">
-      <c r="A233" s="11"/>
+      <c r="A233" s="12"/>
     </row>
     <row r="234">
-      <c r="A234" s="11"/>
+      <c r="A234" s="12"/>
     </row>
     <row r="235">
-      <c r="A235" s="11"/>
+      <c r="A235" s="12"/>
     </row>
     <row r="236">
-      <c r="A236" s="11"/>
+      <c r="A236" s="12"/>
     </row>
     <row r="237">
-      <c r="A237" s="11"/>
+      <c r="A237" s="12"/>
     </row>
     <row r="238">
-      <c r="A238" s="11"/>
+      <c r="A238" s="12"/>
     </row>
     <row r="239">
-      <c r="A239" s="11"/>
+      <c r="A239" s="12"/>
     </row>
     <row r="240">
-      <c r="A240" s="11"/>
+      <c r="A240" s="12"/>
     </row>
     <row r="241">
-      <c r="A241" s="11"/>
+      <c r="A241" s="12"/>
     </row>
     <row r="242">
-      <c r="A242" s="11"/>
+      <c r="A242" s="12"/>
     </row>
     <row r="243">
-      <c r="A243" s="11"/>
+      <c r="A243" s="12"/>
     </row>
     <row r="244">
-      <c r="A244" s="11"/>
+      <c r="A244" s="12"/>
     </row>
     <row r="245">
-      <c r="A245" s="11"/>
+      <c r="A245" s="12"/>
     </row>
     <row r="246">
-      <c r="A246" s="11"/>
+      <c r="A246" s="12"/>
     </row>
     <row r="247">
-      <c r="A247" s="11"/>
+      <c r="A247" s="12"/>
     </row>
     <row r="248">
-      <c r="A248" s="11"/>
+      <c r="A248" s="12"/>
     </row>
     <row r="249">
-      <c r="A249" s="11"/>
+      <c r="A249" s="12"/>
     </row>
     <row r="250">
-      <c r="A250" s="11"/>
+      <c r="A250" s="12"/>
     </row>
     <row r="251">
-      <c r="A251" s="11"/>
+      <c r="A251" s="12"/>
     </row>
     <row r="252">
-      <c r="A252" s="11"/>
+      <c r="A252" s="12"/>
     </row>
     <row r="253">
-      <c r="A253" s="11"/>
+      <c r="A253" s="12"/>
     </row>
     <row r="254">
-      <c r="A254" s="11"/>
+      <c r="A254" s="12"/>
     </row>
     <row r="255">
-      <c r="A255" s="11"/>
+      <c r="A255" s="12"/>
     </row>
     <row r="256">
-      <c r="A256" s="11"/>
+      <c r="A256" s="12"/>
     </row>
     <row r="257">
-      <c r="A257" s="11"/>
+      <c r="A257" s="12"/>
     </row>
     <row r="258">
-      <c r="A258" s="11"/>
+      <c r="A258" s="12"/>
     </row>
     <row r="259">
-      <c r="A259" s="11"/>
+      <c r="A259" s="12"/>
     </row>
     <row r="260">
-      <c r="A260" s="11"/>
+      <c r="A260" s="12"/>
     </row>
     <row r="261">
-      <c r="A261" s="11"/>
+      <c r="A261" s="12"/>
     </row>
     <row r="262">
-      <c r="A262" s="11"/>
+      <c r="A262" s="12"/>
     </row>
     <row r="263">
-      <c r="A263" s="11"/>
+      <c r="A263" s="12"/>
     </row>
     <row r="264">
-      <c r="A264" s="11"/>
+      <c r="A264" s="12"/>
     </row>
     <row r="265">
-      <c r="A265" s="11"/>
+      <c r="A265" s="12"/>
     </row>
     <row r="266">
-      <c r="A266" s="11"/>
+      <c r="A266" s="12"/>
     </row>
     <row r="267">
-      <c r="A267" s="11"/>
+      <c r="A267" s="12"/>
     </row>
     <row r="268">
-      <c r="A268" s="11"/>
+      <c r="A268" s="12"/>
     </row>
     <row r="269">
-      <c r="A269" s="11"/>
+      <c r="A269" s="12"/>
     </row>
     <row r="270">
-      <c r="A270" s="11"/>
+      <c r="A270" s="12"/>
     </row>
     <row r="271">
-      <c r="A271" s="11"/>
+      <c r="A271" s="12"/>
     </row>
     <row r="272">
-      <c r="A272" s="11"/>
+      <c r="A272" s="12"/>
     </row>
     <row r="273">
-      <c r="A273" s="11"/>
+      <c r="A273" s="12"/>
     </row>
     <row r="274">
-      <c r="A274" s="11"/>
+      <c r="A274" s="12"/>
     </row>
     <row r="275">
-      <c r="A275" s="11"/>
+      <c r="A275" s="12"/>
     </row>
     <row r="276">
-      <c r="A276" s="11"/>
+      <c r="A276" s="12"/>
     </row>
     <row r="277">
-      <c r="A277" s="11"/>
+      <c r="A277" s="12"/>
     </row>
     <row r="278">
-      <c r="A278" s="11"/>
+      <c r="A278" s="12"/>
     </row>
     <row r="279">
-      <c r="A279" s="11"/>
+      <c r="A279" s="12"/>
     </row>
     <row r="280">
-      <c r="A280" s="11"/>
+      <c r="A280" s="12"/>
     </row>
     <row r="281">
-      <c r="A281" s="11"/>
+      <c r="A281" s="12"/>
     </row>
     <row r="282">
-      <c r="A282" s="11"/>
+      <c r="A282" s="12"/>
     </row>
     <row r="283">
-      <c r="A283" s="11"/>
+      <c r="A283" s="12"/>
     </row>
     <row r="284">
-      <c r="A284" s="11"/>
+      <c r="A284" s="12"/>
     </row>
     <row r="285">
-      <c r="A285" s="11"/>
+      <c r="A285" s="12"/>
     </row>
     <row r="286">
-      <c r="A286" s="11"/>
+      <c r="A286" s="12"/>
     </row>
     <row r="287">
-      <c r="A287" s="11"/>
+      <c r="A287" s="12"/>
     </row>
     <row r="288">
-      <c r="A288" s="11"/>
+      <c r="A288" s="12"/>
     </row>
     <row r="289">
-      <c r="A289" s="11"/>
+      <c r="A289" s="12"/>
     </row>
     <row r="290">
-      <c r="A290" s="11"/>
+      <c r="A290" s="12"/>
     </row>
     <row r="291">
-      <c r="A291" s="11"/>
+      <c r="A291" s="12"/>
     </row>
     <row r="292">
-      <c r="A292" s="11"/>
+      <c r="A292" s="12"/>
     </row>
     <row r="293">
-      <c r="A293" s="11"/>
+      <c r="A293" s="12"/>
     </row>
     <row r="294">
-      <c r="A294" s="11"/>
+      <c r="A294" s="12"/>
     </row>
     <row r="295">
-      <c r="A295" s="11"/>
+      <c r="A295" s="12"/>
     </row>
     <row r="296">
-      <c r="A296" s="11"/>
+      <c r="A296" s="12"/>
     </row>
     <row r="297">
-      <c r="A297" s="11"/>
+      <c r="A297" s="12"/>
     </row>
     <row r="298">
-      <c r="A298" s="11"/>
+      <c r="A298" s="12"/>
     </row>
     <row r="299">
-      <c r="A299" s="11"/>
+      <c r="A299" s="12"/>
     </row>
     <row r="300">
-      <c r="A300" s="11"/>
+      <c r="A300" s="12"/>
     </row>
     <row r="301">
-      <c r="A301" s="11"/>
+      <c r="A301" s="12"/>
     </row>
     <row r="302">
-      <c r="A302" s="11"/>
+      <c r="A302" s="12"/>
     </row>
     <row r="303">
-      <c r="A303" s="11"/>
+      <c r="A303" s="12"/>
     </row>
     <row r="304">
-      <c r="A304" s="11"/>
+      <c r="A304" s="12"/>
     </row>
     <row r="305">
-      <c r="A305" s="11"/>
+      <c r="A305" s="12"/>
     </row>
     <row r="306">
-      <c r="A306" s="11"/>
+      <c r="A306" s="12"/>
     </row>
     <row r="307">
-      <c r="A307" s="11"/>
+      <c r="A307" s="12"/>
     </row>
     <row r="308">
-      <c r="A308" s="11"/>
+      <c r="A308" s="12"/>
     </row>
     <row r="309">
-      <c r="A309" s="11"/>
+      <c r="A309" s="12"/>
     </row>
     <row r="310">
-      <c r="A310" s="11"/>
+      <c r="A310" s="12"/>
     </row>
     <row r="311">
-      <c r="A311" s="11"/>
+      <c r="A311" s="12"/>
     </row>
     <row r="312">
-      <c r="A312" s="11"/>
+      <c r="A312" s="12"/>
     </row>
     <row r="313">
-      <c r="A313" s="11"/>
+      <c r="A313" s="12"/>
     </row>
     <row r="314">
-      <c r="A314" s="11"/>
+      <c r="A314" s="12"/>
     </row>
     <row r="315">
-      <c r="A315" s="11"/>
+      <c r="A315" s="12"/>
     </row>
     <row r="316">
-      <c r="A316" s="11"/>
+      <c r="A316" s="12"/>
     </row>
     <row r="317">
-      <c r="A317" s="11"/>
+      <c r="A317" s="12"/>
     </row>
     <row r="318">
-      <c r="A318" s="11"/>
+      <c r="A318" s="12"/>
     </row>
     <row r="319">
-      <c r="A319" s="11"/>
+      <c r="A319" s="12"/>
     </row>
     <row r="320">
-      <c r="A320" s="11"/>
+      <c r="A320" s="12"/>
     </row>
     <row r="321">
-      <c r="A321" s="11"/>
+      <c r="A321" s="12"/>
     </row>
     <row r="322">
-      <c r="A322" s="11"/>
+      <c r="A322" s="12"/>
     </row>
     <row r="323">
-      <c r="A323" s="11"/>
+      <c r="A323" s="12"/>
     </row>
     <row r="324">
-      <c r="A324" s="11"/>
+      <c r="A324" s="12"/>
     </row>
     <row r="325">
-      <c r="A325" s="11"/>
+      <c r="A325" s="12"/>
     </row>
     <row r="326">
-      <c r="A326" s="11"/>
+      <c r="A326" s="12"/>
     </row>
     <row r="327">
-      <c r="A327" s="11"/>
+      <c r="A327" s="12"/>
     </row>
     <row r="328">
-      <c r="A328" s="11"/>
+      <c r="A328" s="12"/>
     </row>
     <row r="329">
-      <c r="A329" s="11"/>
+      <c r="A329" s="12"/>
     </row>
     <row r="330">
-      <c r="A330" s="11"/>
+      <c r="A330" s="12"/>
     </row>
     <row r="331">
-      <c r="A331" s="11"/>
+      <c r="A331" s="12"/>
     </row>
     <row r="332">
-      <c r="A332" s="11"/>
+      <c r="A332" s="12"/>
     </row>
     <row r="333">
-      <c r="A333" s="11"/>
+      <c r="A333" s="12"/>
     </row>
     <row r="334">
-      <c r="A334" s="11"/>
+      <c r="A334" s="12"/>
     </row>
     <row r="335">
-      <c r="A335" s="11"/>
+      <c r="A335" s="12"/>
     </row>
     <row r="336">
-      <c r="A336" s="11"/>
+      <c r="A336" s="12"/>
     </row>
     <row r="337">
-      <c r="A337" s="11"/>
+      <c r="A337" s="12"/>
     </row>
     <row r="338">
-      <c r="A338" s="11"/>
+      <c r="A338" s="12"/>
     </row>
     <row r="339">
-      <c r="A339" s="11"/>
+      <c r="A339" s="12"/>
     </row>
     <row r="340">
-      <c r="A340" s="11"/>
+      <c r="A340" s="12"/>
     </row>
     <row r="341">
-      <c r="A341" s="11"/>
+      <c r="A341" s="12"/>
     </row>
     <row r="342">
-      <c r="A342" s="11"/>
+      <c r="A342" s="12"/>
     </row>
     <row r="343">
-      <c r="A343" s="11"/>
+      <c r="A343" s="12"/>
     </row>
     <row r="344">
-      <c r="A344" s="11"/>
+      <c r="A344" s="12"/>
     </row>
     <row r="345">
-      <c r="A345" s="11"/>
+      <c r="A345" s="12"/>
     </row>
     <row r="346">
-      <c r="A346" s="11"/>
+      <c r="A346" s="12"/>
     </row>
     <row r="347">
-      <c r="A347" s="11"/>
+      <c r="A347" s="12"/>
     </row>
     <row r="348">
-      <c r="A348" s="11"/>
+      <c r="A348" s="12"/>
     </row>
     <row r="349">
-      <c r="A349" s="11"/>
+      <c r="A349" s="12"/>
     </row>
     <row r="350">
-      <c r="A350" s="11"/>
+      <c r="A350" s="12"/>
     </row>
     <row r="351">
-      <c r="A351" s="11"/>
+      <c r="A351" s="12"/>
     </row>
     <row r="352">
-      <c r="A352" s="11"/>
+      <c r="A352" s="12"/>
     </row>
     <row r="353">
-      <c r="A353" s="11"/>
+      <c r="A353" s="12"/>
     </row>
     <row r="354">
-      <c r="A354" s="11"/>
+      <c r="A354" s="12"/>
     </row>
     <row r="355">
-      <c r="A355" s="11"/>
+      <c r="A355" s="12"/>
     </row>
     <row r="356">
-      <c r="A356" s="11"/>
+      <c r="A356" s="12"/>
     </row>
     <row r="357">
-      <c r="A357" s="11"/>
+      <c r="A357" s="12"/>
     </row>
     <row r="358">
-      <c r="A358" s="11"/>
+      <c r="A358" s="12"/>
     </row>
     <row r="359">
-      <c r="A359" s="11"/>
+      <c r="A359" s="12"/>
     </row>
     <row r="360">
-      <c r="A360" s="11"/>
+      <c r="A360" s="12"/>
     </row>
     <row r="361">
-      <c r="A361" s="11"/>
+      <c r="A361" s="12"/>
     </row>
     <row r="362">
-      <c r="A362" s="11"/>
+      <c r="A362" s="12"/>
     </row>
     <row r="363">
-      <c r="A363" s="11"/>
+      <c r="A363" s="12"/>
     </row>
     <row r="364">
-      <c r="A364" s="11"/>
+      <c r="A364" s="12"/>
     </row>
     <row r="365">
-      <c r="A365" s="11"/>
+      <c r="A365" s="12"/>
     </row>
     <row r="366">
-      <c r="A366" s="11"/>
+      <c r="A366" s="12"/>
     </row>
     <row r="367">
-      <c r="A367" s="11"/>
+      <c r="A367" s="12"/>
     </row>
     <row r="368">
-      <c r="A368" s="11"/>
+      <c r="A368" s="12"/>
     </row>
     <row r="369">
-      <c r="A369" s="11"/>
+      <c r="A369" s="12"/>
     </row>
     <row r="370">
-      <c r="A370" s="11"/>
+      <c r="A370" s="12"/>
     </row>
     <row r="371">
-      <c r="A371" s="11"/>
+      <c r="A371" s="12"/>
     </row>
     <row r="372">
-      <c r="A372" s="11"/>
+      <c r="A372" s="12"/>
     </row>
     <row r="373">
-      <c r="A373" s="11"/>
+      <c r="A373" s="12"/>
     </row>
     <row r="374">
-      <c r="A374" s="11"/>
+      <c r="A374" s="12"/>
     </row>
     <row r="375">
-      <c r="A375" s="11"/>
+      <c r="A375" s="12"/>
     </row>
     <row r="376">
-      <c r="A376" s="11"/>
+      <c r="A376" s="12"/>
     </row>
     <row r="377">
-      <c r="A377" s="11"/>
+      <c r="A377" s="12"/>
     </row>
     <row r="378">
-      <c r="A378" s="11"/>
+      <c r="A378" s="12"/>
     </row>
     <row r="379">
-      <c r="A379" s="11"/>
+      <c r="A379" s="12"/>
     </row>
     <row r="380">
-      <c r="A380" s="11"/>
+      <c r="A380" s="12"/>
     </row>
     <row r="381">
-      <c r="A381" s="11"/>
+      <c r="A381" s="12"/>
     </row>
     <row r="382">
-      <c r="A382" s="11"/>
+      <c r="A382" s="12"/>
     </row>
     <row r="383">
-      <c r="A383" s="11"/>
+      <c r="A383" s="12"/>
     </row>
     <row r="384">
-      <c r="A384" s="11"/>
+      <c r="A384" s="12"/>
     </row>
     <row r="385">
-      <c r="A385" s="11"/>
+      <c r="A385" s="12"/>
     </row>
     <row r="386">
-      <c r="A386" s="11"/>
+      <c r="A386" s="12"/>
     </row>
     <row r="387">
-      <c r="A387" s="11"/>
+      <c r="A387" s="12"/>
     </row>
     <row r="388">
-      <c r="A388" s="11"/>
+      <c r="A388" s="12"/>
     </row>
     <row r="389">
-      <c r="A389" s="11"/>
+      <c r="A389" s="12"/>
     </row>
     <row r="390">
-      <c r="A390" s="11"/>
+      <c r="A390" s="12"/>
     </row>
     <row r="391">
-      <c r="A391" s="11"/>
+      <c r="A391" s="12"/>
     </row>
     <row r="392">
-      <c r="A392" s="11"/>
+      <c r="A392" s="12"/>
     </row>
     <row r="393">
-      <c r="A393" s="11"/>
+      <c r="A393" s="12"/>
     </row>
     <row r="394">
-      <c r="A394" s="11"/>
+      <c r="A394" s="12"/>
     </row>
     <row r="395">
-      <c r="A395" s="11"/>
+      <c r="A395" s="12"/>
     </row>
     <row r="396">
-      <c r="A396" s="11"/>
+      <c r="A396" s="12"/>
     </row>
     <row r="397">
-      <c r="A397" s="11"/>
+      <c r="A397" s="12"/>
     </row>
     <row r="398">
-      <c r="A398" s="11"/>
+      <c r="A398" s="12"/>
     </row>
     <row r="399">
-      <c r="A399" s="11"/>
+      <c r="A399" s="12"/>
     </row>
     <row r="400">
-      <c r="A400" s="11"/>
+      <c r="A400" s="12"/>
     </row>
     <row r="401">
-      <c r="A401" s="11"/>
+      <c r="A401" s="12"/>
     </row>
     <row r="402">
-      <c r="A402" s="11"/>
+      <c r="A402" s="12"/>
     </row>
     <row r="403">
-      <c r="A403" s="11"/>
+      <c r="A403" s="12"/>
     </row>
     <row r="404">
-      <c r="A404" s="11"/>
+      <c r="A404" s="12"/>
     </row>
     <row r="405">
-      <c r="A405" s="11"/>
+      <c r="A405" s="12"/>
     </row>
     <row r="406">
-      <c r="A406" s="11"/>
+      <c r="A406" s="12"/>
     </row>
     <row r="407">
-      <c r="A407" s="11"/>
+      <c r="A407" s="12"/>
     </row>
     <row r="408">
-      <c r="A408" s="11"/>
+      <c r="A408" s="12"/>
     </row>
     <row r="409">
-      <c r="A409" s="11"/>
+      <c r="A409" s="12"/>
     </row>
     <row r="410">
-      <c r="A410" s="11"/>
+      <c r="A410" s="12"/>
     </row>
     <row r="411">
-      <c r="A411" s="11"/>
+      <c r="A411" s="12"/>
     </row>
     <row r="412">
-      <c r="A412" s="11"/>
+      <c r="A412" s="12"/>
     </row>
     <row r="413">
-      <c r="A413" s="11"/>
+      <c r="A413" s="12"/>
     </row>
     <row r="414">
-      <c r="A414" s="11"/>
+      <c r="A414" s="12"/>
     </row>
     <row r="415">
-      <c r="A415" s="11"/>
+      <c r="A415" s="12"/>
     </row>
     <row r="416">
-      <c r="A416" s="11"/>
+      <c r="A416" s="12"/>
     </row>
     <row r="417">
-      <c r="A417" s="11"/>
+      <c r="A417" s="12"/>
     </row>
     <row r="418">
-      <c r="A418" s="11"/>
+      <c r="A418" s="12"/>
     </row>
     <row r="419">
-      <c r="A419" s="11"/>
+      <c r="A419" s="12"/>
     </row>
     <row r="420">
-      <c r="A420" s="11"/>
+      <c r="A420" s="12"/>
     </row>
     <row r="421">
-      <c r="A421" s="11"/>
+      <c r="A421" s="12"/>
     </row>
     <row r="422">
-      <c r="A422" s="11"/>
+      <c r="A422" s="12"/>
     </row>
     <row r="423">
-      <c r="A423" s="11"/>
+      <c r="A423" s="12"/>
     </row>
     <row r="424">
-      <c r="A424" s="11"/>
+      <c r="A424" s="12"/>
     </row>
     <row r="425">
-      <c r="A425" s="11"/>
+      <c r="A425" s="12"/>
     </row>
     <row r="426">
-      <c r="A426" s="11"/>
+      <c r="A426" s="12"/>
     </row>
     <row r="427">
-      <c r="A427" s="11"/>
+      <c r="A427" s="12"/>
     </row>
     <row r="428">
-      <c r="A428" s="11"/>
+      <c r="A428" s="12"/>
     </row>
     <row r="429">
-      <c r="A429" s="11"/>
+      <c r="A429" s="12"/>
     </row>
     <row r="430">
-      <c r="A430" s="11"/>
+      <c r="A430" s="12"/>
     </row>
     <row r="431">
-      <c r="A431" s="11"/>
+      <c r="A431" s="12"/>
     </row>
     <row r="432">
-      <c r="A432" s="11"/>
+      <c r="A432" s="12"/>
     </row>
     <row r="433">
-      <c r="A433" s="11"/>
+      <c r="A433" s="12"/>
     </row>
     <row r="434">
-      <c r="A434" s="11"/>
+      <c r="A434" s="12"/>
     </row>
     <row r="435">
-      <c r="A435" s="11"/>
+      <c r="A435" s="12"/>
     </row>
     <row r="436">
-      <c r="A436" s="11"/>
+      <c r="A436" s="12"/>
     </row>
     <row r="437">
-      <c r="A437" s="11"/>
+      <c r="A437" s="12"/>
     </row>
     <row r="438">
-      <c r="A438" s="11"/>
+      <c r="A438" s="12"/>
     </row>
     <row r="439">
-      <c r="A439" s="11"/>
+      <c r="A439" s="12"/>
     </row>
     <row r="440">
-      <c r="A440" s="11"/>
+      <c r="A440" s="12"/>
     </row>
     <row r="441">
-      <c r="A441" s="11"/>
+      <c r="A441" s="12"/>
     </row>
     <row r="442">
-      <c r="A442" s="11"/>
+      <c r="A442" s="12"/>
     </row>
     <row r="443">
-      <c r="A443" s="11"/>
+      <c r="A443" s="12"/>
     </row>
     <row r="444">
-      <c r="A444" s="11"/>
+      <c r="A444" s="12"/>
     </row>
     <row r="445">
-      <c r="A445" s="11"/>
+      <c r="A445" s="12"/>
     </row>
     <row r="446">
-      <c r="A446" s="11"/>
+      <c r="A446" s="12"/>
     </row>
     <row r="447">
-      <c r="A447" s="11"/>
+      <c r="A447" s="12"/>
     </row>
     <row r="448">
-      <c r="A448" s="11"/>
+      <c r="A448" s="12"/>
     </row>
     <row r="449">
-      <c r="A449" s="11"/>
+      <c r="A449" s="12"/>
     </row>
     <row r="450">
-      <c r="A450" s="11"/>
+      <c r="A450" s="12"/>
     </row>
     <row r="451">
-      <c r="A451" s="11"/>
+      <c r="A451" s="12"/>
     </row>
     <row r="452">
-      <c r="A452" s="11"/>
+      <c r="A452" s="12"/>
     </row>
     <row r="453">
-      <c r="A453" s="11"/>
+      <c r="A453" s="12"/>
     </row>
     <row r="454">
-      <c r="A454" s="11"/>
+      <c r="A454" s="12"/>
     </row>
     <row r="455">
-      <c r="A455" s="11"/>
+      <c r="A455" s="12"/>
     </row>
     <row r="456">
-      <c r="A456" s="11"/>
+      <c r="A456" s="12"/>
     </row>
     <row r="457">
-      <c r="A457" s="11"/>
+      <c r="A457" s="12"/>
     </row>
     <row r="458">
-      <c r="A458" s="11"/>
+      <c r="A458" s="12"/>
     </row>
     <row r="459">
-      <c r="A459" s="11"/>
+      <c r="A459" s="12"/>
     </row>
     <row r="460">
-      <c r="A460" s="11"/>
+      <c r="A460" s="12"/>
     </row>
     <row r="461">
-      <c r="A461" s="11"/>
+      <c r="A461" s="12"/>
     </row>
     <row r="462">
-      <c r="A462" s="11"/>
+      <c r="A462" s="12"/>
     </row>
     <row r="463">
-      <c r="A463" s="11"/>
+      <c r="A463" s="12"/>
     </row>
     <row r="464">
-      <c r="A464" s="11"/>
+      <c r="A464" s="12"/>
     </row>
     <row r="465">
-      <c r="A465" s="11"/>
+      <c r="A465" s="12"/>
     </row>
     <row r="466">
-      <c r="A466" s="11"/>
+      <c r="A466" s="12"/>
     </row>
     <row r="467">
-      <c r="A467" s="11"/>
+      <c r="A467" s="12"/>
     </row>
     <row r="468">
-      <c r="A468" s="11"/>
+      <c r="A468" s="12"/>
     </row>
     <row r="469">
-      <c r="A469" s="11"/>
+      <c r="A469" s="12"/>
     </row>
     <row r="470">
-      <c r="A470" s="11"/>
+      <c r="A470" s="12"/>
     </row>
     <row r="471">
-      <c r="A471" s="11"/>
+      <c r="A471" s="12"/>
     </row>
     <row r="472">
-      <c r="A472" s="11"/>
+      <c r="A472" s="12"/>
     </row>
     <row r="473">
-      <c r="A473" s="11"/>
+      <c r="A473" s="12"/>
     </row>
     <row r="474">
-      <c r="A474" s="11"/>
+      <c r="A474" s="12"/>
     </row>
     <row r="475">
-      <c r="A475" s="11"/>
+      <c r="A475" s="12"/>
     </row>
     <row r="476">
-      <c r="A476" s="11"/>
+      <c r="A476" s="12"/>
     </row>
     <row r="477">
-      <c r="A477" s="11"/>
+      <c r="A477" s="12"/>
     </row>
     <row r="478">
-      <c r="A478" s="11"/>
+      <c r="A478" s="12"/>
     </row>
     <row r="479">
-      <c r="A479" s="11"/>
+      <c r="A479" s="12"/>
     </row>
     <row r="480">
-      <c r="A480" s="11"/>
+      <c r="A480" s="12"/>
     </row>
     <row r="481">
-      <c r="A481" s="11"/>
+      <c r="A481" s="12"/>
     </row>
     <row r="482">
-      <c r="A482" s="11"/>
+      <c r="A482" s="12"/>
     </row>
     <row r="483">
-      <c r="A483" s="11"/>
+      <c r="A483" s="12"/>
     </row>
     <row r="484">
-      <c r="A484" s="11"/>
+      <c r="A484" s="12"/>
     </row>
     <row r="485">
-      <c r="A485" s="11"/>
+      <c r="A485" s="12"/>
     </row>
     <row r="486">
-      <c r="A486" s="11"/>
+      <c r="A486" s="12"/>
     </row>
     <row r="487">
-      <c r="A487" s="11"/>
+      <c r="A487" s="12"/>
     </row>
     <row r="488">
-      <c r="A488" s="11"/>
+      <c r="A488" s="12"/>
     </row>
     <row r="489">
-      <c r="A489" s="11"/>
+      <c r="A489" s="12"/>
     </row>
     <row r="490">
-      <c r="A490" s="11"/>
+      <c r="A490" s="12"/>
     </row>
     <row r="491">
-      <c r="A491" s="11"/>
+      <c r="A491" s="12"/>
     </row>
     <row r="492">
-      <c r="A492" s="11"/>
+      <c r="A492" s="12"/>
     </row>
     <row r="493">
-      <c r="A493" s="11"/>
+      <c r="A493" s="12"/>
     </row>
     <row r="494">
-      <c r="A494" s="11"/>
+      <c r="A494" s="12"/>
     </row>
     <row r="495">
-      <c r="A495" s="11"/>
+      <c r="A495" s="12"/>
     </row>
     <row r="496">
-      <c r="A496" s="11"/>
+      <c r="A496" s="12"/>
     </row>
     <row r="497">
-      <c r="A497" s="11"/>
+      <c r="A497" s="12"/>
     </row>
     <row r="498">
-      <c r="A498" s="11"/>
+      <c r="A498" s="12"/>
     </row>
     <row r="499">
-      <c r="A499" s="11"/>
+      <c r="A499" s="12"/>
     </row>
     <row r="500">
-      <c r="A500" s="11"/>
+      <c r="A500" s="12"/>
     </row>
     <row r="501">
-      <c r="A501" s="11"/>
+      <c r="A501" s="12"/>
     </row>
     <row r="502">
-      <c r="A502" s="11"/>
+      <c r="A502" s="12"/>
     </row>
     <row r="503">
-      <c r="A503" s="11"/>
+      <c r="A503" s="12"/>
     </row>
     <row r="504">
-      <c r="A504" s="11"/>
+      <c r="A504" s="12"/>
     </row>
     <row r="505">
-      <c r="A505" s="11"/>
+      <c r="A505" s="12"/>
     </row>
     <row r="506">
-      <c r="A506" s="11"/>
+      <c r="A506" s="12"/>
     </row>
     <row r="507">
-      <c r="A507" s="11"/>
+      <c r="A507" s="12"/>
     </row>
     <row r="508">
-      <c r="A508" s="11"/>
+      <c r="A508" s="12"/>
     </row>
     <row r="509">
-      <c r="A509" s="11"/>
+      <c r="A509" s="12"/>
     </row>
     <row r="510">
-      <c r="A510" s="11"/>
+      <c r="A510" s="12"/>
     </row>
     <row r="511">
-      <c r="A511" s="11"/>
+      <c r="A511" s="12"/>
     </row>
     <row r="512">
-      <c r="A512" s="11"/>
+      <c r="A512" s="12"/>
     </row>
     <row r="513">
-      <c r="A513" s="11"/>
+      <c r="A513" s="12"/>
     </row>
     <row r="514">
-      <c r="A514" s="11"/>
+      <c r="A514" s="12"/>
     </row>
     <row r="515">
-      <c r="A515" s="11"/>
+      <c r="A515" s="12"/>
     </row>
     <row r="516">
-      <c r="A516" s="11"/>
+      <c r="A516" s="12"/>
     </row>
     <row r="517">
-      <c r="A517" s="11"/>
+      <c r="A517" s="12"/>
     </row>
     <row r="518">
-      <c r="A518" s="11"/>
+      <c r="A518" s="12"/>
     </row>
     <row r="519">
-      <c r="A519" s="11"/>
+      <c r="A519" s="12"/>
     </row>
     <row r="520">
-      <c r="A520" s="11"/>
+      <c r="A520" s="12"/>
     </row>
     <row r="521">
-      <c r="A521" s="11"/>
+      <c r="A521" s="12"/>
     </row>
     <row r="522">
-      <c r="A522" s="11"/>
+      <c r="A522" s="12"/>
     </row>
     <row r="523">
-      <c r="A523" s="11"/>
+      <c r="A523" s="12"/>
     </row>
     <row r="524">
-      <c r="A524" s="11"/>
+      <c r="A524" s="12"/>
     </row>
     <row r="525">
-      <c r="A525" s="11"/>
+      <c r="A525" s="12"/>
     </row>
     <row r="526">
-      <c r="A526" s="11"/>
+      <c r="A526" s="12"/>
     </row>
     <row r="527">
-      <c r="A527" s="11"/>
+      <c r="A527" s="12"/>
     </row>
     <row r="528">
-      <c r="A528" s="11"/>
+      <c r="A528" s="12"/>
     </row>
     <row r="529">
-      <c r="A529" s="11"/>
+      <c r="A529" s="12"/>
     </row>
     <row r="530">
-      <c r="A530" s="11"/>
+      <c r="A530" s="12"/>
     </row>
     <row r="531">
-      <c r="A531" s="11"/>
+      <c r="A531" s="12"/>
     </row>
     <row r="532">
-      <c r="A532" s="11"/>
+      <c r="A532" s="12"/>
     </row>
     <row r="533">
-      <c r="A533" s="11"/>
+      <c r="A533" s="12"/>
     </row>
     <row r="534">
-      <c r="A534" s="11"/>
+      <c r="A534" s="12"/>
     </row>
     <row r="535">
-      <c r="A535" s="11"/>
+      <c r="A535" s="12"/>
     </row>
     <row r="536">
-      <c r="A536" s="11"/>
+      <c r="A536" s="12"/>
     </row>
     <row r="537">
-      <c r="A537" s="11"/>
+      <c r="A537" s="12"/>
     </row>
     <row r="538">
-      <c r="A538" s="11"/>
+      <c r="A538" s="12"/>
     </row>
     <row r="539">
-      <c r="A539" s="11"/>
+      <c r="A539" s="12"/>
     </row>
     <row r="540">
-      <c r="A540" s="11"/>
+      <c r="A540" s="12"/>
     </row>
     <row r="541">
-      <c r="A541" s="11"/>
+      <c r="A541" s="12"/>
     </row>
     <row r="542">
-      <c r="A542" s="11"/>
+      <c r="A542" s="12"/>
     </row>
     <row r="543">
-      <c r="A543" s="11"/>
+      <c r="A543" s="12"/>
     </row>
     <row r="544">
-      <c r="A544" s="11"/>
+      <c r="A544" s="12"/>
     </row>
     <row r="545">
-      <c r="A545" s="11"/>
+      <c r="A545" s="12"/>
     </row>
     <row r="546">
-      <c r="A546" s="11"/>
+      <c r="A546" s="12"/>
     </row>
     <row r="547">
-      <c r="A547" s="11"/>
+      <c r="A547" s="12"/>
     </row>
     <row r="548">
-      <c r="A548" s="11"/>
+      <c r="A548" s="12"/>
     </row>
     <row r="549">
-      <c r="A549" s="11"/>
+      <c r="A549" s="12"/>
     </row>
     <row r="550">
-      <c r="A550" s="11"/>
+      <c r="A550" s="12"/>
     </row>
     <row r="551">
-      <c r="A551" s="11"/>
+      <c r="A551" s="12"/>
     </row>
     <row r="552">
-      <c r="A552" s="11"/>
+      <c r="A552" s="12"/>
     </row>
     <row r="553">
-      <c r="A553" s="11"/>
+      <c r="A553" s="12"/>
     </row>
     <row r="554">
-      <c r="A554" s="11"/>
+      <c r="A554" s="12"/>
     </row>
     <row r="555">
-      <c r="A555" s="11"/>
+      <c r="A555" s="12"/>
     </row>
     <row r="556">
-      <c r="A556" s="11"/>
+      <c r="A556" s="12"/>
     </row>
     <row r="557">
-      <c r="A557" s="11"/>
+      <c r="A557" s="12"/>
     </row>
     <row r="558">
-      <c r="A558" s="11"/>
+      <c r="A558" s="12"/>
     </row>
     <row r="559">
-      <c r="A559" s="11"/>
+      <c r="A559" s="12"/>
     </row>
     <row r="560">
-      <c r="A560" s="11"/>
+      <c r="A560" s="12"/>
     </row>
     <row r="561">
-      <c r="A561" s="11"/>
+      <c r="A561" s="12"/>
     </row>
     <row r="562">
-      <c r="A562" s="11"/>
+      <c r="A562" s="12"/>
     </row>
     <row r="563">
-      <c r="A563" s="11"/>
+      <c r="A563" s="12"/>
     </row>
     <row r="564">
-      <c r="A564" s="11"/>
+      <c r="A564" s="12"/>
     </row>
     <row r="565">
-      <c r="A565" s="11"/>
+      <c r="A565" s="12"/>
     </row>
     <row r="566">
-      <c r="A566" s="11"/>
+      <c r="A566" s="12"/>
     </row>
     <row r="567">
-      <c r="A567" s="11"/>
+      <c r="A567" s="12"/>
     </row>
     <row r="568">
-      <c r="A568" s="11"/>
+      <c r="A568" s="12"/>
     </row>
     <row r="569">
-      <c r="A569" s="11"/>
+      <c r="A569" s="12"/>
     </row>
     <row r="570">
-      <c r="A570" s="11"/>
+      <c r="A570" s="12"/>
     </row>
     <row r="571">
-      <c r="A571" s="11"/>
+      <c r="A571" s="12"/>
     </row>
     <row r="572">
-      <c r="A572" s="11"/>
+      <c r="A572" s="12"/>
     </row>
     <row r="573">
-      <c r="A573" s="11"/>
+      <c r="A573" s="12"/>
     </row>
     <row r="574">
-      <c r="A574" s="11"/>
+      <c r="A574" s="12"/>
     </row>
     <row r="575">
-      <c r="A575" s="11"/>
+      <c r="A575" s="12"/>
     </row>
     <row r="576">
-      <c r="A576" s="11"/>
+      <c r="A576" s="12"/>
     </row>
     <row r="577">
-      <c r="A577" s="11"/>
+      <c r="A577" s="12"/>
     </row>
     <row r="578">
-      <c r="A578" s="11"/>
+      <c r="A578" s="12"/>
     </row>
     <row r="579">
-      <c r="A579" s="11"/>
+      <c r="A579" s="12"/>
     </row>
     <row r="580">
-      <c r="A580" s="11"/>
+      <c r="A580" s="12"/>
     </row>
     <row r="581">
-      <c r="A581" s="11"/>
+      <c r="A581" s="12"/>
     </row>
     <row r="582">
-      <c r="A582" s="11"/>
+      <c r="A582" s="12"/>
     </row>
     <row r="583">
-      <c r="A583" s="11"/>
+      <c r="A583" s="12"/>
     </row>
     <row r="584">
-      <c r="A584" s="11"/>
+      <c r="A584" s="12"/>
     </row>
     <row r="585">
-      <c r="A585" s="11"/>
+      <c r="A585" s="12"/>
     </row>
     <row r="586">
-      <c r="A586" s="11"/>
+      <c r="A586" s="12"/>
     </row>
     <row r="587">
-      <c r="A587" s="11"/>
+      <c r="A587" s="12"/>
     </row>
     <row r="588">
-      <c r="A588" s="11"/>
+      <c r="A588" s="12"/>
     </row>
     <row r="589">
-      <c r="A589" s="11"/>
+      <c r="A589" s="12"/>
     </row>
     <row r="590">
-      <c r="A590" s="11"/>
+      <c r="A590" s="12"/>
     </row>
     <row r="591">
-      <c r="A591" s="11"/>
+      <c r="A591" s="12"/>
     </row>
     <row r="592">
-      <c r="A592" s="11"/>
+      <c r="A592" s="12"/>
     </row>
     <row r="593">
-      <c r="A593" s="11"/>
+      <c r="A593" s="12"/>
     </row>
     <row r="594">
-      <c r="A594" s="11"/>
+      <c r="A594" s="12"/>
     </row>
     <row r="595">
-      <c r="A595" s="11"/>
+      <c r="A595" s="12"/>
     </row>
     <row r="596">
-      <c r="A596" s="11"/>
+      <c r="A596" s="12"/>
     </row>
     <row r="597">
-      <c r="A597" s="11"/>
+      <c r="A597" s="12"/>
     </row>
     <row r="598">
-      <c r="A598" s="11"/>
+      <c r="A598" s="12"/>
     </row>
     <row r="599">
-      <c r="A599" s="11"/>
+      <c r="A599" s="12"/>
     </row>
     <row r="600">
-      <c r="A600" s="11"/>
+      <c r="A600" s="12"/>
     </row>
     <row r="601">
-      <c r="A601" s="11"/>
+      <c r="A601" s="12"/>
     </row>
     <row r="602">
-      <c r="A602" s="11"/>
+      <c r="A602" s="12"/>
     </row>
     <row r="603">
-      <c r="A603" s="11"/>
+      <c r="A603" s="12"/>
     </row>
     <row r="604">
-      <c r="A604" s="11"/>
+      <c r="A604" s="12"/>
     </row>
     <row r="605">
-      <c r="A605" s="11"/>
+      <c r="A605" s="12"/>
     </row>
     <row r="606">
-      <c r="A606" s="11"/>
+      <c r="A606" s="12"/>
     </row>
     <row r="607">
-      <c r="A607" s="11"/>
+      <c r="A607" s="12"/>
     </row>
     <row r="608">
-      <c r="A608" s="11"/>
+      <c r="A608" s="12"/>
     </row>
     <row r="609">
-      <c r="A609" s="11"/>
+      <c r="A609" s="12"/>
     </row>
     <row r="610">
-      <c r="A610" s="11"/>
+      <c r="A610" s="12"/>
     </row>
     <row r="611">
-      <c r="A611" s="11"/>
+      <c r="A611" s="12"/>
     </row>
     <row r="612">
-      <c r="A612" s="11"/>
+      <c r="A612" s="12"/>
     </row>
     <row r="613">
-      <c r="A613" s="11"/>
+      <c r="A613" s="12"/>
     </row>
     <row r="614">
-      <c r="A614" s="11"/>
+      <c r="A614" s="12"/>
     </row>
     <row r="615">
-      <c r="A615" s="11"/>
+      <c r="A615" s="12"/>
     </row>
     <row r="616">
-      <c r="A616" s="11"/>
+      <c r="A616" s="12"/>
     </row>
     <row r="617">
-      <c r="A617" s="11"/>
+      <c r="A617" s="12"/>
     </row>
     <row r="618">
-      <c r="A618" s="11"/>
+      <c r="A618" s="12"/>
     </row>
     <row r="619">
-      <c r="A619" s="11"/>
+      <c r="A619" s="12"/>
     </row>
     <row r="620">
-      <c r="A620" s="11"/>
+      <c r="A620" s="12"/>
     </row>
     <row r="621">
-      <c r="A621" s="11"/>
+      <c r="A621" s="12"/>
     </row>
     <row r="622">
-      <c r="A622" s="11"/>
+      <c r="A622" s="12"/>
     </row>
     <row r="623">
-      <c r="A623" s="11"/>
+      <c r="A623" s="12"/>
     </row>
     <row r="624">
-      <c r="A624" s="11"/>
+      <c r="A624" s="12"/>
     </row>
     <row r="625">
-      <c r="A625" s="11"/>
+      <c r="A625" s="12"/>
     </row>
     <row r="626">
-      <c r="A626" s="11"/>
+      <c r="A626" s="12"/>
     </row>
     <row r="627">
-      <c r="A627" s="11"/>
+      <c r="A627" s="12"/>
     </row>
     <row r="628">
-      <c r="A628" s="11"/>
+      <c r="A628" s="12"/>
     </row>
     <row r="629">
-      <c r="A629" s="11"/>
+      <c r="A629" s="12"/>
     </row>
     <row r="630">
-      <c r="A630" s="11"/>
+      <c r="A630" s="12"/>
     </row>
     <row r="631">
-      <c r="A631" s="11"/>
+      <c r="A631" s="12"/>
     </row>
     <row r="632">
-      <c r="A632" s="11"/>
+      <c r="A632" s="12"/>
     </row>
     <row r="633">
-      <c r="A633" s="11"/>
+      <c r="A633" s="12"/>
     </row>
     <row r="634">
-      <c r="A634" s="11"/>
+      <c r="A634" s="12"/>
     </row>
     <row r="635">
-      <c r="A635" s="11"/>
+      <c r="A635" s="12"/>
     </row>
     <row r="636">
-      <c r="A636" s="11"/>
+      <c r="A636" s="12"/>
     </row>
     <row r="637">
-      <c r="A637" s="11"/>
+      <c r="A637" s="12"/>
     </row>
     <row r="638">
-      <c r="A638" s="11"/>
+      <c r="A638" s="12"/>
     </row>
     <row r="639">
-      <c r="A639" s="11"/>
+      <c r="A639" s="12"/>
     </row>
     <row r="640">
-      <c r="A640" s="11"/>
+      <c r="A640" s="12"/>
     </row>
     <row r="641">
-      <c r="A641" s="11"/>
+      <c r="A641" s="12"/>
     </row>
     <row r="642">
-      <c r="A642" s="11"/>
+      <c r="A642" s="12"/>
     </row>
     <row r="643">
-      <c r="A643" s="11"/>
+      <c r="A643" s="12"/>
     </row>
     <row r="644">
-      <c r="A644" s="11"/>
+      <c r="A644" s="12"/>
     </row>
     <row r="645">
-      <c r="A645" s="11"/>
+      <c r="A645" s="12"/>
     </row>
     <row r="646">
-      <c r="A646" s="11"/>
+      <c r="A646" s="12"/>
     </row>
     <row r="647">
-      <c r="A647" s="11"/>
+      <c r="A647" s="12"/>
     </row>
     <row r="648">
-      <c r="A648" s="11"/>
+      <c r="A648" s="12"/>
     </row>
     <row r="649">
-      <c r="A649" s="11"/>
+      <c r="A649" s="12"/>
     </row>
     <row r="650">
-      <c r="A650" s="11"/>
+      <c r="A650" s="12"/>
     </row>
     <row r="651">
-      <c r="A651" s="11"/>
+      <c r="A651" s="12"/>
     </row>
     <row r="652">
-      <c r="A652" s="11"/>
+      <c r="A652" s="12"/>
     </row>
     <row r="653">
-      <c r="A653" s="11"/>
+      <c r="A653" s="12"/>
     </row>
     <row r="654">
-      <c r="A654" s="11"/>
+      <c r="A654" s="12"/>
     </row>
     <row r="655">
-      <c r="A655" s="11"/>
+      <c r="A655" s="12"/>
     </row>
     <row r="656">
-      <c r="A656" s="11"/>
+      <c r="A656" s="12"/>
     </row>
     <row r="657">
-      <c r="A657" s="11"/>
+      <c r="A657" s="12"/>
     </row>
     <row r="658">
-      <c r="A658" s="11"/>
+      <c r="A658" s="12"/>
     </row>
     <row r="659">
-      <c r="A659" s="11"/>
+      <c r="A659" s="12"/>
     </row>
     <row r="660">
-      <c r="A660" s="11"/>
+      <c r="A660" s="12"/>
     </row>
     <row r="661">
-      <c r="A661" s="11"/>
+      <c r="A661" s="12"/>
     </row>
     <row r="662">
-      <c r="A662" s="11"/>
+      <c r="A662" s="12"/>
     </row>
     <row r="663">
-      <c r="A663" s="11"/>
+      <c r="A663" s="12"/>
     </row>
     <row r="664">
-      <c r="A664" s="11"/>
+      <c r="A664" s="12"/>
     </row>
     <row r="665">
-      <c r="A665" s="11"/>
+      <c r="A665" s="12"/>
     </row>
     <row r="666">
-      <c r="A666" s="11"/>
+      <c r="A666" s="12"/>
     </row>
     <row r="667">
-      <c r="A667" s="11"/>
+      <c r="A667" s="12"/>
     </row>
     <row r="668">
-      <c r="A668" s="11"/>
+      <c r="A668" s="12"/>
     </row>
     <row r="669">
-      <c r="A669" s="11"/>
+      <c r="A669" s="12"/>
     </row>
     <row r="670">
-      <c r="A670" s="11"/>
+      <c r="A670" s="12"/>
     </row>
     <row r="671">
-      <c r="A671" s="11"/>
+      <c r="A671" s="12"/>
     </row>
     <row r="672">
-      <c r="A672" s="11"/>
+      <c r="A672" s="12"/>
     </row>
     <row r="673">
-      <c r="A673" s="11"/>
+      <c r="A673" s="12"/>
     </row>
     <row r="674">
-      <c r="A674" s="11"/>
+      <c r="A674" s="12"/>
     </row>
     <row r="675">
-      <c r="A675" s="11"/>
+      <c r="A675" s="12"/>
     </row>
     <row r="676">
-      <c r="A676" s="11"/>
+      <c r="A676" s="12"/>
     </row>
     <row r="677">
-      <c r="A677" s="11"/>
+      <c r="A677" s="12"/>
     </row>
     <row r="678">
-      <c r="A678" s="11"/>
+      <c r="A678" s="12"/>
     </row>
     <row r="679">
-      <c r="A679" s="11"/>
+      <c r="A679" s="12"/>
     </row>
     <row r="680">
-      <c r="A680" s="11"/>
+      <c r="A680" s="12"/>
     </row>
     <row r="681">
-      <c r="A681" s="11"/>
+      <c r="A681" s="12"/>
     </row>
     <row r="682">
-      <c r="A682" s="11"/>
+      <c r="A682" s="12"/>
     </row>
     <row r="683">
-      <c r="A683" s="11"/>
+      <c r="A683" s="12"/>
     </row>
     <row r="684">
-      <c r="A684" s="11"/>
+      <c r="A684" s="12"/>
     </row>
     <row r="685">
-      <c r="A685" s="11"/>
+      <c r="A685" s="12"/>
     </row>
     <row r="686">
-      <c r="A686" s="11"/>
+      <c r="A686" s="12"/>
     </row>
     <row r="687">
-      <c r="A687" s="11"/>
+      <c r="A687" s="12"/>
     </row>
     <row r="688">
-      <c r="A688" s="11"/>
+      <c r="A688" s="12"/>
     </row>
     <row r="689">
-      <c r="A689" s="11"/>
+      <c r="A689" s="12"/>
     </row>
     <row r="690">
-      <c r="A690" s="11"/>
+      <c r="A690" s="12"/>
     </row>
     <row r="691">
-      <c r="A691" s="11"/>
+      <c r="A691" s="12"/>
     </row>
     <row r="692">
-      <c r="A692" s="11"/>
+      <c r="A692" s="12"/>
     </row>
     <row r="693">
-      <c r="A693" s="11"/>
+      <c r="A693" s="12"/>
     </row>
     <row r="694">
-      <c r="A694" s="11"/>
+      <c r="A694" s="12"/>
     </row>
     <row r="695">
-      <c r="A695" s="11"/>
+      <c r="A695" s="12"/>
     </row>
     <row r="696">
-      <c r="A696" s="11"/>
+      <c r="A696" s="12"/>
     </row>
     <row r="697">
-      <c r="A697" s="11"/>
+      <c r="A697" s="12"/>
     </row>
     <row r="698">
-      <c r="A698" s="11"/>
+      <c r="A698" s="12"/>
     </row>
     <row r="699">
-      <c r="A699" s="11"/>
+      <c r="A699" s="12"/>
     </row>
     <row r="700">
-      <c r="A700" s="11"/>
+      <c r="A700" s="12"/>
     </row>
     <row r="701">
-      <c r="A701" s="11"/>
+      <c r="A701" s="12"/>
     </row>
     <row r="702">
-      <c r="A702" s="11"/>
+      <c r="A702" s="12"/>
     </row>
     <row r="703">
-      <c r="A703" s="11"/>
+      <c r="A703" s="12"/>
     </row>
     <row r="704">
-      <c r="A704" s="11"/>
+      <c r="A704" s="12"/>
     </row>
     <row r="705">
-      <c r="A705" s="11"/>
+      <c r="A705" s="12"/>
     </row>
     <row r="706">
-      <c r="A706" s="11"/>
+      <c r="A706" s="12"/>
     </row>
     <row r="707">
-      <c r="A707" s="11"/>
+      <c r="A707" s="12"/>
     </row>
     <row r="708">
-      <c r="A708" s="11"/>
+      <c r="A708" s="12"/>
     </row>
     <row r="709">
-      <c r="A709" s="11"/>
+      <c r="A709" s="12"/>
     </row>
     <row r="710">
-      <c r="A710" s="11"/>
+      <c r="A710" s="12"/>
     </row>
     <row r="711">
-      <c r="A711" s="11"/>
+      <c r="A711" s="12"/>
     </row>
     <row r="712">
-      <c r="A712" s="11"/>
+      <c r="A712" s="12"/>
     </row>
     <row r="713">
-      <c r="A713" s="11"/>
+      <c r="A713" s="12"/>
     </row>
     <row r="714">
-      <c r="A714" s="11"/>
+      <c r="A714" s="12"/>
     </row>
     <row r="715">
-      <c r="A715" s="11"/>
+      <c r="A715" s="12"/>
     </row>
     <row r="716">
-      <c r="A716" s="11"/>
+      <c r="A716" s="12"/>
     </row>
     <row r="717">
-      <c r="A717" s="11"/>
+      <c r="A717" s="12"/>
     </row>
     <row r="718">
-      <c r="A718" s="11"/>
+      <c r="A718" s="12"/>
     </row>
     <row r="719">
-      <c r="A719" s="11"/>
+      <c r="A719" s="12"/>
     </row>
     <row r="720">
-      <c r="A720" s="11"/>
+      <c r="A720" s="12"/>
     </row>
     <row r="721">
-      <c r="A721" s="11"/>
+      <c r="A721" s="12"/>
     </row>
     <row r="722">
-      <c r="A722" s="11"/>
+      <c r="A722" s="12"/>
     </row>
     <row r="723">
-      <c r="A723" s="11"/>
+      <c r="A723" s="12"/>
     </row>
     <row r="724">
-      <c r="A724" s="11"/>
+      <c r="A724" s="12"/>
     </row>
     <row r="725">
-      <c r="A725" s="11"/>
+      <c r="A725" s="12"/>
     </row>
     <row r="726">
-      <c r="A726" s="11"/>
+      <c r="A726" s="12"/>
     </row>
     <row r="727">
-      <c r="A727" s="11"/>
+      <c r="A727" s="12"/>
     </row>
     <row r="728">
-      <c r="A728" s="11"/>
+      <c r="A728" s="12"/>
     </row>
     <row r="729">
-      <c r="A729" s="11"/>
+      <c r="A729" s="12"/>
     </row>
     <row r="730">
-      <c r="A730" s="11"/>
+      <c r="A730" s="12"/>
     </row>
     <row r="731">
-      <c r="A731" s="11"/>
+      <c r="A731" s="12"/>
     </row>
     <row r="732">
-      <c r="A732" s="11"/>
+      <c r="A732" s="12"/>
     </row>
     <row r="733">
-      <c r="A733" s="11"/>
+      <c r="A733" s="12"/>
     </row>
     <row r="734">
-      <c r="A734" s="11"/>
+      <c r="A734" s="12"/>
     </row>
     <row r="735">
-      <c r="A735" s="11"/>
+      <c r="A735" s="12"/>
     </row>
     <row r="736">
-      <c r="A736" s="11"/>
+      <c r="A736" s="12"/>
     </row>
     <row r="737">
-      <c r="A737" s="11"/>
+      <c r="A737" s="12"/>
     </row>
     <row r="738">
-      <c r="A738" s="11"/>
+      <c r="A738" s="12"/>
     </row>
     <row r="739">
-      <c r="A739" s="11"/>
+      <c r="A739" s="12"/>
     </row>
     <row r="740">
-      <c r="A740" s="11"/>
+      <c r="A740" s="12"/>
     </row>
     <row r="741">
-      <c r="A741" s="11"/>
+      <c r="A741" s="12"/>
     </row>
     <row r="742">
-      <c r="A742" s="11"/>
+      <c r="A742" s="12"/>
     </row>
     <row r="743">
-      <c r="A743" s="11"/>
+      <c r="A743" s="12"/>
     </row>
     <row r="744">
-      <c r="A744" s="11"/>
+      <c r="A744" s="12"/>
     </row>
     <row r="745">
-      <c r="A745" s="11"/>
+      <c r="A745" s="12"/>
     </row>
     <row r="746">
-      <c r="A746" s="11"/>
+      <c r="A746" s="12"/>
     </row>
     <row r="747">
-      <c r="A747" s="11"/>
+      <c r="A747" s="12"/>
     </row>
     <row r="748">
-      <c r="A748" s="11"/>
+      <c r="A748" s="12"/>
     </row>
     <row r="749">
-      <c r="A749" s="11"/>
+      <c r="A749" s="12"/>
     </row>
     <row r="750">
-      <c r="A750" s="11"/>
+      <c r="A750" s="12"/>
     </row>
     <row r="751">
-      <c r="A751" s="11"/>
+      <c r="A751" s="12"/>
     </row>
     <row r="752">
-      <c r="A752" s="11"/>
+      <c r="A752" s="12"/>
     </row>
     <row r="753">
-      <c r="A753" s="11"/>
+      <c r="A753" s="12"/>
     </row>
     <row r="754">
-      <c r="A754" s="11"/>
+      <c r="A754" s="12"/>
     </row>
     <row r="755">
-      <c r="A755" s="11"/>
+      <c r="A755" s="12"/>
     </row>
     <row r="756">
-      <c r="A756" s="11"/>
+      <c r="A756" s="12"/>
     </row>
     <row r="757">
-      <c r="A757" s="11"/>
+      <c r="A757" s="12"/>
     </row>
     <row r="758">
-      <c r="A758" s="11"/>
+      <c r="A758" s="12"/>
     </row>
     <row r="759">
-      <c r="A759" s="11"/>
+      <c r="A759" s="12"/>
     </row>
     <row r="760">
-      <c r="A760" s="11"/>
+      <c r="A760" s="12"/>
     </row>
     <row r="761">
-      <c r="A761" s="11"/>
+      <c r="A761" s="12"/>
     </row>
     <row r="762">
-      <c r="A762" s="11"/>
+      <c r="A762" s="12"/>
     </row>
     <row r="763">
-      <c r="A763" s="11"/>
+      <c r="A763" s="12"/>
     </row>
     <row r="764">
-      <c r="A764" s="11"/>
+      <c r="A764" s="12"/>
     </row>
     <row r="765">
-      <c r="A765" s="11"/>
+      <c r="A765" s="12"/>
     </row>
     <row r="766">
-      <c r="A766" s="11"/>
+      <c r="A766" s="12"/>
     </row>
     <row r="767">
-      <c r="A767" s="11"/>
+      <c r="A767" s="12"/>
     </row>
     <row r="768">
-      <c r="A768" s="11"/>
+      <c r="A768" s="12"/>
     </row>
     <row r="769">
-      <c r="A769" s="11"/>
+      <c r="A769" s="12"/>
     </row>
     <row r="770">
-      <c r="A770" s="11"/>
+      <c r="A770" s="12"/>
     </row>
     <row r="771">
-      <c r="A771" s="11"/>
+      <c r="A771" s="12"/>
     </row>
     <row r="772">
-      <c r="A772" s="11"/>
+      <c r="A772" s="12"/>
     </row>
     <row r="773">
-      <c r="A773" s="11"/>
+      <c r="A773" s="12"/>
     </row>
     <row r="774">
-      <c r="A774" s="11"/>
+      <c r="A774" s="12"/>
     </row>
     <row r="775">
-      <c r="A775" s="11"/>
+      <c r="A775" s="12"/>
     </row>
     <row r="776">
-      <c r="A776" s="11"/>
+      <c r="A776" s="12"/>
     </row>
     <row r="777">
-      <c r="A777" s="11"/>
+      <c r="A777" s="12"/>
     </row>
     <row r="778">
-      <c r="A778" s="11"/>
+      <c r="A778" s="12"/>
     </row>
     <row r="779">
-      <c r="A779" s="11"/>
+      <c r="A779" s="12"/>
     </row>
     <row r="780">
-      <c r="A780" s="11"/>
+      <c r="A780" s="12"/>
     </row>
     <row r="781">
-      <c r="A781" s="11"/>
+      <c r="A781" s="12"/>
     </row>
     <row r="782">
-      <c r="A782" s="11"/>
+      <c r="A782" s="12"/>
     </row>
     <row r="783">
-      <c r="A783" s="11"/>
+      <c r="A783" s="12"/>
     </row>
     <row r="784">
-      <c r="A784" s="11"/>
+      <c r="A784" s="12"/>
     </row>
     <row r="785">
-      <c r="A785" s="11"/>
+      <c r="A785" s="12"/>
     </row>
     <row r="786">
-      <c r="A786" s="11"/>
+      <c r="A786" s="12"/>
     </row>
     <row r="787">
-      <c r="A787" s="11"/>
+      <c r="A787" s="12"/>
     </row>
     <row r="788">
-      <c r="A788" s="11"/>
+      <c r="A788" s="12"/>
     </row>
     <row r="789">
-      <c r="A789" s="11"/>
+      <c r="A789" s="12"/>
     </row>
     <row r="790">
-      <c r="A790" s="11"/>
+      <c r="A790" s="12"/>
     </row>
     <row r="791">
-      <c r="A791" s="11"/>
+      <c r="A791" s="12"/>
     </row>
     <row r="792">
-      <c r="A792" s="11"/>
+      <c r="A792" s="12"/>
     </row>
     <row r="793">
-      <c r="A793" s="11"/>
+      <c r="A793" s="12"/>
     </row>
     <row r="794">
-      <c r="A794" s="11"/>
+      <c r="A794" s="12"/>
     </row>
     <row r="795">
-      <c r="A795" s="11"/>
+      <c r="A795" s="12"/>
     </row>
     <row r="796">
-      <c r="A796" s="11"/>
+      <c r="A796" s="12"/>
     </row>
     <row r="797">
-      <c r="A797" s="11"/>
+      <c r="A797" s="12"/>
     </row>
     <row r="798">
-      <c r="A798" s="11"/>
+      <c r="A798" s="12"/>
     </row>
     <row r="799">
-      <c r="A799" s="11"/>
+      <c r="A799" s="12"/>
     </row>
     <row r="800">
-      <c r="A800" s="11"/>
+      <c r="A800" s="12"/>
     </row>
     <row r="801">
-      <c r="A801" s="11"/>
+      <c r="A801" s="12"/>
     </row>
     <row r="802">
-      <c r="A802" s="11"/>
+      <c r="A802" s="12"/>
     </row>
     <row r="803">
-      <c r="A803" s="11"/>
+      <c r="A803" s="12"/>
     </row>
     <row r="804">
-      <c r="A804" s="11"/>
+      <c r="A804" s="12"/>
     </row>
     <row r="805">
-      <c r="A805" s="11"/>
+      <c r="A805" s="12"/>
     </row>
     <row r="806">
-      <c r="A806" s="11"/>
+      <c r="A806" s="12"/>
     </row>
     <row r="807">
-      <c r="A807" s="11"/>
+      <c r="A807" s="12"/>
     </row>
     <row r="808">
-      <c r="A808" s="11"/>
+      <c r="A808" s="12"/>
     </row>
     <row r="809">
-      <c r="A809" s="11"/>
+      <c r="A809" s="12"/>
     </row>
     <row r="810">
-      <c r="A810" s="11"/>
+      <c r="A810" s="12"/>
     </row>
     <row r="811">
-      <c r="A811" s="11"/>
+      <c r="A811" s="12"/>
     </row>
     <row r="812">
-      <c r="A812" s="11"/>
+      <c r="A812" s="12"/>
     </row>
     <row r="813">
-      <c r="A813" s="11"/>
+      <c r="A813" s="12"/>
     </row>
     <row r="814">
-      <c r="A814" s="11"/>
+      <c r="A814" s="12"/>
     </row>
     <row r="815">
-      <c r="A815" s="11"/>
+      <c r="A815" s="12"/>
     </row>
     <row r="816">
-      <c r="A816" s="11"/>
+      <c r="A816" s="12"/>
     </row>
     <row r="817">
-      <c r="A817" s="11"/>
+      <c r="A817" s="12"/>
     </row>
     <row r="818">
-      <c r="A818" s="11"/>
+      <c r="A818" s="12"/>
     </row>
     <row r="819">
-      <c r="A819" s="11"/>
+      <c r="A819" s="12"/>
     </row>
     <row r="820">
-      <c r="A820" s="11"/>
+      <c r="A820" s="12"/>
     </row>
     <row r="821">
-      <c r="A821" s="11"/>
+      <c r="A821" s="12"/>
     </row>
     <row r="822">
-      <c r="A822" s="11"/>
+      <c r="A822" s="12"/>
     </row>
     <row r="823">
-      <c r="A823" s="11"/>
+      <c r="A823" s="12"/>
     </row>
     <row r="824">
-      <c r="A824" s="11"/>
+      <c r="A824" s="12"/>
     </row>
     <row r="825">
-      <c r="A825" s="11"/>
+      <c r="A825" s="12"/>
     </row>
     <row r="826">
-      <c r="A826" s="11"/>
+      <c r="A826" s="12"/>
     </row>
     <row r="827">
-      <c r="A827" s="11"/>
+      <c r="A827" s="12"/>
     </row>
     <row r="828">
-      <c r="A828" s="11"/>
+      <c r="A828" s="12"/>
     </row>
     <row r="829">
-      <c r="A829" s="11"/>
+      <c r="A829" s="12"/>
     </row>
     <row r="830">
-      <c r="A830" s="11"/>
+      <c r="A830" s="12"/>
     </row>
     <row r="831">
-      <c r="A831" s="11"/>
+      <c r="A831" s="12"/>
     </row>
     <row r="832">
-      <c r="A832" s="11"/>
+      <c r="A832" s="12"/>
     </row>
     <row r="833">
-      <c r="A833" s="11"/>
+      <c r="A833" s="12"/>
     </row>
     <row r="834">
-      <c r="A834" s="11"/>
+      <c r="A834" s="12"/>
     </row>
     <row r="835">
-      <c r="A835" s="11"/>
+      <c r="A835" s="12"/>
     </row>
     <row r="836">
-      <c r="A836" s="11"/>
+      <c r="A836" s="12"/>
     </row>
     <row r="837">
-      <c r="A837" s="11"/>
+      <c r="A837" s="12"/>
     </row>
     <row r="838">
-      <c r="A838" s="11"/>
+      <c r="A838" s="12"/>
     </row>
     <row r="839">
-      <c r="A839" s="11"/>
+      <c r="A839" s="12"/>
     </row>
     <row r="840">
-      <c r="A840" s="11"/>
+      <c r="A840" s="12"/>
     </row>
     <row r="841">
-      <c r="A841" s="11"/>
+      <c r="A841" s="12"/>
     </row>
     <row r="842">
-      <c r="A842" s="11"/>
+      <c r="A842" s="12"/>
     </row>
     <row r="843">
-      <c r="A843" s="11"/>
+      <c r="A843" s="12"/>
     </row>
     <row r="844">
-      <c r="A844" s="11"/>
+      <c r="A844" s="12"/>
     </row>
     <row r="845">
-      <c r="A845" s="11"/>
+      <c r="A845" s="12"/>
     </row>
     <row r="846">
-      <c r="A846" s="11"/>
+      <c r="A846" s="12"/>
     </row>
     <row r="847">
-      <c r="A847" s="11"/>
+      <c r="A847" s="12"/>
     </row>
     <row r="848">
-      <c r="A848" s="11"/>
+      <c r="A848" s="12"/>
     </row>
     <row r="849">
-      <c r="A849" s="11"/>
+      <c r="A849" s="12"/>
     </row>
     <row r="850">
-      <c r="A850" s="11"/>
+      <c r="A850" s="12"/>
     </row>
     <row r="851">
-      <c r="A851" s="11"/>
+      <c r="A851" s="12"/>
     </row>
     <row r="852">
-      <c r="A852" s="11"/>
+      <c r="A852" s="12"/>
     </row>
     <row r="853">
-      <c r="A853" s="11"/>
+      <c r="A853" s="12"/>
     </row>
     <row r="854">
-      <c r="A854" s="11"/>
+      <c r="A854" s="12"/>
     </row>
     <row r="855">
-      <c r="A855" s="11"/>
+      <c r="A855" s="12"/>
     </row>
     <row r="856">
-      <c r="A856" s="11"/>
+      <c r="A856" s="12"/>
     </row>
     <row r="857">
-      <c r="A857" s="11"/>
+      <c r="A857" s="12"/>
     </row>
     <row r="858">
-      <c r="A858" s="11"/>
+      <c r="A858" s="12"/>
     </row>
     <row r="859">
-      <c r="A859" s="11"/>
+      <c r="A859" s="12"/>
     </row>
     <row r="860">
-      <c r="A860" s="11"/>
+      <c r="A860" s="12"/>
     </row>
     <row r="861">
-      <c r="A861" s="11"/>
+      <c r="A861" s="12"/>
     </row>
     <row r="862">
-      <c r="A862" s="11"/>
+      <c r="A862" s="12"/>
     </row>
     <row r="863">
-      <c r="A863" s="11"/>
+      <c r="A863" s="12"/>
     </row>
     <row r="864">
-      <c r="A864" s="11"/>
+      <c r="A864" s="12"/>
     </row>
     <row r="865">
-      <c r="A865" s="11"/>
+      <c r="A865" s="12"/>
     </row>
     <row r="866">
-      <c r="A866" s="11"/>
+      <c r="A866" s="12"/>
     </row>
     <row r="867">
-      <c r="A867" s="11"/>
+      <c r="A867" s="12"/>
     </row>
     <row r="868">
-      <c r="A868" s="11"/>
+      <c r="A868" s="12"/>
     </row>
     <row r="869">
-      <c r="A869" s="11"/>
+      <c r="A869" s="12"/>
     </row>
     <row r="870">
-      <c r="A870" s="11"/>
+      <c r="A870" s="12"/>
     </row>
     <row r="871">
-      <c r="A871" s="11"/>
+      <c r="A871" s="12"/>
     </row>
     <row r="872">
-      <c r="A872" s="11"/>
+      <c r="A872" s="12"/>
     </row>
     <row r="873">
-      <c r="A873" s="11"/>
+      <c r="A873" s="12"/>
     </row>
     <row r="874">
-      <c r="A874" s="11"/>
+      <c r="A874" s="12"/>
     </row>
     <row r="875">
-      <c r="A875" s="11"/>
+      <c r="A875" s="12"/>
     </row>
     <row r="876">
-      <c r="A876" s="11"/>
+      <c r="A876" s="12"/>
     </row>
     <row r="877">
-      <c r="A877" s="11"/>
+      <c r="A877" s="12"/>
     </row>
     <row r="878">
-      <c r="A878" s="11"/>
+      <c r="A878" s="12"/>
     </row>
     <row r="879">
-      <c r="A879" s="11"/>
+      <c r="A879" s="12"/>
     </row>
     <row r="880">
-      <c r="A880" s="11"/>
+      <c r="A880" s="12"/>
     </row>
     <row r="881">
-      <c r="A881" s="11"/>
+      <c r="A881" s="12"/>
     </row>
     <row r="882">
-      <c r="A882" s="11"/>
+      <c r="A882" s="12"/>
     </row>
     <row r="883">
-      <c r="A883" s="11"/>
+      <c r="A883" s="12"/>
     </row>
     <row r="884">
-      <c r="A884" s="11"/>
+      <c r="A884" s="12"/>
     </row>
     <row r="885">
-      <c r="A885" s="11"/>
+      <c r="A885" s="12"/>
     </row>
     <row r="886">
-      <c r="A886" s="11"/>
+      <c r="A886" s="12"/>
     </row>
     <row r="887">
-      <c r="A887" s="11"/>
+      <c r="A887" s="12"/>
     </row>
     <row r="888">
-      <c r="A888" s="11"/>
+      <c r="A888" s="12"/>
     </row>
     <row r="889">
-      <c r="A889" s="11"/>
+      <c r="A889" s="12"/>
     </row>
     <row r="890">
-      <c r="A890" s="11"/>
+      <c r="A890" s="12"/>
     </row>
     <row r="891">
-      <c r="A891" s="11"/>
+      <c r="A891" s="12"/>
     </row>
     <row r="892">
-      <c r="A892" s="11"/>
+      <c r="A892" s="12"/>
     </row>
     <row r="893">
-      <c r="A893" s="11"/>
+      <c r="A893" s="12"/>
     </row>
     <row r="894">
-      <c r="A894" s="11"/>
+      <c r="A894" s="12"/>
     </row>
     <row r="895">
-      <c r="A895" s="11"/>
+      <c r="A895" s="12"/>
     </row>
     <row r="896">
-      <c r="A896" s="11"/>
+      <c r="A896" s="12"/>
     </row>
     <row r="897">
-      <c r="A897" s="11"/>
+      <c r="A897" s="12"/>
     </row>
     <row r="898">
-      <c r="A898" s="11"/>
+      <c r="A898" s="12"/>
     </row>
     <row r="899">
-      <c r="A899" s="11"/>
+      <c r="A899" s="12"/>
     </row>
     <row r="900">
-      <c r="A900" s="11"/>
+      <c r="A900" s="12"/>
     </row>
     <row r="901">
-      <c r="A901" s="11"/>
+      <c r="A901" s="12"/>
     </row>
     <row r="902">
-      <c r="A902" s="11"/>
+      <c r="A902" s="12"/>
     </row>
     <row r="903">
-      <c r="A903" s="11"/>
+      <c r="A903" s="12"/>
     </row>
     <row r="904">
-      <c r="A904" s="11"/>
+      <c r="A904" s="12"/>
     </row>
     <row r="905">
-      <c r="A905" s="11"/>
+      <c r="A905" s="12"/>
     </row>
     <row r="906">
-      <c r="A906" s="11"/>
+      <c r="A906" s="12"/>
     </row>
     <row r="907">
-      <c r="A907" s="11"/>
+      <c r="A907" s="12"/>
     </row>
     <row r="908">
-      <c r="A908" s="11"/>
+      <c r="A908" s="12"/>
     </row>
     <row r="909">
-      <c r="A909" s="11"/>
+      <c r="A909" s="12"/>
     </row>
     <row r="910">
-      <c r="A910" s="11"/>
+      <c r="A910" s="12"/>
     </row>
     <row r="911">
-      <c r="A911" s="11"/>
+      <c r="A911" s="12"/>
     </row>
     <row r="912">
-      <c r="A912" s="11"/>
+      <c r="A912" s="12"/>
     </row>
     <row r="913">
-      <c r="A913" s="11"/>
+      <c r="A913" s="12"/>
     </row>
     <row r="914">
-      <c r="A914" s="11"/>
+      <c r="A914" s="12"/>
     </row>
     <row r="915">
-      <c r="A915" s="11"/>
+      <c r="A915" s="12"/>
     </row>
     <row r="916">
-      <c r="A916" s="11"/>
+      <c r="A916" s="12"/>
     </row>
     <row r="917">
-      <c r="A917" s="11"/>
+      <c r="A917" s="12"/>
     </row>
     <row r="918">
-      <c r="A918" s="11"/>
+      <c r="A918" s="12"/>
     </row>
     <row r="919">
-      <c r="A919" s="11"/>
+      <c r="A919" s="12"/>
     </row>
     <row r="920">
-      <c r="A920" s="11"/>
+      <c r="A920" s="12"/>
     </row>
     <row r="921">
-      <c r="A921" s="11"/>
+      <c r="A921" s="12"/>
     </row>
     <row r="922">
-      <c r="A922" s="11"/>
+      <c r="A922" s="12"/>
     </row>
     <row r="923">
-      <c r="A923" s="11"/>
+      <c r="A923" s="12"/>
     </row>
     <row r="924">
-      <c r="A924" s="11"/>
+      <c r="A924" s="12"/>
     </row>
     <row r="925">
-      <c r="A925" s="11"/>
+      <c r="A925" s="12"/>
     </row>
     <row r="926">
-      <c r="A926" s="11"/>
+      <c r="A926" s="12"/>
     </row>
     <row r="927">
-      <c r="A927" s="11"/>
+      <c r="A927" s="12"/>
     </row>
     <row r="928">
-      <c r="A928" s="11"/>
+      <c r="A928" s="12"/>
     </row>
     <row r="929">
-      <c r="A929" s="11"/>
+      <c r="A929" s="12"/>
     </row>
     <row r="930">
-      <c r="A930" s="11"/>
+      <c r="A930" s="12"/>
     </row>
     <row r="931">
-      <c r="A931" s="11"/>
+      <c r="A931" s="12"/>
     </row>
     <row r="932">
-      <c r="A932" s="11"/>
+      <c r="A932" s="12"/>
     </row>
     <row r="933">
-      <c r="A933" s="11"/>
+      <c r="A933" s="12"/>
     </row>
     <row r="934">
-      <c r="A934" s="11"/>
+      <c r="A934" s="12"/>
     </row>
     <row r="935">
-      <c r="A935" s="11"/>
+      <c r="A935" s="12"/>
     </row>
     <row r="936">
-      <c r="A936" s="11"/>
+      <c r="A936" s="12"/>
     </row>
     <row r="937">
-      <c r="A937" s="11"/>
+      <c r="A937" s="12"/>
     </row>
     <row r="938">
-      <c r="A938" s="11"/>
+      <c r="A938" s="12"/>
     </row>
     <row r="939">
-      <c r="A939" s="11"/>
+      <c r="A939" s="12"/>
     </row>
     <row r="940">
-      <c r="A940" s="11"/>
+      <c r="A940" s="12"/>
     </row>
     <row r="941">
-      <c r="A941" s="11"/>
+      <c r="A941" s="12"/>
     </row>
     <row r="942">
-      <c r="A942" s="11"/>
+      <c r="A942" s="12"/>
     </row>
     <row r="943">
-      <c r="A943" s="11"/>
+      <c r="A943" s="12"/>
     </row>
     <row r="944">
-      <c r="A944" s="11"/>
+      <c r="A944" s="12"/>
     </row>
     <row r="945">
-      <c r="A945" s="11"/>
+      <c r="A945" s="12"/>
     </row>
     <row r="946">
-      <c r="A946" s="11"/>
+      <c r="A946" s="12"/>
     </row>
     <row r="947">
-      <c r="A947" s="11"/>
+      <c r="A947" s="12"/>
     </row>
     <row r="948">
-      <c r="A948" s="11"/>
+      <c r="A948" s="12"/>
     </row>
     <row r="949">
-      <c r="A949" s="11"/>
+      <c r="A949" s="12"/>
     </row>
     <row r="950">
-      <c r="A950" s="11"/>
+      <c r="A950" s="12"/>
     </row>
     <row r="951">
-      <c r="A951" s="11"/>
+      <c r="A951" s="12"/>
     </row>
     <row r="952">
-      <c r="A952" s="11"/>
+      <c r="A952" s="12"/>
     </row>
     <row r="953">
-      <c r="A953" s="11"/>
+      <c r="A953" s="12"/>
     </row>
     <row r="954">
-      <c r="A954" s="11"/>
+      <c r="A954" s="12"/>
     </row>
     <row r="955">
-      <c r="A955" s="11"/>
+      <c r="A955" s="12"/>
     </row>
     <row r="956">
-      <c r="A956" s="11"/>
+      <c r="A956" s="12"/>
     </row>
     <row r="957">
-      <c r="A957" s="11"/>
+      <c r="A957" s="12"/>
     </row>
     <row r="958">
-      <c r="A958" s="11"/>
+      <c r="A958" s="12"/>
     </row>
     <row r="959">
-      <c r="A959" s="11"/>
+      <c r="A959" s="12"/>
     </row>
     <row r="960">
-      <c r="A960" s="11"/>
+      <c r="A960" s="12"/>
     </row>
     <row r="961">
-      <c r="A961" s="11"/>
+      <c r="A961" s="12"/>
     </row>
     <row r="962">
-      <c r="A962" s="11"/>
+      <c r="A962" s="12"/>
     </row>
     <row r="963">
-      <c r="A963" s="11"/>
+      <c r="A963" s="12"/>
     </row>
     <row r="964">
-      <c r="A964" s="11"/>
+      <c r="A964" s="12"/>
     </row>
     <row r="965">
-      <c r="A965" s="11"/>
+      <c r="A965" s="12"/>
     </row>
     <row r="966">
-      <c r="A966" s="11"/>
+      <c r="A966" s="12"/>
     </row>
     <row r="967">
-      <c r="A967" s="11"/>
+      <c r="A967" s="12"/>
     </row>
     <row r="968">
-      <c r="A968" s="11"/>
+      <c r="A968" s="12"/>
     </row>
     <row r="969">
-      <c r="A969" s="11"/>
+      <c r="A969" s="12"/>
     </row>
     <row r="970">
-      <c r="A970" s="11"/>
+      <c r="A970" s="12"/>
     </row>
     <row r="971">
-      <c r="A971" s="11"/>
+      <c r="A971" s="12"/>
     </row>
     <row r="972">
-      <c r="A972" s="11"/>
+      <c r="A972" s="12"/>
     </row>
     <row r="973">
-      <c r="A973" s="11"/>
+      <c r="A973" s="12"/>
     </row>
     <row r="974">
-      <c r="A974" s="11"/>
+      <c r="A974" s="12"/>
     </row>
     <row r="975">
-      <c r="A975" s="11"/>
+      <c r="A975" s="12"/>
     </row>
     <row r="976">
-      <c r="A976" s="11"/>
+      <c r="A976" s="12"/>
     </row>
     <row r="977">
-      <c r="A977" s="11"/>
+      <c r="A977" s="12"/>
     </row>
     <row r="978">
-      <c r="A978" s="11"/>
+      <c r="A978" s="12"/>
     </row>
     <row r="979">
-      <c r="A979" s="11"/>
+      <c r="A979" s="12"/>
     </row>
     <row r="980">
-      <c r="A980" s="11"/>
+      <c r="A980" s="12"/>
     </row>
     <row r="981">
-      <c r="A981" s="11"/>
+      <c r="A981" s="12"/>
     </row>
     <row r="982">
-      <c r="A982" s="11"/>
+      <c r="A982" s="12"/>
     </row>
     <row r="983">
-      <c r="A983" s="11"/>
+      <c r="A983" s="12"/>
     </row>
     <row r="984">
-      <c r="A984" s="11"/>
+      <c r="A984" s="12"/>
     </row>
     <row r="985">
-      <c r="A985" s="11"/>
+      <c r="A985" s="12"/>
     </row>
     <row r="986">
-      <c r="A986" s="11"/>
+      <c r="A986" s="12"/>
     </row>
     <row r="987">
-      <c r="A987" s="11"/>
+      <c r="A987" s="12"/>
     </row>
     <row r="988">
-      <c r="A988" s="11"/>
+      <c r="A988" s="12"/>
     </row>
     <row r="989">
-      <c r="A989" s="11"/>
+      <c r="A989" s="12"/>
     </row>
     <row r="990">
-      <c r="A990" s="11"/>
+      <c r="A990" s="12"/>
     </row>
     <row r="991">
-      <c r="A991" s="11"/>
+      <c r="A991" s="12"/>
     </row>
     <row r="992">
-      <c r="A992" s="11"/>
+      <c r="A992" s="12"/>
     </row>
     <row r="993">
-      <c r="A993" s="11"/>
+      <c r="A993" s="12"/>
     </row>
     <row r="994">
-      <c r="A994" s="11"/>
+      <c r="A994" s="12"/>
     </row>
     <row r="995">
-      <c r="A995" s="11"/>
+      <c r="A995" s="12"/>
     </row>
     <row r="996">
-      <c r="A996" s="11"/>
+      <c r="A996" s="12"/>
     </row>
     <row r="997">
-      <c r="A997" s="11"/>
+      <c r="A997" s="12"/>
     </row>
     <row r="998">
-      <c r="A998" s="11"/>
+      <c r="A998" s="12"/>
     </row>
     <row r="999">
-      <c r="A999" s="11"/>
+      <c r="A999" s="12"/>
     </row>
     <row r="1000">
-      <c r="A1000" s="11"/>
+      <c r="A1000" s="12"/>
     </row>
     <row r="1001">
-      <c r="A1001" s="11"/>
+      <c r="A1001" s="12"/>
     </row>
     <row r="1002">
-      <c r="A1002" s="11"/>
+      <c r="A1002" s="12"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Updated BestFit and Localization. Inventory logic now working.
</commit_message>
<xml_diff>
--- a/Unity/Assets/Resources/Localization/IT Alert UI Translation.xlsx
+++ b/Unity/Assets/Resources/Localization/IT Alert UI Translation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="243">
   <si>
     <t>Key</t>
   </si>
@@ -719,6 +719,30 @@
   </si>
   <si>
     <t>Analysis Output - Antiviruses appear here</t>
+  </si>
+  <si>
+    <t>USE_BUTTON</t>
+  </si>
+  <si>
+    <t>MOVE_BUTTON</t>
+  </si>
+  <si>
+    <t>TAKE_BUTTON</t>
+  </si>
+  <si>
+    <t>Use</t>
+  </si>
+  <si>
+    <t>Move</t>
+  </si>
+  <si>
+    <t>Take</t>
+  </si>
+  <si>
+    <t>PLACE_BUTTON</t>
+  </si>
+  <si>
+    <t>Place</t>
   </si>
 </sst>
 </file>
@@ -1123,7 +1147,7 @@
   <dimension ref="A1:U1002"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2268,16 +2292,48 @@
       </c>
     </row>
     <row r="91" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A91" s="12"/>
+      <c r="A91" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="C91" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="92" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A92" s="12"/>
+      <c r="A92" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="C92" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="93" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A93" s="12"/>
+      <c r="A93" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="C93" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="94" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A94" s="12"/>
+      <c r="A94" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="C94" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="95" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="12"/>

</xml_diff>

<commit_message>
Now possible to place and use an inventory item within one action
</commit_message>
<xml_diff>
--- a/Unity/Assets/Resources/Localization/IT Alert UI Translation.xlsx
+++ b/Unity/Assets/Resources/Localization/IT Alert UI Translation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="245">
   <si>
     <t>Key</t>
   </si>
@@ -743,6 +743,12 @@
   </si>
   <si>
     <t>Place</t>
+  </si>
+  <si>
+    <t>PLACE_AND_USE_BUTTON</t>
+  </si>
+  <si>
+    <t>Place And Use</t>
   </si>
 </sst>
 </file>
@@ -1147,7 +1153,7 @@
   <dimension ref="A1:U1002"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2336,7 +2342,15 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A95" s="12"/>
+      <c r="A95" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="C95" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="96" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="12"/>

</xml_diff>

<commit_message>
Feedback bugs fixed, Dutch translations for new text
</commit_message>
<xml_diff>
--- a/Unity/Assets/Resources/Localization/IT Alert UI Translation.xlsx
+++ b/Unity/Assets/Resources/Localization/IT Alert UI Translation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="260">
   <si>
     <t>Key</t>
   </si>
@@ -691,9 +691,6 @@
     <t>Analyser Tool - Activate to create an antivirus</t>
   </si>
   <si>
-    <t>XXXX</t>
-  </si>
-  <si>
     <t>Inventory - Currently held item</t>
   </si>
   <si>
@@ -749,6 +746,54 @@
   </si>
   <si>
     <t>Place And Use</t>
+  </si>
+  <si>
+    <t>Capture tool - Activeren om een virus sample te verkrijgen</t>
+  </si>
+  <si>
+    <t>Scanner tool - Activeren om verborgen virussen te vinden</t>
+  </si>
+  <si>
+    <t>Analyser tool - Activeren om een antivirus aan te maken</t>
+  </si>
+  <si>
+    <t>Inventaris - Item dat je nu vast hebt</t>
+  </si>
+  <si>
+    <t>Analysis Target - Plaats hier het gevangen virus sample</t>
+  </si>
+  <si>
+    <t>Analysis Output - Het antivirus verschijnt hier</t>
+  </si>
+  <si>
+    <t>Antivirus tool - Wordt gebruikt om virus te vernietigen</t>
+  </si>
+  <si>
+    <t>Transfer tool - Wordt gebruikt om items te verplaatsen tussen systemen</t>
+  </si>
+  <si>
+    <t>Transfer Container - Hier liggen de items die verplaatst worden</t>
+  </si>
+  <si>
+    <t>CPU - Beweeg snelheid op dit systeem</t>
+  </si>
+  <si>
+    <t>Memeory - Overgebleve</t>
+  </si>
+  <si>
+    <t>Gebruiken</t>
+  </si>
+  <si>
+    <t>Verplaatsen</t>
+  </si>
+  <si>
+    <t>Pakken</t>
+  </si>
+  <si>
+    <t>Plaatsen</t>
+  </si>
+  <si>
+    <t>Plaatsen en Gebruiken</t>
   </si>
 </sst>
 </file>
@@ -1152,7 +1197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
       <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
@@ -1160,7 +1205,7 @@
   <cols>
     <col min="1" max="1" width="48.140625" customWidth="1"/>
     <col min="2" max="2" width="51.85546875" customWidth="1"/>
-    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="3" max="3" width="62.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2181,10 +2226,10 @@
         <v>212</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>225</v>
+        <v>244</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -2195,7 +2240,7 @@
         <v>223</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -2206,7 +2251,7 @@
         <v>224</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>225</v>
+        <v>246</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -2214,10 +2259,10 @@
         <v>215</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>225</v>
+        <v>247</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -2225,10 +2270,10 @@
         <v>216</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C84" t="s">
-        <v>225</v>
+        <v>248</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -2236,10 +2281,10 @@
         <v>217</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C85" t="s">
-        <v>225</v>
+        <v>249</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -2247,10 +2292,10 @@
         <v>218</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C86" t="s">
-        <v>225</v>
+        <v>250</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -2258,10 +2303,10 @@
         <v>219</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C87" t="s">
-        <v>225</v>
+        <v>251</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -2269,10 +2314,10 @@
         <v>220</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C88" t="s">
-        <v>225</v>
+        <v>252</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -2280,10 +2325,10 @@
         <v>221</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C89" t="s">
-        <v>225</v>
+        <v>253</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -2291,65 +2336,65 @@
         <v>222</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C90" t="s">
-        <v>225</v>
+        <v>254</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C91" t="s">
-        <v>225</v>
+        <v>255</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C92" t="s">
-        <v>225</v>
+        <v>256</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C93" t="s">
-        <v>225</v>
+        <v>257</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="B94" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="B94" s="6" t="s">
-        <v>242</v>
-      </c>
       <c r="C94" t="s">
-        <v>225</v>
+        <v>258</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="B95" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="B95" s="6" t="s">
-        <v>244</v>
-      </c>
       <c r="C95" t="s">
-        <v>225</v>
+        <v>259</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Various minor fixes relating to Dutch text and buggy UI behaviour
</commit_message>
<xml_diff>
--- a/Unity/Assets/Resources/Localization/IT Alert UI Translation.xlsx
+++ b/Unity/Assets/Resources/Localization/IT Alert UI Translation.xlsx
@@ -19,9 +19,6 @@
     <t>Key</t>
   </si>
   <si>
-    <t>en-gb</t>
-  </si>
-  <si>
     <t>nl</t>
   </si>
   <si>
@@ -794,6 +791,9 @@
   </si>
   <si>
     <t>Plaatsen en Gebruiken</t>
+  </si>
+  <si>
+    <t>en</t>
   </si>
 </sst>
 </file>
@@ -1197,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1213,10 +1213,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -1239,13 +1239,13 @@
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -1253,13 +1253,13 @@
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -1267,13 +1267,13 @@
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -1281,13 +1281,13 @@
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -1295,13 +1295,13 @@
     </row>
     <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -1309,13 +1309,13 @@
     </row>
     <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -1323,13 +1323,13 @@
     </row>
     <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -1337,13 +1337,13 @@
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1351,13 +1351,13 @@
     </row>
     <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1365,13 +1365,13 @@
     </row>
     <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -1379,13 +1379,13 @@
     </row>
     <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1393,13 +1393,13 @@
     </row>
     <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -1407,13 +1407,13 @@
     </row>
     <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -1421,13 +1421,13 @@
     </row>
     <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -1435,13 +1435,13 @@
     </row>
     <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -1449,13 +1449,13 @@
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -1463,13 +1463,13 @@
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -1477,13 +1477,13 @@
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -1491,13 +1491,13 @@
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>50</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -1505,13 +1505,13 @@
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -1519,13 +1519,13 @@
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -1533,13 +1533,13 @@
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -1547,13 +1547,13 @@
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -1561,13 +1561,13 @@
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -1575,13 +1575,13 @@
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -1589,13 +1589,13 @@
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -1603,13 +1603,13 @@
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -1617,13 +1617,13 @@
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -1631,13 +1631,13 @@
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -1645,13 +1645,13 @@
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
@@ -1659,13 +1659,13 @@
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -1673,13 +1673,13 @@
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="C33" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -1687,13 +1687,13 @@
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="C34" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -1701,13 +1701,13 @@
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -1715,13 +1715,13 @@
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="C36" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>91</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
@@ -1729,13 +1729,13 @@
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="C37" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -1743,13 +1743,13 @@
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
@@ -1757,13 +1757,13 @@
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>99</v>
-      </c>
       <c r="C39" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -1771,13 +1771,13 @@
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -1785,13 +1785,13 @@
     </row>
     <row r="41" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="C41" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
@@ -1799,13 +1799,13 @@
     </row>
     <row r="42" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="C42" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -1813,13 +1813,13 @@
     </row>
     <row r="43" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="C43" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>111</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
@@ -1827,574 +1827,574 @@
     </row>
     <row r="44" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="C44" s="5" t="s">
         <v>113</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B45" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="C46" s="9" t="s">
         <v>117</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="C47" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="C48" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B49" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B49" s="9" t="s">
-        <v>126</v>
-      </c>
       <c r="C49" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B50" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="C50" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="C51" s="9" t="s">
         <v>131</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B52" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="C52" s="9" t="s">
         <v>134</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B53" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="C53" s="9" t="s">
         <v>137</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B54" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="C54" s="9" t="s">
         <v>140</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B55" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="C55" s="9" t="s">
         <v>143</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B56" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="C56" s="9" t="s">
         <v>146</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B57" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="C57" s="9" t="s">
         <v>149</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B58" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="C58" s="9" t="s">
         <v>152</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B59" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="C59" s="9" t="s">
         <v>155</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B60" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="C60" s="9" t="s">
         <v>158</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="B61" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="C61" s="9" t="s">
         <v>161</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B62" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="B62" s="9" t="s">
+      <c r="C62" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B63" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="B63" s="9" t="s">
-        <v>167</v>
-      </c>
       <c r="C63" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B64" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="C64" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B65" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="C65" s="9" t="s">
         <v>172</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B66" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="C66" s="9" t="s">
         <v>175</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B67" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="B67" s="9" t="s">
+      <c r="C67" s="9" t="s">
         <v>178</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="B68" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B68" s="9" t="s">
+      <c r="C68" s="9" t="s">
         <v>181</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B69" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="C69" s="9" t="s">
         <v>184</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B70" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="C70" s="9" t="s">
         <v>187</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B71" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="B71" s="9" t="s">
+      <c r="C71" s="9" t="s">
         <v>190</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="B72" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="C72" s="9" t="s">
         <v>193</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B73" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="C73" s="9" t="s">
         <v>196</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B74" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="C74" s="9" t="s">
         <v>199</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B75" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="C75" s="9" t="s">
         <v>202</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="B76" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="C76" s="9" t="s">
         <v>205</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B77" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C77" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="B78" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="B78" s="9" t="s">
-        <v>209</v>
-      </c>
       <c r="C78" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B79" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="B79" s="6" t="s">
-        <v>211</v>
-      </c>
       <c r="C79" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C84" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C85" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C86" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C87" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C88" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C89" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C90" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C91" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C92" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C93" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="B94" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="B94" s="6" t="s">
-        <v>241</v>
-      </c>
       <c r="C94" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="B95" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="B95" s="6" t="s">
-        <v>243</v>
-      </c>
       <c r="C95" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>